<commit_message>
Fixed incorrect typo of fieldName
</commit_message>
<xml_diff>
--- a/data/online-dependency-mf_template.xlsx
+++ b/data/online-dependency-mf_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Source Code\Python\jupiter-service-inventory-importer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01CDF7F-DFD0-4E59-B683-D4A9737F8F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B8DCA0-4A48-4A72-AEC2-D37F2FF0AFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7365" yWindow="3570" windowWidth="14115" windowHeight="13725" xr2:uid="{4FBA0D69-02F4-49F3-BDD3-DC0A888CC705}"/>
+    <workbookView xWindow="7920" yWindow="516" windowWidth="30588" windowHeight="13572" xr2:uid="{4FBA0D69-02F4-49F3-BDD3-DC0A888CC705}"/>
   </bookViews>
   <sheets>
     <sheet name="Consumer Master (MF)" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3486" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3486" uniqueCount="700">
   <si>
     <t>(6) Bulk ACH</t>
   </si>
@@ -2149,9 +2149,6 @@
     <t>mainframe_bulk_ach_transaction_code</t>
   </si>
   <si>
-    <t>mainframe_direct_accress_file_id</t>
-  </si>
-  <si>
     <t>batch_eod_type</t>
   </si>
   <si>
@@ -2162,13 +2159,19 @@
   </si>
   <si>
     <t>remark</t>
+  </si>
+  <si>
+    <t>mainframe_direct_access_file_id</t>
+  </si>
+  <si>
+    <t>70_LCI_406F32E219CD39CADB1105BB61E44B81</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3638,35 +3641,35 @@
   </sheetPr>
   <dimension ref="A1:S387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H81" sqref="H81"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D398" sqref="D398"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="35" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.59765625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="128" style="2" customWidth="1"/>
-    <col min="5" max="5" width="63.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="63.296875" style="2" customWidth="1"/>
     <col min="6" max="6" width="28" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="66.125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="70.125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="30.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="44.25" style="2" customWidth="1"/>
-    <col min="14" max="15" width="35.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="62.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="46.25" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.625" style="1"/>
+    <col min="7" max="7" width="27.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.59765625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="66.09765625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="70.09765625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="30.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="44.296875" style="2" customWidth="1"/>
+    <col min="14" max="15" width="35.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="62.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="46.296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="123" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="123" customFormat="1" ht="29.25" customHeight="1">
       <c r="B1" s="124" t="s">
         <v>683</v>
       </c>
@@ -3701,22 +3704,22 @@
         <v>693</v>
       </c>
       <c r="M1" s="124" t="s">
+        <v>698</v>
+      </c>
+      <c r="N1" s="124" t="s">
         <v>694</v>
       </c>
-      <c r="N1" s="124" t="s">
+      <c r="O1" s="124" t="s">
         <v>695</v>
       </c>
-      <c r="O1" s="124" t="s">
+      <c r="P1" s="124" t="s">
         <v>696</v>
       </c>
-      <c r="P1" s="124" t="s">
+      <c r="Q1" s="124" t="s">
         <v>697</v>
       </c>
-      <c r="Q1" s="124" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:19" hidden="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>3</v>
@@ -3753,7 +3756,7 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" hidden="1">
       <c r="A3" s="4"/>
       <c r="B3" s="11" t="s">
         <v>11</v>
@@ -3788,7 +3791,7 @@
       <c r="P3" s="14"/>
       <c r="Q3" s="10"/>
     </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" hidden="1">
       <c r="A4" s="4"/>
       <c r="B4" s="11" t="s">
         <v>11</v>
@@ -3823,7 +3826,7 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="10"/>
     </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" hidden="1">
       <c r="A5" s="4"/>
       <c r="B5" s="11" t="s">
         <v>11</v>
@@ -3858,7 +3861,7 @@
       <c r="P5" s="14"/>
       <c r="Q5" s="10"/>
     </row>
-    <row r="6" spans="1:19" ht="26.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="26.1" hidden="1" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="11" t="s">
         <v>11</v>
@@ -3893,7 +3896,7 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="10"/>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" hidden="1">
       <c r="A7" s="4"/>
       <c r="B7" s="11" t="s">
         <v>11</v>
@@ -3928,7 +3931,7 @@
       <c r="P7" s="14"/>
       <c r="Q7" s="10"/>
     </row>
-    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" hidden="1">
       <c r="A8" s="4"/>
       <c r="B8" s="11" t="s">
         <v>26</v>
@@ -3963,7 +3966,7 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" hidden="1">
       <c r="A9" s="4"/>
       <c r="B9" s="11" t="s">
         <v>32</v>
@@ -4000,7 +4003,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" hidden="1">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="s">
         <v>32</v>
@@ -4037,7 +4040,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="21" t="s">
         <v>41</v>
@@ -4072,7 +4075,7 @@
       <c r="P11" s="24"/>
       <c r="Q11" s="10"/>
     </row>
-    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" hidden="1">
       <c r="A12" s="4"/>
       <c r="B12" s="11" t="s">
         <v>48</v>
@@ -4107,7 +4110,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" hidden="1">
       <c r="A13" s="4"/>
       <c r="B13" s="11" t="s">
         <v>48</v>
@@ -4144,7 +4147,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" hidden="1">
       <c r="A14" s="4"/>
       <c r="B14" s="11" t="s">
         <v>48</v>
@@ -4181,7 +4184,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" hidden="1">
       <c r="A15" s="4"/>
       <c r="B15" s="11" t="s">
         <v>48</v>
@@ -4216,7 +4219,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" hidden="1">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="s">
         <v>48</v>
@@ -4251,7 +4254,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" hidden="1">
       <c r="A17" s="4"/>
       <c r="B17" s="11" t="s">
         <v>48</v>
@@ -4286,7 +4289,7 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" hidden="1">
       <c r="A18" s="4"/>
       <c r="B18" s="11" t="s">
         <v>48</v>
@@ -4321,7 +4324,7 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" hidden="1">
       <c r="A19" s="4"/>
       <c r="B19" s="11" t="s">
         <v>48</v>
@@ -4356,7 +4359,7 @@
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
     </row>
-    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" hidden="1">
       <c r="A20" s="4"/>
       <c r="B20" s="11" t="s">
         <v>48</v>
@@ -4391,7 +4394,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
     </row>
-    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" hidden="1">
       <c r="A21" s="4"/>
       <c r="B21" s="11" t="s">
         <v>48</v>
@@ -4426,7 +4429,7 @@
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
     </row>
-    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" hidden="1">
       <c r="A22" s="4"/>
       <c r="B22" s="11" t="s">
         <v>48</v>
@@ -4459,7 +4462,7 @@
       <c r="P22" s="14"/>
       <c r="Q22" s="10"/>
     </row>
-    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" hidden="1">
       <c r="A23" s="4"/>
       <c r="B23" s="11" t="s">
         <v>48</v>
@@ -4496,7 +4499,7 @@
       <c r="P23" s="14"/>
       <c r="Q23" s="10"/>
     </row>
-    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" hidden="1">
       <c r="A24" s="4"/>
       <c r="B24" s="11" t="s">
         <v>48</v>
@@ -4533,7 +4536,7 @@
       <c r="P24" s="14"/>
       <c r="Q24" s="10"/>
     </row>
-    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" hidden="1">
       <c r="A25" s="4"/>
       <c r="B25" s="11" t="s">
         <v>48</v>
@@ -4566,7 +4569,7 @@
       <c r="P25" s="14"/>
       <c r="Q25" s="10"/>
     </row>
-    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" hidden="1">
       <c r="A26" s="4"/>
       <c r="B26" s="11" t="s">
         <v>48</v>
@@ -4599,7 +4602,7 @@
       <c r="P26" s="14"/>
       <c r="Q26" s="10"/>
     </row>
-    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" hidden="1">
       <c r="A27" s="4"/>
       <c r="B27" s="11" t="s">
         <v>48</v>
@@ -4634,7 +4637,7 @@
       <c r="P27" s="14"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" hidden="1">
       <c r="A28" s="4"/>
       <c r="B28" s="11" t="s">
         <v>48</v>
@@ -4667,7 +4670,7 @@
       <c r="P28" s="14"/>
       <c r="Q28" s="10"/>
     </row>
-    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" hidden="1">
       <c r="A29" s="4"/>
       <c r="B29" s="11" t="s">
         <v>48</v>
@@ -4702,7 +4705,7 @@
       <c r="P29" s="14"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="30" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" hidden="1">
       <c r="A30" s="4"/>
       <c r="B30" s="11" t="s">
         <v>48</v>
@@ -4735,7 +4738,7 @@
       <c r="P30" s="14"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" hidden="1">
       <c r="A31" s="4"/>
       <c r="B31" s="11" t="s">
         <v>48</v>
@@ -4768,7 +4771,7 @@
       <c r="P31" s="14"/>
       <c r="Q31" s="10"/>
     </row>
-    <row r="32" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" hidden="1">
       <c r="A32" s="4"/>
       <c r="B32" s="11" t="s">
         <v>48</v>
@@ -4801,7 +4804,7 @@
       <c r="P32" s="14"/>
       <c r="Q32" s="10"/>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" hidden="1">
       <c r="A33" s="4"/>
       <c r="B33" s="11" t="s">
         <v>48</v>
@@ -4834,7 +4837,7 @@
       <c r="P33" s="14"/>
       <c r="Q33" s="10"/>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" hidden="1">
       <c r="A34" s="4"/>
       <c r="B34" s="11" t="s">
         <v>48</v>
@@ -4867,7 +4870,7 @@
       <c r="P34" s="14"/>
       <c r="Q34" s="10"/>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" hidden="1">
       <c r="A35" s="4"/>
       <c r="B35" s="11" t="s">
         <v>48</v>
@@ -4900,7 +4903,7 @@
       <c r="P35" s="14"/>
       <c r="Q35" s="10"/>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" hidden="1">
       <c r="A36" s="4"/>
       <c r="B36" s="11" t="s">
         <v>48</v>
@@ -4933,7 +4936,7 @@
       <c r="P36" s="14"/>
       <c r="Q36" s="10"/>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" hidden="1">
       <c r="A37" s="4"/>
       <c r="B37" s="11" t="s">
         <v>48</v>
@@ -4966,7 +4969,7 @@
       <c r="P37" s="14"/>
       <c r="Q37" s="10"/>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" hidden="1">
       <c r="A38" s="4"/>
       <c r="B38" s="11" t="s">
         <v>48</v>
@@ -4999,7 +5002,7 @@
       <c r="P38" s="14"/>
       <c r="Q38" s="10"/>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" hidden="1">
       <c r="A39" s="4"/>
       <c r="B39" s="11" t="s">
         <v>48</v>
@@ -5032,7 +5035,7 @@
       <c r="P39" s="14"/>
       <c r="Q39" s="10"/>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" hidden="1">
       <c r="A40" s="4"/>
       <c r="B40" s="11" t="s">
         <v>3</v>
@@ -5065,7 +5068,7 @@
       <c r="P40" s="14"/>
       <c r="Q40" s="10"/>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" hidden="1">
       <c r="A41" s="4"/>
       <c r="B41" s="11" t="s">
         <v>3</v>
@@ -5098,7 +5101,7 @@
       <c r="P41" s="14"/>
       <c r="Q41" s="10"/>
     </row>
-    <row r="42" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="11" t="s">
         <v>3</v>
@@ -5131,7 +5134,7 @@
       <c r="P42" s="14"/>
       <c r="Q42" s="10"/>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" hidden="1">
       <c r="A43" s="4"/>
       <c r="B43" s="11" t="s">
         <v>3</v>
@@ -5164,7 +5167,7 @@
       <c r="P43" s="14"/>
       <c r="Q43" s="10"/>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" hidden="1">
       <c r="A44" s="4"/>
       <c r="B44" s="11" t="s">
         <v>3</v>
@@ -5197,7 +5200,7 @@
       <c r="P44" s="14"/>
       <c r="Q44" s="10"/>
     </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" hidden="1">
       <c r="A45" s="4"/>
       <c r="B45" s="11" t="s">
         <v>3</v>
@@ -5230,7 +5233,7 @@
       <c r="P45" s="14"/>
       <c r="Q45" s="10"/>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" hidden="1">
       <c r="A46" s="4"/>
       <c r="B46" s="11" t="s">
         <v>3</v>
@@ -5265,7 +5268,7 @@
       <c r="P46" s="14"/>
       <c r="Q46" s="10"/>
     </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" hidden="1">
       <c r="A47" s="4"/>
       <c r="B47" s="11" t="s">
         <v>3</v>
@@ -5298,7 +5301,7 @@
       <c r="P47" s="14"/>
       <c r="Q47" s="10"/>
     </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" hidden="1">
       <c r="A48" s="4"/>
       <c r="B48" s="11" t="s">
         <v>3</v>
@@ -5331,7 +5334,7 @@
       <c r="P48" s="14"/>
       <c r="Q48" s="10"/>
     </row>
-    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" hidden="1">
       <c r="A49" s="4"/>
       <c r="B49" s="11" t="s">
         <v>3</v>
@@ -5364,7 +5367,7 @@
       <c r="P49" s="14"/>
       <c r="Q49" s="10"/>
     </row>
-    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" hidden="1">
       <c r="A50" s="4"/>
       <c r="B50" s="11" t="s">
         <v>3</v>
@@ -5397,7 +5400,7 @@
       <c r="P50" s="14"/>
       <c r="Q50" s="10"/>
     </row>
-    <row r="51" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A51" s="4"/>
       <c r="B51" s="11" t="s">
         <v>3</v>
@@ -5434,7 +5437,7 @@
       <c r="P51" s="14"/>
       <c r="Q51" s="10"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" hidden="1">
       <c r="A52" s="4"/>
       <c r="B52" s="11" t="s">
         <v>3</v>
@@ -5471,7 +5474,7 @@
       <c r="P52" s="14"/>
       <c r="Q52" s="10"/>
     </row>
-    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" hidden="1">
       <c r="A53" s="4"/>
       <c r="B53" s="11" t="s">
         <v>3</v>
@@ -5506,7 +5509,7 @@
       <c r="P53" s="14"/>
       <c r="Q53" s="10"/>
     </row>
-    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" hidden="1">
       <c r="A54" s="4"/>
       <c r="B54" s="11" t="s">
         <v>127</v>
@@ -5539,7 +5542,7 @@
       <c r="P54" s="14"/>
       <c r="Q54" s="10"/>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" hidden="1">
       <c r="A55" s="4"/>
       <c r="B55" s="11" t="s">
         <v>127</v>
@@ -5572,7 +5575,7 @@
       <c r="P55" s="14"/>
       <c r="Q55" s="10"/>
     </row>
-    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" hidden="1">
       <c r="A56" s="4"/>
       <c r="B56" s="11" t="s">
         <v>127</v>
@@ -5605,7 +5608,7 @@
       <c r="P56" s="14"/>
       <c r="Q56" s="10"/>
     </row>
-    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" hidden="1">
       <c r="A57" s="4"/>
       <c r="B57" s="11" t="s">
         <v>127</v>
@@ -5638,7 +5641,7 @@
       <c r="P57" s="14"/>
       <c r="Q57" s="10"/>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" hidden="1">
       <c r="A58" s="4"/>
       <c r="B58" s="11" t="s">
         <v>127</v>
@@ -5671,7 +5674,7 @@
       <c r="P58" s="14"/>
       <c r="Q58" s="10"/>
     </row>
-    <row r="59" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A59" s="4"/>
       <c r="B59" s="11" t="s">
         <v>127</v>
@@ -5704,7 +5707,7 @@
       <c r="P59" s="14"/>
       <c r="Q59" s="10"/>
     </row>
-    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" hidden="1">
       <c r="A60" s="4"/>
       <c r="B60" s="11" t="s">
         <v>127</v>
@@ -5737,7 +5740,7 @@
       <c r="P60" s="14"/>
       <c r="Q60" s="10"/>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" hidden="1">
       <c r="A61" s="4"/>
       <c r="B61" s="11" t="s">
         <v>127</v>
@@ -5770,7 +5773,7 @@
       <c r="P61" s="14"/>
       <c r="Q61" s="10"/>
     </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" hidden="1">
       <c r="A62" s="4"/>
       <c r="B62" s="11" t="s">
         <v>127</v>
@@ -5803,7 +5806,7 @@
       <c r="P62" s="14"/>
       <c r="Q62" s="10"/>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" hidden="1">
       <c r="A63" s="4"/>
       <c r="B63" s="11" t="s">
         <v>127</v>
@@ -5836,7 +5839,7 @@
       <c r="P63" s="14"/>
       <c r="Q63" s="10"/>
     </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" hidden="1">
       <c r="A64" s="4"/>
       <c r="B64" s="11" t="s">
         <v>127</v>
@@ -5869,7 +5872,7 @@
       <c r="P64" s="14"/>
       <c r="Q64" s="10"/>
     </row>
-    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" hidden="1">
       <c r="A65" s="4"/>
       <c r="B65" s="11" t="s">
         <v>127</v>
@@ -5902,7 +5905,7 @@
       <c r="P65" s="14"/>
       <c r="Q65" s="10"/>
     </row>
-    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" hidden="1">
       <c r="A66" s="4"/>
       <c r="B66" s="11" t="s">
         <v>127</v>
@@ -5935,7 +5938,7 @@
       <c r="P66" s="14"/>
       <c r="Q66" s="10"/>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" hidden="1">
       <c r="A67" s="4"/>
       <c r="B67" s="11" t="s">
         <v>127</v>
@@ -5968,7 +5971,7 @@
       <c r="P67" s="14"/>
       <c r="Q67" s="10"/>
     </row>
-    <row r="68" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A68" s="4"/>
       <c r="B68" s="11" t="s">
         <v>127</v>
@@ -6003,7 +6006,7 @@
       <c r="P68" s="14"/>
       <c r="Q68" s="10"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" hidden="1">
       <c r="A69" s="4"/>
       <c r="B69" s="11" t="s">
         <v>127</v>
@@ -6040,7 +6043,7 @@
       <c r="P69" s="14"/>
       <c r="Q69" s="10"/>
     </row>
-    <row r="70" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A70" s="4"/>
       <c r="B70" s="11" t="s">
         <v>127</v>
@@ -6077,7 +6080,7 @@
       <c r="P70" s="14"/>
       <c r="Q70" s="10"/>
     </row>
-    <row r="71" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A71" s="4"/>
       <c r="B71" s="11" t="s">
         <v>127</v>
@@ -6114,7 +6117,7 @@
       <c r="P71" s="14"/>
       <c r="Q71" s="10"/>
     </row>
-    <row r="72" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" ht="39.6" hidden="1">
       <c r="A72" s="4"/>
       <c r="B72" s="11" t="s">
         <v>127</v>
@@ -6151,7 +6154,7 @@
       <c r="P72" s="14"/>
       <c r="Q72" s="10"/>
     </row>
-    <row r="73" spans="1:17" ht="51" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" ht="52.8" hidden="1">
       <c r="A73" s="4"/>
       <c r="B73" s="11" t="s">
         <v>127</v>
@@ -6188,7 +6191,7 @@
       <c r="P73" s="14"/>
       <c r="Q73" s="10"/>
     </row>
-    <row r="74" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" ht="79.2" hidden="1">
       <c r="A74" s="4"/>
       <c r="B74" s="11" t="s">
         <v>127</v>
@@ -6225,7 +6228,7 @@
       <c r="P74" s="14"/>
       <c r="Q74" s="10"/>
     </row>
-    <row r="75" spans="1:17" ht="51" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" ht="52.8" hidden="1">
       <c r="A75" s="4"/>
       <c r="B75" s="11" t="s">
         <v>127</v>
@@ -6262,7 +6265,7 @@
       <c r="P75" s="14"/>
       <c r="Q75" s="10"/>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" hidden="1">
       <c r="A76" s="4"/>
       <c r="B76" s="11" t="s">
         <v>127</v>
@@ -6299,7 +6302,7 @@
       <c r="P76" s="14"/>
       <c r="Q76" s="10"/>
     </row>
-    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" hidden="1">
       <c r="A77" s="4"/>
       <c r="B77" s="11" t="s">
         <v>127</v>
@@ -6336,7 +6339,7 @@
       <c r="P77" s="14"/>
       <c r="Q77" s="10"/>
     </row>
-    <row r="78" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A78" s="4"/>
       <c r="B78" s="11" t="s">
         <v>127</v>
@@ -6371,7 +6374,7 @@
       <c r="P78" s="14"/>
       <c r="Q78" s="10"/>
     </row>
-    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" hidden="1">
       <c r="A79" s="4"/>
       <c r="B79" s="11" t="s">
         <v>127</v>
@@ -6406,7 +6409,7 @@
       <c r="P79" s="14"/>
       <c r="Q79" s="10"/>
     </row>
-    <row r="80" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A80" s="4"/>
       <c r="B80" s="11" t="s">
         <v>127</v>
@@ -6443,7 +6446,7 @@
       <c r="P80" s="14"/>
       <c r="Q80" s="10"/>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" hidden="1">
       <c r="A81" s="4"/>
       <c r="B81" s="11" t="s">
         <v>127</v>
@@ -6480,7 +6483,7 @@
       <c r="P81" s="14"/>
       <c r="Q81" s="10"/>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" hidden="1">
       <c r="A82" s="4"/>
       <c r="B82" s="11" t="s">
         <v>127</v>
@@ -6517,7 +6520,7 @@
       <c r="P82" s="14"/>
       <c r="Q82" s="10"/>
     </row>
-    <row r="83" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A83" s="4"/>
       <c r="B83" s="11" t="s">
         <v>127</v>
@@ -6554,7 +6557,7 @@
       <c r="P83" s="14"/>
       <c r="Q83" s="10"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" hidden="1">
       <c r="A84" s="4"/>
       <c r="B84" s="11" t="s">
         <v>127</v>
@@ -6591,7 +6594,7 @@
       <c r="P84" s="14"/>
       <c r="Q84" s="10"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" hidden="1">
       <c r="A85" s="4"/>
       <c r="B85" s="11" t="s">
         <v>127</v>
@@ -6628,7 +6631,7 @@
       <c r="P85" s="14"/>
       <c r="Q85" s="10"/>
     </row>
-    <row r="86" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A86" s="4"/>
       <c r="B86" s="11" t="s">
         <v>127</v>
@@ -6665,7 +6668,7 @@
       <c r="P86" s="14"/>
       <c r="Q86" s="10"/>
     </row>
-    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" hidden="1">
       <c r="A87" s="4"/>
       <c r="B87" s="11" t="s">
         <v>194</v>
@@ -6700,7 +6703,7 @@
       <c r="P87" s="14"/>
       <c r="Q87" s="10"/>
     </row>
-    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" hidden="1">
       <c r="A88" s="4"/>
       <c r="B88" s="11" t="s">
         <v>194</v>
@@ -6735,7 +6738,7 @@
       <c r="P88" s="14"/>
       <c r="Q88" s="10"/>
     </row>
-    <row r="89" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A89" s="4"/>
       <c r="B89" s="11" t="s">
         <v>194</v>
@@ -6772,7 +6775,7 @@
       <c r="P89" s="14"/>
       <c r="Q89" s="10"/>
     </row>
-    <row r="90" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A90" s="4"/>
       <c r="B90" s="11" t="s">
         <v>194</v>
@@ -6809,7 +6812,7 @@
       <c r="P90" s="14"/>
       <c r="Q90" s="10"/>
     </row>
-    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" hidden="1">
       <c r="A91" s="4"/>
       <c r="B91" s="11" t="s">
         <v>194</v>
@@ -6846,7 +6849,7 @@
       <c r="P91" s="14"/>
       <c r="Q91" s="10"/>
     </row>
-    <row r="92" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A92" s="4"/>
       <c r="B92" s="11" t="s">
         <v>194</v>
@@ -6883,7 +6886,7 @@
       <c r="P92" s="14"/>
       <c r="Q92" s="10"/>
     </row>
-    <row r="93" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" hidden="1">
       <c r="A93" s="4"/>
       <c r="B93" s="11" t="s">
         <v>213</v>
@@ -6916,7 +6919,7 @@
       <c r="P93" s="14"/>
       <c r="Q93" s="10"/>
     </row>
-    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" hidden="1">
       <c r="A94" s="4"/>
       <c r="B94" s="11" t="s">
         <v>213</v>
@@ -6951,7 +6954,7 @@
       <c r="P94" s="14"/>
       <c r="Q94" s="10"/>
     </row>
-    <row r="95" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A95" s="4"/>
       <c r="B95" s="11" t="s">
         <v>213</v>
@@ -6988,7 +6991,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A96" s="4"/>
       <c r="B96" s="11" t="s">
         <v>213</v>
@@ -7025,7 +7028,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A97" s="4"/>
       <c r="B97" s="11" t="s">
         <v>213</v>
@@ -7062,7 +7065,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A98" s="4"/>
       <c r="B98" s="11" t="s">
         <v>213</v>
@@ -7099,7 +7102,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A99" s="4"/>
       <c r="B99" s="11" t="s">
         <v>213</v>
@@ -7136,7 +7139,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" hidden="1">
       <c r="A100" s="4"/>
       <c r="B100" s="11" t="s">
         <v>11</v>
@@ -7169,7 +7172,7 @@
       <c r="P100" s="14"/>
       <c r="Q100" s="10"/>
     </row>
-    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" hidden="1">
       <c r="A101" s="4"/>
       <c r="B101" s="11" t="s">
         <v>11</v>
@@ -7202,7 +7205,7 @@
       <c r="P101" s="14"/>
       <c r="Q101" s="10"/>
     </row>
-    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" hidden="1">
       <c r="A102" s="4"/>
       <c r="B102" s="11" t="s">
         <v>11</v>
@@ -7235,7 +7238,7 @@
       <c r="P102" s="14"/>
       <c r="Q102" s="10"/>
     </row>
-    <row r="103" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A103" s="4"/>
       <c r="B103" s="11" t="s">
         <v>11</v>
@@ -7268,7 +7271,7 @@
       <c r="P103" s="14"/>
       <c r="Q103" s="10"/>
     </row>
-    <row r="104" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A104" s="4"/>
       <c r="B104" s="11" t="s">
         <v>11</v>
@@ -7305,7 +7308,7 @@
       <c r="P104" s="14"/>
       <c r="Q104" s="10"/>
     </row>
-    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" hidden="1">
       <c r="A105" s="4"/>
       <c r="B105" s="11" t="s">
         <v>11</v>
@@ -7342,7 +7345,7 @@
       <c r="P105" s="14"/>
       <c r="Q105" s="10"/>
     </row>
-    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" hidden="1">
       <c r="A106" s="4"/>
       <c r="B106" s="11" t="s">
         <v>11</v>
@@ -7379,7 +7382,7 @@
       <c r="P106" s="14"/>
       <c r="Q106" s="10"/>
     </row>
-    <row r="107" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A107" s="4"/>
       <c r="B107" s="11" t="s">
         <v>11</v>
@@ -7416,7 +7419,7 @@
       <c r="P107" s="14"/>
       <c r="Q107" s="10"/>
     </row>
-    <row r="108" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A108" s="4"/>
       <c r="B108" s="11" t="s">
         <v>11</v>
@@ -7453,7 +7456,7 @@
       <c r="P108" s="14"/>
       <c r="Q108" s="10"/>
     </row>
-    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" hidden="1">
       <c r="A109" s="4"/>
       <c r="B109" s="11" t="s">
         <v>11</v>
@@ -7490,7 +7493,7 @@
       <c r="P109" s="14"/>
       <c r="Q109" s="10"/>
     </row>
-    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" hidden="1">
       <c r="A110" s="4"/>
       <c r="B110" s="5" t="s">
         <v>11</v>
@@ -7527,7 +7530,7 @@
       <c r="P110" s="9"/>
       <c r="Q110" s="10"/>
     </row>
-    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" hidden="1">
       <c r="A111" s="4"/>
       <c r="B111" s="5" t="s">
         <v>11</v>
@@ -7564,7 +7567,7 @@
       <c r="P111" s="9"/>
       <c r="Q111" s="10"/>
     </row>
-    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" hidden="1">
       <c r="A112" s="4"/>
       <c r="B112" s="11" t="s">
         <v>11</v>
@@ -7597,7 +7600,7 @@
       <c r="P112" s="14"/>
       <c r="Q112" s="10"/>
     </row>
-    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17">
       <c r="A113" s="4"/>
       <c r="B113" s="11" t="s">
         <v>11</v>
@@ -7609,7 +7612,7 @@
         <v>246</v>
       </c>
       <c r="E113" s="20" t="s">
-        <v>247</v>
+        <v>699</v>
       </c>
       <c r="F113" s="11" t="s">
         <v>27</v>
@@ -7630,7 +7633,7 @@
       <c r="P113" s="14"/>
       <c r="Q113" s="10"/>
     </row>
-    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" hidden="1">
       <c r="A114" s="4"/>
       <c r="B114" s="11" t="s">
         <v>26</v>
@@ -7663,7 +7666,7 @@
       <c r="P114" s="14"/>
       <c r="Q114" s="10"/>
     </row>
-    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" hidden="1">
       <c r="A115" s="4"/>
       <c r="B115" s="11" t="s">
         <v>26</v>
@@ -7696,7 +7699,7 @@
       <c r="P115" s="14"/>
       <c r="Q115" s="10"/>
     </row>
-    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" hidden="1">
       <c r="A116" s="4"/>
       <c r="B116" s="11" t="s">
         <v>26</v>
@@ -7729,7 +7732,7 @@
       <c r="P116" s="14"/>
       <c r="Q116" s="10"/>
     </row>
-    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" hidden="1">
       <c r="A117" s="4"/>
       <c r="B117" s="11" t="s">
         <v>26</v>
@@ -7762,7 +7765,7 @@
       <c r="P117" s="14"/>
       <c r="Q117" s="10"/>
     </row>
-    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" hidden="1">
       <c r="A118" s="4"/>
       <c r="B118" s="11" t="s">
         <v>26</v>
@@ -7795,7 +7798,7 @@
       <c r="P118" s="14"/>
       <c r="Q118" s="10"/>
     </row>
-    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" hidden="1">
       <c r="A119" s="4"/>
       <c r="B119" s="11" t="s">
         <v>26</v>
@@ -7828,7 +7831,7 @@
       <c r="P119" s="14"/>
       <c r="Q119" s="10"/>
     </row>
-    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" hidden="1">
       <c r="A120" s="4"/>
       <c r="B120" s="11" t="s">
         <v>26</v>
@@ -7861,7 +7864,7 @@
       <c r="P120" s="14"/>
       <c r="Q120" s="10"/>
     </row>
-    <row r="121" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" hidden="1">
       <c r="A121" s="4"/>
       <c r="B121" s="11" t="s">
         <v>26</v>
@@ -7894,7 +7897,7 @@
       <c r="P121" s="14"/>
       <c r="Q121" s="10"/>
     </row>
-    <row r="122" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" hidden="1">
       <c r="A122" s="4"/>
       <c r="B122" s="11" t="s">
         <v>26</v>
@@ -7927,7 +7930,7 @@
       <c r="P122" s="14"/>
       <c r="Q122" s="10"/>
     </row>
-    <row r="123" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" hidden="1">
       <c r="A123" s="4"/>
       <c r="B123" s="11" t="s">
         <v>26</v>
@@ -7960,7 +7963,7 @@
       <c r="P123" s="14"/>
       <c r="Q123" s="10"/>
     </row>
-    <row r="124" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" hidden="1">
       <c r="A124" s="4"/>
       <c r="B124" s="11" t="s">
         <v>26</v>
@@ -8001,7 +8004,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="125" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" hidden="1">
       <c r="A125" s="4"/>
       <c r="B125" s="11" t="s">
         <v>26</v>
@@ -8042,7 +8045,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="126" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" hidden="1">
       <c r="A126" s="4"/>
       <c r="B126" s="11" t="s">
         <v>26</v>
@@ -8083,7 +8086,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="127" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" hidden="1">
       <c r="A127" s="4"/>
       <c r="B127" s="11" t="s">
         <v>26</v>
@@ -8118,7 +8121,7 @@
       <c r="P127" s="14"/>
       <c r="Q127" s="10"/>
     </row>
-    <row r="128" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" hidden="1">
       <c r="A128" s="4"/>
       <c r="B128" s="11" t="s">
         <v>26</v>
@@ -8153,7 +8156,7 @@
       <c r="P128" s="14"/>
       <c r="Q128" s="10"/>
     </row>
-    <row r="129" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" hidden="1">
       <c r="A129" s="4"/>
       <c r="B129" s="11" t="s">
         <v>26</v>
@@ -8188,7 +8191,7 @@
       <c r="P129" s="14"/>
       <c r="Q129" s="10"/>
     </row>
-    <row r="130" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" hidden="1">
       <c r="A130" s="4"/>
       <c r="B130" s="11" t="s">
         <v>26</v>
@@ -8225,7 +8228,7 @@
       <c r="P130" s="14"/>
       <c r="Q130" s="10"/>
     </row>
-    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" hidden="1">
       <c r="A131" s="4"/>
       <c r="B131" s="11" t="s">
         <v>26</v>
@@ -8260,7 +8263,7 @@
       <c r="P131" s="14"/>
       <c r="Q131" s="10"/>
     </row>
-    <row r="132" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" hidden="1">
       <c r="A132" s="4"/>
       <c r="B132" s="11" t="s">
         <v>26</v>
@@ -8299,7 +8302,7 @@
       <c r="P132" s="14"/>
       <c r="Q132" s="10"/>
     </row>
-    <row r="133" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" hidden="1">
       <c r="A133" s="4"/>
       <c r="B133" s="11" t="s">
         <v>26</v>
@@ -8338,7 +8341,7 @@
       <c r="P133" s="14"/>
       <c r="Q133" s="10"/>
     </row>
-    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" hidden="1">
       <c r="A134" s="4"/>
       <c r="B134" s="11" t="s">
         <v>26</v>
@@ -8377,7 +8380,7 @@
       <c r="P134" s="14"/>
       <c r="Q134" s="10"/>
     </row>
-    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" hidden="1">
       <c r="A135" s="4"/>
       <c r="B135" s="11" t="s">
         <v>26</v>
@@ -8416,7 +8419,7 @@
       <c r="P135" s="14"/>
       <c r="Q135" s="10"/>
     </row>
-    <row r="136" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" hidden="1">
       <c r="A136" s="4"/>
       <c r="B136" s="11" t="s">
         <v>26</v>
@@ -8455,7 +8458,7 @@
       <c r="P136" s="14"/>
       <c r="Q136" s="10"/>
     </row>
-    <row r="137" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" hidden="1">
       <c r="A137" s="4"/>
       <c r="B137" s="11" t="s">
         <v>26</v>
@@ -8494,7 +8497,7 @@
       <c r="P137" s="14"/>
       <c r="Q137" s="10"/>
     </row>
-    <row r="138" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" hidden="1">
       <c r="A138" s="4"/>
       <c r="B138" s="11" t="s">
         <v>26</v>
@@ -8533,7 +8536,7 @@
       <c r="P138" s="14"/>
       <c r="Q138" s="10"/>
     </row>
-    <row r="139" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" hidden="1">
       <c r="A139" s="4"/>
       <c r="B139" s="11" t="s">
         <v>26</v>
@@ -8572,7 +8575,7 @@
       <c r="P139" s="14"/>
       <c r="Q139" s="10"/>
     </row>
-    <row r="140" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" hidden="1">
       <c r="A140" s="4"/>
       <c r="B140" s="11" t="s">
         <v>26</v>
@@ -8609,7 +8612,7 @@
       <c r="P140" s="14"/>
       <c r="Q140" s="10"/>
     </row>
-    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" hidden="1">
       <c r="A141" s="4"/>
       <c r="B141" s="11" t="s">
         <v>26</v>
@@ -8646,7 +8649,7 @@
       <c r="P141" s="14"/>
       <c r="Q141" s="10"/>
     </row>
-    <row r="142" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" hidden="1">
       <c r="A142" s="4"/>
       <c r="B142" s="11" t="s">
         <v>26</v>
@@ -8683,7 +8686,7 @@
       <c r="P142" s="14"/>
       <c r="Q142" s="10"/>
     </row>
-    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" hidden="1">
       <c r="A143" s="4"/>
       <c r="B143" s="11" t="s">
         <v>26</v>
@@ -8720,7 +8723,7 @@
       <c r="P143" s="14"/>
       <c r="Q143" s="10"/>
     </row>
-    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" hidden="1">
       <c r="A144" s="4"/>
       <c r="B144" s="11" t="s">
         <v>26</v>
@@ -8757,7 +8760,7 @@
       <c r="P144" s="14"/>
       <c r="Q144" s="10"/>
     </row>
-    <row r="145" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" hidden="1">
       <c r="A145" s="4"/>
       <c r="B145" s="11" t="s">
         <v>26</v>
@@ -8794,7 +8797,7 @@
       <c r="P145" s="14"/>
       <c r="Q145" s="10"/>
     </row>
-    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" hidden="1">
       <c r="A146" s="4"/>
       <c r="B146" s="11" t="s">
         <v>26</v>
@@ -8831,7 +8834,7 @@
       <c r="P146" s="14"/>
       <c r="Q146" s="10"/>
     </row>
-    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" hidden="1">
       <c r="A147" s="4"/>
       <c r="B147" s="11" t="s">
         <v>26</v>
@@ -8868,7 +8871,7 @@
       <c r="P147" s="14"/>
       <c r="Q147" s="10"/>
     </row>
-    <row r="148" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" hidden="1">
       <c r="A148" s="4"/>
       <c r="B148" s="11" t="s">
         <v>26</v>
@@ -8905,7 +8908,7 @@
       <c r="P148" s="14"/>
       <c r="Q148" s="10"/>
     </row>
-    <row r="149" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" hidden="1">
       <c r="A149" s="4"/>
       <c r="B149" s="11" t="s">
         <v>26</v>
@@ -8942,7 +8945,7 @@
       <c r="P149" s="14"/>
       <c r="Q149" s="10"/>
     </row>
-    <row r="150" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" hidden="1">
       <c r="A150" s="4"/>
       <c r="B150" s="11" t="s">
         <v>26</v>
@@ -8979,7 +8982,7 @@
       <c r="P150" s="14"/>
       <c r="Q150" s="10"/>
     </row>
-    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" hidden="1">
       <c r="A151" s="4"/>
       <c r="B151" s="11" t="s">
         <v>26</v>
@@ -9016,7 +9019,7 @@
       <c r="P151" s="14"/>
       <c r="Q151" s="10"/>
     </row>
-    <row r="152" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" hidden="1">
       <c r="A152" s="4"/>
       <c r="B152" s="11" t="s">
         <v>26</v>
@@ -9053,7 +9056,7 @@
       <c r="P152" s="14"/>
       <c r="Q152" s="10"/>
     </row>
-    <row r="153" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A153" s="4"/>
       <c r="B153" s="11" t="s">
         <v>26</v>
@@ -9090,7 +9093,7 @@
       <c r="P153" s="14"/>
       <c r="Q153" s="10"/>
     </row>
-    <row r="154" spans="1:17" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" ht="26.4" hidden="1">
       <c r="A154" s="4"/>
       <c r="B154" s="11" t="s">
         <v>32</v>
@@ -9125,7 +9128,7 @@
       <c r="P154" s="14"/>
       <c r="Q154" s="10"/>
     </row>
-    <row r="155" spans="1:17" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" ht="26.4" hidden="1">
       <c r="A155" s="4"/>
       <c r="B155" s="11" t="s">
         <v>32</v>
@@ -9158,7 +9161,7 @@
       <c r="P155" s="14"/>
       <c r="Q155" s="10"/>
     </row>
-    <row r="156" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A156" s="4"/>
       <c r="B156" s="11" t="s">
         <v>32</v>
@@ -9193,7 +9196,7 @@
       <c r="P156" s="14"/>
       <c r="Q156" s="10"/>
     </row>
-    <row r="157" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" hidden="1">
       <c r="A157" s="4"/>
       <c r="B157" s="11" t="s">
         <v>32</v>
@@ -9230,7 +9233,7 @@
       <c r="P157" s="14"/>
       <c r="Q157" s="10"/>
     </row>
-    <row r="158" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" hidden="1">
       <c r="A158" s="4"/>
       <c r="B158" s="11" t="s">
         <v>32</v>
@@ -9267,7 +9270,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A159" s="4"/>
       <c r="B159" s="11" t="s">
         <v>32</v>
@@ -9302,7 +9305,7 @@
       <c r="P159" s="14"/>
       <c r="Q159" s="10"/>
     </row>
-    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:17" hidden="1">
       <c r="A160" s="4"/>
       <c r="B160" s="11" t="s">
         <v>32</v>
@@ -9337,7 +9340,7 @@
       <c r="P160" s="14"/>
       <c r="Q160" s="10"/>
     </row>
-    <row r="161" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A161" s="4"/>
       <c r="B161" s="11" t="s">
         <v>32</v>
@@ -9372,7 +9375,7 @@
       <c r="P161" s="14"/>
       <c r="Q161" s="10"/>
     </row>
-    <row r="162" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" hidden="1">
       <c r="A162" s="4"/>
       <c r="B162" s="11" t="s">
         <v>32</v>
@@ -9407,7 +9410,7 @@
       <c r="P162" s="14"/>
       <c r="Q162" s="10"/>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" hidden="1">
       <c r="A163" s="4"/>
       <c r="B163" s="11" t="s">
         <v>32</v>
@@ -9444,7 +9447,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" hidden="1">
       <c r="A164" s="4"/>
       <c r="B164" s="11" t="s">
         <v>32</v>
@@ -9477,7 +9480,7 @@
       <c r="P164" s="14"/>
       <c r="Q164" s="10"/>
     </row>
-    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" hidden="1">
       <c r="A165" s="4"/>
       <c r="B165" s="11" t="s">
         <v>32</v>
@@ -9510,7 +9513,7 @@
       <c r="P165" s="14"/>
       <c r="Q165" s="10"/>
     </row>
-    <row r="166" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A166" s="4"/>
       <c r="B166" s="11" t="s">
         <v>32</v>
@@ -9543,7 +9546,7 @@
       <c r="P166" s="14"/>
       <c r="Q166" s="10"/>
     </row>
-    <row r="167" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A167" s="4"/>
       <c r="B167" s="11" t="s">
         <v>32</v>
@@ -9576,7 +9579,7 @@
       <c r="P167" s="14"/>
       <c r="Q167" s="10"/>
     </row>
-    <row r="168" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" hidden="1">
       <c r="A168" s="4"/>
       <c r="B168" s="11" t="s">
         <v>32</v>
@@ -9611,7 +9614,7 @@
       <c r="P168" s="14"/>
       <c r="Q168" s="10"/>
     </row>
-    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" hidden="1">
       <c r="A169" s="4"/>
       <c r="B169" s="11" t="s">
         <v>32</v>
@@ -9644,7 +9647,7 @@
       <c r="P169" s="14"/>
       <c r="Q169" s="10"/>
     </row>
-    <row r="170" spans="1:17" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" ht="26.4" hidden="1">
       <c r="A170" s="4"/>
       <c r="B170" s="11" t="s">
         <v>32</v>
@@ -9677,7 +9680,7 @@
       <c r="P170" s="14"/>
       <c r="Q170" s="10"/>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" hidden="1">
       <c r="A171" s="4"/>
       <c r="B171" s="11" t="s">
         <v>32</v>
@@ -9714,7 +9717,7 @@
       <c r="P171" s="14"/>
       <c r="Q171" s="10"/>
     </row>
-    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" hidden="1">
       <c r="A172" s="4"/>
       <c r="B172" s="11" t="s">
         <v>32</v>
@@ -9747,7 +9750,7 @@
       <c r="P172" s="14"/>
       <c r="Q172" s="10"/>
     </row>
-    <row r="173" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" hidden="1">
       <c r="A173" s="4"/>
       <c r="B173" s="11" t="s">
         <v>32</v>
@@ -9780,7 +9783,7 @@
       <c r="P173" s="46"/>
       <c r="Q173" s="10"/>
     </row>
-    <row r="174" spans="1:17" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" ht="26.4" hidden="1">
       <c r="A174" s="4"/>
       <c r="B174" s="11">
         <v>72</v>
@@ -9829,7 +9832,7 @@
       </c>
       <c r="Q174" s="10"/>
     </row>
-    <row r="175" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" hidden="1">
       <c r="A175" s="4"/>
       <c r="B175" s="11">
         <v>72</v>
@@ -9878,7 +9881,7 @@
       </c>
       <c r="Q175" s="10"/>
     </row>
-    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" hidden="1">
       <c r="A176" s="4"/>
       <c r="B176" s="5" t="s">
         <v>353</v>
@@ -9911,7 +9914,7 @@
       <c r="P176" s="9"/>
       <c r="Q176" s="10"/>
     </row>
-    <row r="177" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" hidden="1">
       <c r="A177" s="4"/>
       <c r="B177" s="5" t="s">
         <v>353</v>
@@ -9944,7 +9947,7 @@
       <c r="P177" s="9"/>
       <c r="Q177" s="10"/>
     </row>
-    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" hidden="1">
       <c r="A178" s="4"/>
       <c r="B178" s="5" t="s">
         <v>353</v>
@@ -9977,7 +9980,7 @@
       <c r="P178" s="9"/>
       <c r="Q178" s="10"/>
     </row>
-    <row r="179" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" hidden="1">
       <c r="A179" s="4"/>
       <c r="B179" s="5" t="s">
         <v>353</v>
@@ -10016,7 +10019,7 @@
       </c>
       <c r="Q179" s="10"/>
     </row>
-    <row r="180" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" hidden="1">
       <c r="A180" s="4"/>
       <c r="B180" s="5" t="s">
         <v>353</v>
@@ -10055,7 +10058,7 @@
       </c>
       <c r="Q180" s="10"/>
     </row>
-    <row r="181" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" hidden="1">
       <c r="A181" s="4"/>
       <c r="B181" s="5" t="s">
         <v>353</v>
@@ -10094,7 +10097,7 @@
       </c>
       <c r="Q181" s="10"/>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" hidden="1">
       <c r="A182" s="4"/>
       <c r="B182" s="5" t="s">
         <v>353</v>
@@ -10131,7 +10134,7 @@
       <c r="P182" s="9"/>
       <c r="Q182" s="10"/>
     </row>
-    <row r="183" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" hidden="1">
       <c r="A183" s="4"/>
       <c r="B183" s="5" t="s">
         <v>353</v>
@@ -10166,7 +10169,7 @@
       <c r="P183" s="9"/>
       <c r="Q183" s="10"/>
     </row>
-    <row r="184" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" hidden="1">
       <c r="A184" s="4"/>
       <c r="B184" s="5" t="s">
         <v>353</v>
@@ -10209,7 +10212,7 @@
       </c>
       <c r="Q184" s="10"/>
     </row>
-    <row r="185" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" hidden="1">
       <c r="A185" s="4"/>
       <c r="B185" s="5" t="s">
         <v>353</v>
@@ -10252,7 +10255,7 @@
       </c>
       <c r="Q185" s="10"/>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" hidden="1">
       <c r="A186" s="4"/>
       <c r="B186" s="5" t="s">
         <v>353</v>
@@ -10291,7 +10294,7 @@
       <c r="P186" s="9"/>
       <c r="Q186" s="10"/>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" hidden="1">
       <c r="A187" s="4"/>
       <c r="B187" s="5" t="s">
         <v>353</v>
@@ -10330,7 +10333,7 @@
       <c r="P187" s="9"/>
       <c r="Q187" s="10"/>
     </row>
-    <row r="188" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" hidden="1">
       <c r="A188" s="4"/>
       <c r="B188" s="5" t="s">
         <v>353</v>
@@ -10367,7 +10370,7 @@
       <c r="P188" s="9"/>
       <c r="Q188" s="10"/>
     </row>
-    <row r="189" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" hidden="1">
       <c r="A189" s="4"/>
       <c r="B189" s="5" t="s">
         <v>353</v>
@@ -10404,7 +10407,7 @@
       <c r="P189" s="9"/>
       <c r="Q189" s="10"/>
     </row>
-    <row r="190" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" hidden="1">
       <c r="A190" s="4"/>
       <c r="B190" s="5" t="s">
         <v>390</v>
@@ -10437,7 +10440,7 @@
       <c r="P190" s="9"/>
       <c r="Q190" s="10"/>
     </row>
-    <row r="191" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" hidden="1">
       <c r="A191" s="4"/>
       <c r="B191" s="5" t="s">
         <v>390</v>
@@ -10470,7 +10473,7 @@
       <c r="P191" s="9"/>
       <c r="Q191" s="10"/>
     </row>
-    <row r="192" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" hidden="1">
       <c r="A192" s="4"/>
       <c r="B192" s="5" t="s">
         <v>390</v>
@@ -10503,7 +10506,7 @@
       <c r="P192" s="9"/>
       <c r="Q192" s="10"/>
     </row>
-    <row r="193" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" hidden="1">
       <c r="A193" s="4"/>
       <c r="B193" s="5" t="s">
         <v>390</v>
@@ -10536,7 +10539,7 @@
       <c r="P193" s="9"/>
       <c r="Q193" s="10"/>
     </row>
-    <row r="194" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" hidden="1">
       <c r="A194" s="4"/>
       <c r="B194" s="5" t="s">
         <v>390</v>
@@ -10569,7 +10572,7 @@
       <c r="P194" s="9"/>
       <c r="Q194" s="10"/>
     </row>
-    <row r="195" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" hidden="1">
       <c r="A195" s="4"/>
       <c r="B195" s="5" t="s">
         <v>390</v>
@@ -10608,7 +10611,7 @@
       </c>
       <c r="Q195" s="10"/>
     </row>
-    <row r="196" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" hidden="1">
       <c r="A196" s="4"/>
       <c r="B196" s="5" t="s">
         <v>390</v>
@@ -10647,7 +10650,7 @@
       </c>
       <c r="Q196" s="10"/>
     </row>
-    <row r="197" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" hidden="1">
       <c r="A197" s="4"/>
       <c r="B197" s="5" t="s">
         <v>390</v>
@@ -10686,7 +10689,7 @@
       </c>
       <c r="Q197" s="10"/>
     </row>
-    <row r="198" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" hidden="1">
       <c r="A198" s="4"/>
       <c r="B198" s="5" t="s">
         <v>390</v>
@@ -10725,7 +10728,7 @@
       </c>
       <c r="Q198" s="10"/>
     </row>
-    <row r="199" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" hidden="1">
       <c r="A199" s="4"/>
       <c r="B199" s="5" t="s">
         <v>390</v>
@@ -10762,7 +10765,7 @@
       <c r="P199" s="9"/>
       <c r="Q199" s="10"/>
     </row>
-    <row r="200" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" hidden="1">
       <c r="A200" s="4"/>
       <c r="B200" s="5" t="s">
         <v>390</v>
@@ -10799,7 +10802,7 @@
       <c r="P200" s="64"/>
       <c r="Q200" s="10"/>
     </row>
-    <row r="201" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" hidden="1">
       <c r="A201" s="4"/>
       <c r="B201" s="65">
         <v>60</v>
@@ -10848,7 +10851,7 @@
       </c>
       <c r="Q201" s="10"/>
     </row>
-    <row r="202" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" hidden="1">
       <c r="A202" s="4"/>
       <c r="B202" s="65">
         <v>60</v>
@@ -10897,7 +10900,7 @@
       </c>
       <c r="Q202" s="10"/>
     </row>
-    <row r="203" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" hidden="1">
       <c r="A203" s="4"/>
       <c r="B203" s="65">
         <v>60</v>
@@ -10946,7 +10949,7 @@
       </c>
       <c r="Q203" s="10"/>
     </row>
-    <row r="204" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" hidden="1">
       <c r="A204" s="4"/>
       <c r="B204" s="65">
         <v>60</v>
@@ -10995,7 +10998,7 @@
       </c>
       <c r="Q204" s="10"/>
     </row>
-    <row r="205" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" hidden="1">
       <c r="A205" s="4"/>
       <c r="B205" s="65">
         <v>60</v>
@@ -11044,7 +11047,7 @@
       </c>
       <c r="Q205" s="10"/>
     </row>
-    <row r="206" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" hidden="1">
       <c r="A206" s="4"/>
       <c r="B206" s="65">
         <v>60</v>
@@ -11093,7 +11096,7 @@
       </c>
       <c r="Q206" s="10"/>
     </row>
-    <row r="207" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" hidden="1">
       <c r="A207" s="4"/>
       <c r="B207" s="65">
         <v>60</v>
@@ -11142,7 +11145,7 @@
       </c>
       <c r="Q207" s="10"/>
     </row>
-    <row r="208" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" hidden="1">
       <c r="A208" s="4"/>
       <c r="B208" s="65">
         <v>60</v>
@@ -11191,7 +11194,7 @@
       </c>
       <c r="Q208" s="10"/>
     </row>
-    <row r="209" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" hidden="1">
       <c r="A209" s="4"/>
       <c r="B209" s="65">
         <v>60</v>
@@ -11240,7 +11243,7 @@
       </c>
       <c r="Q209" s="10"/>
     </row>
-    <row r="210" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" hidden="1">
       <c r="A210" s="4"/>
       <c r="B210" s="65">
         <v>60</v>
@@ -11289,7 +11292,7 @@
       </c>
       <c r="Q210" s="10"/>
     </row>
-    <row r="211" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A211" s="4"/>
       <c r="B211" s="70">
         <v>60</v>
@@ -11338,7 +11341,7 @@
       </c>
       <c r="Q211" s="10"/>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" hidden="1">
       <c r="A212" s="4"/>
       <c r="B212" s="7" t="s">
         <v>425</v>
@@ -11375,7 +11378,7 @@
       <c r="P212" s="83"/>
       <c r="Q212" s="10"/>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" hidden="1">
       <c r="A213" s="4"/>
       <c r="B213" s="65">
         <v>60</v>
@@ -11424,7 +11427,7 @@
       </c>
       <c r="Q213" s="10"/>
     </row>
-    <row r="214" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A214" s="4"/>
       <c r="B214" s="65">
         <v>60</v>
@@ -11473,7 +11476,7 @@
       </c>
       <c r="Q214" s="10"/>
     </row>
-    <row r="215" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" hidden="1">
       <c r="A215" s="4"/>
       <c r="B215" s="65">
         <v>60</v>
@@ -11522,7 +11525,7 @@
       </c>
       <c r="Q215" s="10"/>
     </row>
-    <row r="216" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" hidden="1">
       <c r="A216" s="4"/>
       <c r="B216" s="65">
         <v>60</v>
@@ -11571,7 +11574,7 @@
       </c>
       <c r="Q216" s="10"/>
     </row>
-    <row r="217" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" hidden="1">
       <c r="A217" s="4"/>
       <c r="B217" s="65">
         <v>60</v>
@@ -11620,7 +11623,7 @@
       </c>
       <c r="Q217" s="10"/>
     </row>
-    <row r="218" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" hidden="1">
       <c r="A218" s="4"/>
       <c r="B218" s="65">
         <v>60</v>
@@ -11669,7 +11672,7 @@
       </c>
       <c r="Q218" s="10"/>
     </row>
-    <row r="219" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" hidden="1">
       <c r="A219" s="4"/>
       <c r="B219" s="65">
         <v>60</v>
@@ -11718,7 +11721,7 @@
       </c>
       <c r="Q219" s="10"/>
     </row>
-    <row r="220" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" hidden="1">
       <c r="A220" s="4"/>
       <c r="B220" s="65">
         <v>60</v>
@@ -11767,7 +11770,7 @@
       </c>
       <c r="Q220" s="10"/>
     </row>
-    <row r="221" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17" hidden="1">
       <c r="A221" s="4"/>
       <c r="B221" s="65">
         <v>60</v>
@@ -11816,7 +11819,7 @@
       </c>
       <c r="Q221" s="10"/>
     </row>
-    <row r="222" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" hidden="1">
       <c r="A222" s="4"/>
       <c r="B222" s="65">
         <v>60</v>
@@ -11865,7 +11868,7 @@
       </c>
       <c r="Q222" s="10"/>
     </row>
-    <row r="223" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" hidden="1">
       <c r="A223" s="4"/>
       <c r="B223" s="65">
         <v>60</v>
@@ -11914,7 +11917,7 @@
       </c>
       <c r="Q223" s="10"/>
     </row>
-    <row r="224" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17" hidden="1">
       <c r="A224" s="4"/>
       <c r="B224" s="65">
         <v>60</v>
@@ -11963,7 +11966,7 @@
       </c>
       <c r="Q224" s="10"/>
     </row>
-    <row r="225" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" hidden="1">
       <c r="A225" s="4"/>
       <c r="B225" s="65">
         <v>60</v>
@@ -12012,7 +12015,7 @@
       </c>
       <c r="Q225" s="10"/>
     </row>
-    <row r="226" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" hidden="1">
       <c r="A226" s="4"/>
       <c r="B226" s="65">
         <v>60</v>
@@ -12061,7 +12064,7 @@
       </c>
       <c r="Q226" s="10"/>
     </row>
-    <row r="227" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:17" hidden="1">
       <c r="A227" s="4"/>
       <c r="B227" s="65">
         <v>60</v>
@@ -12110,7 +12113,7 @@
       </c>
       <c r="Q227" s="10"/>
     </row>
-    <row r="228" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17" hidden="1">
       <c r="A228" s="4"/>
       <c r="B228" s="65">
         <v>60</v>
@@ -12159,7 +12162,7 @@
       </c>
       <c r="Q228" s="10"/>
     </row>
-    <row r="229" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17" hidden="1">
       <c r="A229" s="4"/>
       <c r="B229" s="65">
         <v>60</v>
@@ -12208,7 +12211,7 @@
       </c>
       <c r="Q229" s="10"/>
     </row>
-    <row r="230" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17" hidden="1">
       <c r="A230" s="4"/>
       <c r="B230" s="65">
         <v>60</v>
@@ -12257,7 +12260,7 @@
       </c>
       <c r="Q230" s="10"/>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" hidden="1">
       <c r="A231" s="4"/>
       <c r="B231" s="65">
         <v>60</v>
@@ -12306,7 +12309,7 @@
       </c>
       <c r="Q231" s="10"/>
     </row>
-    <row r="232" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" hidden="1">
       <c r="A232" s="4"/>
       <c r="B232" s="68">
         <v>60</v>
@@ -12355,7 +12358,7 @@
       </c>
       <c r="Q232" s="10"/>
     </row>
-    <row r="233" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" hidden="1">
       <c r="A233" s="4"/>
       <c r="B233" s="66">
         <v>654</v>
@@ -12404,7 +12407,7 @@
       </c>
       <c r="Q233" s="10"/>
     </row>
-    <row r="234" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" hidden="1">
       <c r="A234" s="4"/>
       <c r="B234" s="66">
         <v>654</v>
@@ -12453,7 +12456,7 @@
       </c>
       <c r="Q234" s="10"/>
     </row>
-    <row r="235" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17" hidden="1">
       <c r="A235" s="4"/>
       <c r="B235" s="66">
         <v>654</v>
@@ -12502,7 +12505,7 @@
       </c>
       <c r="Q235" s="10"/>
     </row>
-    <row r="236" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" hidden="1">
       <c r="A236" s="4"/>
       <c r="B236" s="66">
         <v>654</v>
@@ -12551,7 +12554,7 @@
       </c>
       <c r="Q236" s="10"/>
     </row>
-    <row r="237" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" hidden="1">
       <c r="A237" s="4"/>
       <c r="B237" s="66">
         <v>654</v>
@@ -12600,7 +12603,7 @@
       </c>
       <c r="Q237" s="10"/>
     </row>
-    <row r="238" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:17" hidden="1">
       <c r="A238" s="4"/>
       <c r="B238" s="66">
         <v>654</v>
@@ -12649,7 +12652,7 @@
       </c>
       <c r="Q238" s="10"/>
     </row>
-    <row r="239" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17" hidden="1">
       <c r="A239" s="4"/>
       <c r="B239" s="66">
         <v>654</v>
@@ -12698,7 +12701,7 @@
       </c>
       <c r="Q239" s="10"/>
     </row>
-    <row r="240" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" hidden="1">
       <c r="A240" s="4"/>
       <c r="B240" s="66">
         <v>654</v>
@@ -12747,7 +12750,7 @@
       </c>
       <c r="Q240" s="10"/>
     </row>
-    <row r="241" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17" hidden="1">
       <c r="A241" s="4"/>
       <c r="B241" s="66">
         <v>654</v>
@@ -12794,7 +12797,7 @@
       </c>
       <c r="Q241" s="10"/>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17" hidden="1">
       <c r="A242" s="4"/>
       <c r="B242" s="66">
         <v>654</v>
@@ -12843,7 +12846,7 @@
       </c>
       <c r="Q242" s="10"/>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:17" hidden="1">
       <c r="A243" s="4"/>
       <c r="B243" s="66">
         <v>654</v>
@@ -12892,7 +12895,7 @@
       </c>
       <c r="Q243" s="10"/>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17" hidden="1">
       <c r="A244" s="4"/>
       <c r="B244" s="66">
         <v>654</v>
@@ -12941,7 +12944,7 @@
       </c>
       <c r="Q244" s="10"/>
     </row>
-    <row r="245" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17" hidden="1">
       <c r="A245" s="4"/>
       <c r="B245" s="66">
         <v>654</v>
@@ -12990,7 +12993,7 @@
       </c>
       <c r="Q245" s="10"/>
     </row>
-    <row r="246" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17" hidden="1">
       <c r="A246" s="4"/>
       <c r="B246" s="66">
         <v>654</v>
@@ -13039,7 +13042,7 @@
       </c>
       <c r="Q246" s="10"/>
     </row>
-    <row r="247" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:17" hidden="1">
       <c r="A247" s="4"/>
       <c r="B247" s="66">
         <v>654</v>
@@ -13088,7 +13091,7 @@
       </c>
       <c r="Q247" s="10"/>
     </row>
-    <row r="248" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:17" hidden="1">
       <c r="A248" s="4"/>
       <c r="B248" s="66">
         <v>654</v>
@@ -13137,7 +13140,7 @@
       </c>
       <c r="Q248" s="10"/>
     </row>
-    <row r="249" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:17" hidden="1">
       <c r="A249" s="4"/>
       <c r="B249" s="70">
         <v>654</v>
@@ -13186,7 +13189,7 @@
       </c>
       <c r="Q249" s="10"/>
     </row>
-    <row r="250" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:17" hidden="1">
       <c r="A250" s="4"/>
       <c r="B250" s="11" t="s">
         <v>490</v>
@@ -13221,7 +13224,7 @@
       <c r="P250" s="14"/>
       <c r="Q250" s="10"/>
     </row>
-    <row r="251" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:17" hidden="1">
       <c r="A251" s="4"/>
       <c r="B251" s="11" t="s">
         <v>490</v>
@@ -13256,7 +13259,7 @@
       <c r="P251" s="14"/>
       <c r="Q251" s="10"/>
     </row>
-    <row r="252" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:17" hidden="1">
       <c r="A252" s="4"/>
       <c r="B252" s="11" t="s">
         <v>490</v>
@@ -13293,7 +13296,7 @@
       <c r="P252" s="14"/>
       <c r="Q252" s="10"/>
     </row>
-    <row r="253" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:17" hidden="1">
       <c r="A253" s="4"/>
       <c r="B253" s="11" t="s">
         <v>490</v>
@@ -13334,7 +13337,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="254" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:17" hidden="1">
       <c r="A254" s="4"/>
       <c r="B254" s="11" t="s">
         <v>490</v>
@@ -13373,7 +13376,7 @@
       <c r="P254" s="14"/>
       <c r="Q254" s="10"/>
     </row>
-    <row r="255" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:17" hidden="1">
       <c r="A255" s="4"/>
       <c r="B255" s="11" t="s">
         <v>490</v>
@@ -13412,7 +13415,7 @@
       <c r="P255" s="14"/>
       <c r="Q255" s="10"/>
     </row>
-    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:17" hidden="1">
       <c r="A256" s="4"/>
       <c r="B256" s="11" t="s">
         <v>490</v>
@@ -13451,7 +13454,7 @@
       <c r="P256" s="14"/>
       <c r="Q256" s="10"/>
     </row>
-    <row r="257" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:17" hidden="1">
       <c r="A257" s="4"/>
       <c r="B257" s="5" t="s">
         <v>490</v>
@@ -13490,7 +13493,7 @@
       <c r="P257" s="9"/>
       <c r="Q257" s="10"/>
     </row>
-    <row r="258" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:17" hidden="1">
       <c r="A258" s="4"/>
       <c r="B258" s="11" t="s">
         <v>490</v>
@@ -13527,7 +13530,7 @@
       <c r="P258" s="14"/>
       <c r="Q258" s="10"/>
     </row>
-    <row r="259" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:17" hidden="1">
       <c r="A259" s="4"/>
       <c r="B259" s="11" t="s">
         <v>490</v>
@@ -13564,7 +13567,7 @@
       <c r="P259" s="14"/>
       <c r="Q259" s="10"/>
     </row>
-    <row r="260" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:17" hidden="1">
       <c r="A260" s="4"/>
       <c r="B260" s="11" t="s">
         <v>490</v>
@@ -13599,7 +13602,7 @@
       <c r="P260" s="14"/>
       <c r="Q260" s="10"/>
     </row>
-    <row r="261" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:17" hidden="1">
       <c r="A261" s="4"/>
       <c r="B261" s="11" t="s">
         <v>490</v>
@@ -13634,7 +13637,7 @@
       <c r="P261" s="14"/>
       <c r="Q261" s="10"/>
     </row>
-    <row r="262" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:17" hidden="1">
       <c r="A262" s="4"/>
       <c r="B262" s="5" t="s">
         <v>490</v>
@@ -13671,7 +13674,7 @@
       <c r="P262" s="9"/>
       <c r="Q262" s="10"/>
     </row>
-    <row r="263" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:17" hidden="1">
       <c r="A263" s="4"/>
       <c r="B263" s="5" t="s">
         <v>490</v>
@@ -13706,7 +13709,7 @@
       <c r="P263" s="9"/>
       <c r="Q263" s="10"/>
     </row>
-    <row r="264" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:17" hidden="1">
       <c r="A264" s="4"/>
       <c r="B264" s="5" t="s">
         <v>490</v>
@@ -13741,7 +13744,7 @@
       <c r="P264" s="9"/>
       <c r="Q264" s="10"/>
     </row>
-    <row r="265" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17" hidden="1">
       <c r="A265" s="4"/>
       <c r="B265" s="11" t="s">
         <v>490</v>
@@ -13778,7 +13781,7 @@
       <c r="P265" s="14"/>
       <c r="Q265" s="10"/>
     </row>
-    <row r="266" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:17" hidden="1">
       <c r="A266" s="4"/>
       <c r="B266" s="11" t="s">
         <v>490</v>
@@ -13813,7 +13816,7 @@
       <c r="P266" s="14"/>
       <c r="Q266" s="10"/>
     </row>
-    <row r="267" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:17" hidden="1">
       <c r="A267" s="4"/>
       <c r="B267" s="11" t="s">
         <v>490</v>
@@ -13848,7 +13851,7 @@
       <c r="P267" s="14"/>
       <c r="Q267" s="10"/>
     </row>
-    <row r="268" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:17" hidden="1">
       <c r="A268" s="4"/>
       <c r="B268" s="11" t="s">
         <v>490</v>
@@ -13885,7 +13888,7 @@
       <c r="P268" s="14"/>
       <c r="Q268" s="10"/>
     </row>
-    <row r="269" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:17" hidden="1">
       <c r="A269" s="4"/>
       <c r="B269" s="11" t="s">
         <v>490</v>
@@ -13920,7 +13923,7 @@
       <c r="P269" s="14"/>
       <c r="Q269" s="10"/>
     </row>
-    <row r="270" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:17" hidden="1">
       <c r="A270" s="4"/>
       <c r="B270" s="11" t="s">
         <v>490</v>
@@ -13955,7 +13958,7 @@
       <c r="P270" s="14"/>
       <c r="Q270" s="10"/>
     </row>
-    <row r="271" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:17" hidden="1">
       <c r="A271" s="4"/>
       <c r="B271" s="11" t="s">
         <v>490</v>
@@ -13990,7 +13993,7 @@
       <c r="P271" s="14"/>
       <c r="Q271" s="10"/>
     </row>
-    <row r="272" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:17" hidden="1">
       <c r="A272" s="4"/>
       <c r="B272" s="11" t="s">
         <v>490</v>
@@ -14025,7 +14028,7 @@
       <c r="P272" s="14"/>
       <c r="Q272" s="10"/>
     </row>
-    <row r="273" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:17" hidden="1">
       <c r="A273" s="4"/>
       <c r="B273" s="11" t="s">
         <v>490</v>
@@ -14064,7 +14067,7 @@
       <c r="P273" s="14"/>
       <c r="Q273" s="10"/>
     </row>
-    <row r="274" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:17" hidden="1">
       <c r="A274" s="4"/>
       <c r="B274" s="11" t="s">
         <v>490</v>
@@ -14103,7 +14106,7 @@
       <c r="P274" s="14"/>
       <c r="Q274" s="10"/>
     </row>
-    <row r="275" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:17" hidden="1">
       <c r="A275" s="4"/>
       <c r="B275" s="11" t="s">
         <v>490</v>
@@ -14140,7 +14143,7 @@
       <c r="P275" s="14"/>
       <c r="Q275" s="10"/>
     </row>
-    <row r="276" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:17" hidden="1">
       <c r="A276" s="4"/>
       <c r="B276" s="11" t="s">
         <v>490</v>
@@ -14177,7 +14180,7 @@
       <c r="P276" s="14"/>
       <c r="Q276" s="10"/>
     </row>
-    <row r="277" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:17" hidden="1">
       <c r="A277" s="4"/>
       <c r="B277" s="11" t="s">
         <v>490</v>
@@ -14210,7 +14213,7 @@
       <c r="P277" s="14"/>
       <c r="Q277" s="10"/>
     </row>
-    <row r="278" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:17" hidden="1">
       <c r="A278" s="4"/>
       <c r="B278" s="11" t="s">
         <v>490</v>
@@ -14243,7 +14246,7 @@
       <c r="P278" s="14"/>
       <c r="Q278" s="10"/>
     </row>
-    <row r="279" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:17" hidden="1">
       <c r="A279" s="4"/>
       <c r="B279" s="11" t="s">
         <v>490</v>
@@ -14276,7 +14279,7 @@
       <c r="P279" s="14"/>
       <c r="Q279" s="10"/>
     </row>
-    <row r="280" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:17" hidden="1">
       <c r="A280" s="4"/>
       <c r="B280" s="11" t="s">
         <v>490</v>
@@ -14311,7 +14314,7 @@
       <c r="P280" s="14"/>
       <c r="Q280" s="10"/>
     </row>
-    <row r="281" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:17" hidden="1">
       <c r="A281" s="4"/>
       <c r="B281" s="11" t="s">
         <v>490</v>
@@ -14344,7 +14347,7 @@
       <c r="P281" s="14"/>
       <c r="Q281" s="10"/>
     </row>
-    <row r="282" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:17" hidden="1">
       <c r="A282" s="4"/>
       <c r="B282" s="11" t="s">
         <v>490</v>
@@ -14379,7 +14382,7 @@
       <c r="P282" s="14"/>
       <c r="Q282" s="10"/>
     </row>
-    <row r="283" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:17" hidden="1">
       <c r="A283" s="4"/>
       <c r="B283" s="11" t="s">
         <v>490</v>
@@ -14414,7 +14417,7 @@
       <c r="P283" s="14"/>
       <c r="Q283" s="10"/>
     </row>
-    <row r="284" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:17" hidden="1">
       <c r="A284" s="4"/>
       <c r="B284" s="11" t="s">
         <v>490</v>
@@ -14449,7 +14452,7 @@
       <c r="P284" s="14"/>
       <c r="Q284" s="10"/>
     </row>
-    <row r="285" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:17" hidden="1">
       <c r="A285" s="4"/>
       <c r="B285" s="11" t="s">
         <v>490</v>
@@ -14484,7 +14487,7 @@
       <c r="P285" s="14"/>
       <c r="Q285" s="10"/>
     </row>
-    <row r="286" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:17" hidden="1">
       <c r="A286" s="4"/>
       <c r="B286" s="11" t="s">
         <v>490</v>
@@ -14517,7 +14520,7 @@
       <c r="P286" s="14"/>
       <c r="Q286" s="10"/>
     </row>
-    <row r="287" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:17" hidden="1">
       <c r="A287" s="4"/>
       <c r="B287" s="11" t="s">
         <v>490</v>
@@ -14552,7 +14555,7 @@
       <c r="P287" s="14"/>
       <c r="Q287" s="10"/>
     </row>
-    <row r="288" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:17" hidden="1">
       <c r="A288" s="4"/>
       <c r="B288" s="11" t="s">
         <v>490</v>
@@ -14587,7 +14590,7 @@
       <c r="P288" s="14"/>
       <c r="Q288" s="10"/>
     </row>
-    <row r="289" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" hidden="1">
       <c r="A289" s="4"/>
       <c r="B289" s="11" t="s">
         <v>490</v>
@@ -14622,7 +14625,7 @@
       <c r="P289" s="14"/>
       <c r="Q289" s="10"/>
     </row>
-    <row r="290" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" hidden="1">
       <c r="A290" s="4"/>
       <c r="B290" s="11" t="s">
         <v>490</v>
@@ -14657,7 +14660,7 @@
       <c r="P290" s="14"/>
       <c r="Q290" s="10"/>
     </row>
-    <row r="291" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" hidden="1">
       <c r="A291" s="4"/>
       <c r="B291" s="11" t="s">
         <v>490</v>
@@ -14692,7 +14695,7 @@
       <c r="P291" s="14"/>
       <c r="Q291" s="10"/>
     </row>
-    <row r="292" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" hidden="1">
       <c r="A292" s="4"/>
       <c r="B292" s="11" t="s">
         <v>490</v>
@@ -14727,7 +14730,7 @@
       <c r="P292" s="14"/>
       <c r="Q292" s="10"/>
     </row>
-    <row r="293" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" hidden="1">
       <c r="A293" s="4"/>
       <c r="B293" s="11" t="s">
         <v>490</v>
@@ -14762,7 +14765,7 @@
       <c r="P293" s="14"/>
       <c r="Q293" s="10"/>
     </row>
-    <row r="294" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" hidden="1">
       <c r="A294" s="4"/>
       <c r="B294" s="11" t="s">
         <v>490</v>
@@ -14797,7 +14800,7 @@
       <c r="P294" s="14"/>
       <c r="Q294" s="10"/>
     </row>
-    <row r="295" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" hidden="1">
       <c r="A295" s="4"/>
       <c r="B295" s="11" t="s">
         <v>490</v>
@@ -14832,7 +14835,7 @@
       <c r="P295" s="14"/>
       <c r="Q295" s="10"/>
     </row>
-    <row r="296" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" hidden="1">
       <c r="A296" s="4"/>
       <c r="B296" s="11" t="s">
         <v>490</v>
@@ -14867,7 +14870,7 @@
       <c r="P296" s="14"/>
       <c r="Q296" s="10"/>
     </row>
-    <row r="297" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" hidden="1">
       <c r="A297" s="4"/>
       <c r="B297" s="11" t="s">
         <v>490</v>
@@ -14902,7 +14905,7 @@
       <c r="P297" s="14"/>
       <c r="Q297" s="10"/>
     </row>
-    <row r="298" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A298" s="4"/>
       <c r="B298" s="11" t="s">
         <v>490</v>
@@ -14937,7 +14940,7 @@
       <c r="P298" s="14"/>
       <c r="Q298" s="10"/>
     </row>
-    <row r="299" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A299" s="4"/>
       <c r="B299" s="11" t="s">
         <v>539</v>
@@ -14972,7 +14975,7 @@
       <c r="P299" s="14"/>
       <c r="Q299" s="10"/>
     </row>
-    <row r="300" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" hidden="1">
       <c r="A300" s="4"/>
       <c r="B300" s="11" t="s">
         <v>539</v>
@@ -15007,7 +15010,7 @@
       <c r="P300" s="14"/>
       <c r="Q300" s="10"/>
     </row>
-    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" hidden="1">
       <c r="A301" s="4"/>
       <c r="B301" s="11" t="s">
         <v>545</v>
@@ -15044,7 +15047,7 @@
       <c r="P301" s="14"/>
       <c r="Q301" s="10"/>
     </row>
-    <row r="302" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" hidden="1">
       <c r="A302" s="4"/>
       <c r="B302" s="11" t="s">
         <v>545</v>
@@ -15081,7 +15084,7 @@
       <c r="P302" s="14"/>
       <c r="Q302" s="10"/>
     </row>
-    <row r="303" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" hidden="1">
       <c r="A303" s="4"/>
       <c r="B303" s="11" t="s">
         <v>545</v>
@@ -15118,7 +15121,7 @@
       <c r="P303" s="14"/>
       <c r="Q303" s="10"/>
     </row>
-    <row r="304" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" hidden="1">
       <c r="A304" s="4"/>
       <c r="B304" s="11" t="s">
         <v>545</v>
@@ -15153,7 +15156,7 @@
       <c r="P304" s="14"/>
       <c r="Q304" s="10"/>
     </row>
-    <row r="305" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" hidden="1">
       <c r="A305" s="4"/>
       <c r="B305" s="11" t="s">
         <v>545</v>
@@ -15188,7 +15191,7 @@
       <c r="P305" s="14"/>
       <c r="Q305" s="10"/>
     </row>
-    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" hidden="1">
       <c r="A306" s="4"/>
       <c r="B306" s="11" t="s">
         <v>553</v>
@@ -15221,7 +15224,7 @@
       <c r="P306" s="14"/>
       <c r="Q306" s="10"/>
     </row>
-    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" hidden="1">
       <c r="A307" s="4"/>
       <c r="B307" s="11" t="s">
         <v>553</v>
@@ -15256,7 +15259,7 @@
       <c r="P307" s="14"/>
       <c r="Q307" s="10"/>
     </row>
-    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" hidden="1">
       <c r="A308" s="4"/>
       <c r="B308" s="11" t="s">
         <v>553</v>
@@ -15291,7 +15294,7 @@
       <c r="P308" s="14"/>
       <c r="Q308" s="10"/>
     </row>
-    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" hidden="1">
       <c r="A309" s="4"/>
       <c r="B309" s="11" t="s">
         <v>553</v>
@@ -15326,7 +15329,7 @@
       <c r="P309" s="14"/>
       <c r="Q309" s="10"/>
     </row>
-    <row r="310" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" hidden="1">
       <c r="A310" s="4"/>
       <c r="B310" s="11" t="s">
         <v>553</v>
@@ -15361,7 +15364,7 @@
       <c r="P310" s="14"/>
       <c r="Q310" s="10"/>
     </row>
-    <row r="311" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:17" hidden="1">
       <c r="A311" s="4"/>
       <c r="B311" s="11" t="s">
         <v>553</v>
@@ -15398,7 +15401,7 @@
       <c r="P311" s="14"/>
       <c r="Q311" s="10"/>
     </row>
-    <row r="312" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" hidden="1">
       <c r="A312" s="4"/>
       <c r="B312" s="11" t="s">
         <v>553</v>
@@ -15435,7 +15438,7 @@
       <c r="P312" s="14"/>
       <c r="Q312" s="10"/>
     </row>
-    <row r="313" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A313" s="4"/>
       <c r="B313" s="11" t="s">
         <v>553</v>
@@ -15472,7 +15475,7 @@
       <c r="P313" s="14"/>
       <c r="Q313" s="10"/>
     </row>
-    <row r="314" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:17" hidden="1">
       <c r="A314" s="4"/>
       <c r="B314" s="11" t="s">
         <v>553</v>
@@ -15509,7 +15512,7 @@
       <c r="P314" s="14"/>
       <c r="Q314" s="10"/>
     </row>
-    <row r="315" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A315" s="4"/>
       <c r="B315" s="11" t="s">
         <v>553</v>
@@ -15546,7 +15549,7 @@
       <c r="P315" s="14"/>
       <c r="Q315" s="10"/>
     </row>
-    <row r="316" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" hidden="1">
       <c r="A316" s="4"/>
       <c r="B316" s="11" t="s">
         <v>553</v>
@@ -15581,7 +15584,7 @@
       <c r="P316" s="14"/>
       <c r="Q316" s="10"/>
     </row>
-    <row r="317" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" hidden="1">
       <c r="A317" s="4"/>
       <c r="B317" s="11" t="s">
         <v>553</v>
@@ -15616,7 +15619,7 @@
       <c r="P317" s="14"/>
       <c r="Q317" s="10"/>
     </row>
-    <row r="318" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" hidden="1">
       <c r="A318" s="4"/>
       <c r="B318" s="11" t="s">
         <v>553</v>
@@ -15651,7 +15654,7 @@
       <c r="P318" s="14"/>
       <c r="Q318" s="10"/>
     </row>
-    <row r="319" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" hidden="1">
       <c r="A319" s="4"/>
       <c r="B319" s="11" t="s">
         <v>553</v>
@@ -15686,7 +15689,7 @@
       <c r="P319" s="14"/>
       <c r="Q319" s="10"/>
     </row>
-    <row r="320" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" hidden="1">
       <c r="A320" s="4"/>
       <c r="B320" s="11" t="s">
         <v>553</v>
@@ -15719,7 +15722,7 @@
       <c r="P320" s="14"/>
       <c r="Q320" s="10"/>
     </row>
-    <row r="321" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" hidden="1">
       <c r="A321" s="4"/>
       <c r="B321" s="11" t="s">
         <v>553</v>
@@ -15752,7 +15755,7 @@
       <c r="P321" s="14"/>
       <c r="Q321" s="10"/>
     </row>
-    <row r="322" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" hidden="1">
       <c r="A322" s="4"/>
       <c r="B322" s="11" t="s">
         <v>553</v>
@@ -15785,7 +15788,7 @@
       <c r="P322" s="14"/>
       <c r="Q322" s="10"/>
     </row>
-    <row r="323" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" hidden="1">
       <c r="A323" s="4"/>
       <c r="B323" s="11" t="s">
         <v>553</v>
@@ -15820,7 +15823,7 @@
       <c r="P323" s="14"/>
       <c r="Q323" s="10"/>
     </row>
-    <row r="324" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" hidden="1">
       <c r="A324" s="4"/>
       <c r="B324" s="11" t="s">
         <v>553</v>
@@ -15855,7 +15858,7 @@
       <c r="P324" s="14"/>
       <c r="Q324" s="10"/>
     </row>
-    <row r="325" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" hidden="1">
       <c r="A325" s="4"/>
       <c r="B325" s="11" t="s">
         <v>553</v>
@@ -15890,7 +15893,7 @@
       <c r="P325" s="14"/>
       <c r="Q325" s="10"/>
     </row>
-    <row r="326" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" hidden="1">
       <c r="A326" s="4"/>
       <c r="B326" s="11" t="s">
         <v>553</v>
@@ -15925,7 +15928,7 @@
       <c r="P326" s="14"/>
       <c r="Q326" s="10"/>
     </row>
-    <row r="327" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" hidden="1">
       <c r="A327" s="4"/>
       <c r="B327" s="11" t="s">
         <v>553</v>
@@ -15960,7 +15963,7 @@
       <c r="P327" s="14"/>
       <c r="Q327" s="10"/>
     </row>
-    <row r="328" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" hidden="1">
       <c r="A328" s="4"/>
       <c r="B328" s="11" t="s">
         <v>553</v>
@@ -15995,7 +15998,7 @@
       <c r="P328" s="14"/>
       <c r="Q328" s="10"/>
     </row>
-    <row r="329" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" hidden="1">
       <c r="A329" s="4"/>
       <c r="B329" s="11" t="s">
         <v>553</v>
@@ -16030,7 +16033,7 @@
       <c r="P329" s="14"/>
       <c r="Q329" s="10"/>
     </row>
-    <row r="330" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" hidden="1">
       <c r="A330" s="4"/>
       <c r="B330" s="11" t="s">
         <v>553</v>
@@ -16065,7 +16068,7 @@
       <c r="P330" s="14"/>
       <c r="Q330" s="10"/>
     </row>
-    <row r="331" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" hidden="1">
       <c r="A331" s="4"/>
       <c r="B331" s="11" t="s">
         <v>597</v>
@@ -16098,7 +16101,7 @@
       <c r="P331" s="99"/>
       <c r="Q331" s="10"/>
     </row>
-    <row r="332" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" hidden="1">
       <c r="A332" s="4"/>
       <c r="B332" s="11" t="s">
         <v>597</v>
@@ -16131,7 +16134,7 @@
       <c r="P332" s="103"/>
       <c r="Q332" s="10"/>
     </row>
-    <row r="333" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17" hidden="1">
       <c r="A333" s="4"/>
       <c r="B333" s="11" t="s">
         <v>597</v>
@@ -16164,7 +16167,7 @@
       <c r="P333" s="14"/>
       <c r="Q333" s="10"/>
     </row>
-    <row r="334" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17" hidden="1">
       <c r="A334" s="4"/>
       <c r="B334" s="11" t="s">
         <v>597</v>
@@ -16203,7 +16206,7 @@
       <c r="P334" s="14"/>
       <c r="Q334" s="10"/>
     </row>
-    <row r="335" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17" hidden="1">
       <c r="A335" s="4"/>
       <c r="B335" s="11" t="s">
         <v>606</v>
@@ -16236,7 +16239,7 @@
       <c r="P335" s="14"/>
       <c r="Q335" s="10"/>
     </row>
-    <row r="336" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17" hidden="1">
       <c r="A336" s="4"/>
       <c r="B336" s="11" t="s">
         <v>606</v>
@@ -16269,7 +16272,7 @@
       <c r="P336" s="14"/>
       <c r="Q336" s="10"/>
     </row>
-    <row r="337" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" hidden="1">
       <c r="A337" s="4"/>
       <c r="B337" s="11" t="s">
         <v>606</v>
@@ -16302,7 +16305,7 @@
       <c r="P337" s="14"/>
       <c r="Q337" s="10"/>
     </row>
-    <row r="338" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" hidden="1">
       <c r="A338" s="4"/>
       <c r="B338" s="11" t="s">
         <v>606</v>
@@ -16335,7 +16338,7 @@
       <c r="P338" s="14"/>
       <c r="Q338" s="10"/>
     </row>
-    <row r="339" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" hidden="1">
       <c r="A339" s="4"/>
       <c r="B339" s="11" t="s">
         <v>606</v>
@@ -16368,7 +16371,7 @@
       <c r="P339" s="14"/>
       <c r="Q339" s="10"/>
     </row>
-    <row r="340" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
       <c r="A340" s="4"/>
       <c r="B340" s="11" t="s">
         <v>606</v>
@@ -16401,7 +16404,7 @@
       <c r="P340" s="14"/>
       <c r="Q340" s="10"/>
     </row>
-    <row r="341" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" hidden="1">
       <c r="A341" s="4"/>
       <c r="B341" s="11" t="s">
         <v>41</v>
@@ -16440,7 +16443,7 @@
       <c r="P341" s="14"/>
       <c r="Q341" s="10"/>
     </row>
-    <row r="342" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" hidden="1">
       <c r="A342" s="4"/>
       <c r="B342" s="11" t="s">
         <v>41</v>
@@ -16479,7 +16482,7 @@
       <c r="P342" s="14"/>
       <c r="Q342" s="10"/>
     </row>
-    <row r="343" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" hidden="1">
       <c r="A343" s="4"/>
       <c r="B343" s="11" t="s">
         <v>41</v>
@@ -16518,7 +16521,7 @@
       <c r="P343" s="14"/>
       <c r="Q343" s="10"/>
     </row>
-    <row r="344" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" hidden="1">
       <c r="A344" s="4"/>
       <c r="B344" s="11" t="s">
         <v>41</v>
@@ -16557,7 +16560,7 @@
       <c r="P344" s="14"/>
       <c r="Q344" s="10"/>
     </row>
-    <row r="345" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" hidden="1">
       <c r="A345" s="4"/>
       <c r="B345" s="11" t="s">
         <v>41</v>
@@ -16596,7 +16599,7 @@
       <c r="P345" s="14"/>
       <c r="Q345" s="10"/>
     </row>
-    <row r="346" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" hidden="1">
       <c r="A346" s="4"/>
       <c r="B346" s="11" t="s">
         <v>41</v>
@@ -16635,7 +16638,7 @@
       <c r="P346" s="14"/>
       <c r="Q346" s="10"/>
     </row>
-    <row r="347" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17" hidden="1">
       <c r="A347" s="4"/>
       <c r="B347" s="11" t="s">
         <v>41</v>
@@ -16674,7 +16677,7 @@
       <c r="P347" s="14"/>
       <c r="Q347" s="10"/>
     </row>
-    <row r="348" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:17" hidden="1">
       <c r="A348" s="4"/>
       <c r="B348" s="5" t="s">
         <v>41</v>
@@ -16713,7 +16716,7 @@
       <c r="P348" s="9"/>
       <c r="Q348" s="10"/>
     </row>
-    <row r="349" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" hidden="1">
       <c r="A349" s="4"/>
       <c r="B349" s="5" t="s">
         <v>41</v>
@@ -16752,7 +16755,7 @@
       <c r="P349" s="9"/>
       <c r="Q349" s="10"/>
     </row>
-    <row r="350" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" hidden="1">
       <c r="A350" s="4"/>
       <c r="B350" s="11" t="s">
         <v>41</v>
@@ -16791,7 +16794,7 @@
       <c r="P350" s="9"/>
       <c r="Q350" s="10"/>
     </row>
-    <row r="351" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:17" hidden="1">
       <c r="A351" s="4"/>
       <c r="B351" s="11" t="s">
         <v>41</v>
@@ -16830,7 +16833,7 @@
       <c r="P351" s="14"/>
       <c r="Q351" s="10"/>
     </row>
-    <row r="352" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:17" hidden="1">
       <c r="A352" s="4"/>
       <c r="B352" s="11" t="s">
         <v>41</v>
@@ -16869,7 +16872,7 @@
       <c r="P352" s="14"/>
       <c r="Q352" s="10"/>
     </row>
-    <row r="353" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17" hidden="1">
       <c r="A353" s="4"/>
       <c r="B353" s="11" t="s">
         <v>41</v>
@@ -16908,7 +16911,7 @@
       <c r="P353" s="14"/>
       <c r="Q353" s="10"/>
     </row>
-    <row r="354" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17" hidden="1">
       <c r="A354" s="4"/>
       <c r="B354" s="11" t="s">
         <v>41</v>
@@ -16947,7 +16950,7 @@
       <c r="P354" s="14"/>
       <c r="Q354" s="10"/>
     </row>
-    <row r="355" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:17" hidden="1">
       <c r="A355" s="4"/>
       <c r="B355" s="11" t="s">
         <v>41</v>
@@ -16986,7 +16989,7 @@
       <c r="P355" s="14"/>
       <c r="Q355" s="10"/>
     </row>
-    <row r="356" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:17" hidden="1">
       <c r="A356" s="4"/>
       <c r="B356" s="11" t="s">
         <v>41</v>
@@ -17025,7 +17028,7 @@
       <c r="P356" s="14"/>
       <c r="Q356" s="10"/>
     </row>
-    <row r="357" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:17" hidden="1">
       <c r="A357" s="4"/>
       <c r="B357" s="11" t="s">
         <v>41</v>
@@ -17064,7 +17067,7 @@
       <c r="P357" s="14"/>
       <c r="Q357" s="10"/>
     </row>
-    <row r="358" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17" hidden="1">
       <c r="A358" s="4"/>
       <c r="B358" s="11" t="s">
         <v>41</v>
@@ -17103,7 +17106,7 @@
       <c r="P358" s="14"/>
       <c r="Q358" s="10"/>
     </row>
-    <row r="359" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:17" hidden="1">
       <c r="A359" s="4"/>
       <c r="B359" s="11" t="s">
         <v>41</v>
@@ -17142,7 +17145,7 @@
       <c r="P359" s="14"/>
       <c r="Q359" s="10"/>
     </row>
-    <row r="360" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:17" hidden="1">
       <c r="A360" s="4"/>
       <c r="B360" s="5" t="s">
         <v>41</v>
@@ -17181,7 +17184,7 @@
       <c r="P360" s="9"/>
       <c r="Q360" s="10"/>
     </row>
-    <row r="361" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:17" hidden="1">
       <c r="A361" s="4"/>
       <c r="B361" s="5" t="s">
         <v>41</v>
@@ -17220,7 +17223,7 @@
       <c r="P361" s="9"/>
       <c r="Q361" s="10"/>
     </row>
-    <row r="362" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:17" hidden="1">
       <c r="A362" s="4"/>
       <c r="B362" s="11" t="s">
         <v>41</v>
@@ -17259,7 +17262,7 @@
       <c r="P362" s="14"/>
       <c r="Q362" s="10"/>
     </row>
-    <row r="363" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:17" hidden="1">
       <c r="A363" s="4"/>
       <c r="B363" s="11" t="s">
         <v>41</v>
@@ -17298,7 +17301,7 @@
       <c r="P363" s="14"/>
       <c r="Q363" s="10"/>
     </row>
-    <row r="364" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" hidden="1">
       <c r="A364" s="4"/>
       <c r="B364" s="11" t="s">
         <v>41</v>
@@ -17337,7 +17340,7 @@
       <c r="P364" s="14"/>
       <c r="Q364" s="10"/>
     </row>
-    <row r="365" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:17" hidden="1">
       <c r="A365" s="4"/>
       <c r="B365" s="11" t="s">
         <v>41</v>
@@ -17374,7 +17377,7 @@
       <c r="P365" s="14"/>
       <c r="Q365" s="10"/>
     </row>
-    <row r="366" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:17" hidden="1">
       <c r="A366" s="4"/>
       <c r="B366" s="11" t="s">
         <v>41</v>
@@ -17411,7 +17414,7 @@
       <c r="P366" s="14"/>
       <c r="Q366" s="10"/>
     </row>
-    <row r="367" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:17" hidden="1">
       <c r="A367" s="4"/>
       <c r="B367" s="11" t="s">
         <v>41</v>
@@ -17448,7 +17451,7 @@
       <c r="P367" s="14"/>
       <c r="Q367" s="10"/>
     </row>
-    <row r="368" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:17" hidden="1">
       <c r="A368" s="4"/>
       <c r="B368" s="21" t="s">
         <v>41</v>
@@ -17481,7 +17484,7 @@
       <c r="P368" s="24"/>
       <c r="Q368" s="10"/>
     </row>
-    <row r="369" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:17" hidden="1">
       <c r="A369" s="4"/>
       <c r="B369" s="21" t="s">
         <v>41</v>
@@ -17514,7 +17517,7 @@
       <c r="P369" s="24"/>
       <c r="Q369" s="10"/>
     </row>
-    <row r="370" spans="1:17" s="111" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:17" s="111" customFormat="1" hidden="1">
       <c r="A370" s="4"/>
       <c r="B370" s="5" t="s">
         <v>41</v>
@@ -17549,7 +17552,7 @@
       <c r="P370" s="9"/>
       <c r="Q370" s="10"/>
     </row>
-    <row r="371" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:17" hidden="1">
       <c r="A371" s="4"/>
       <c r="B371" s="112" t="s">
         <v>41</v>
@@ -17584,7 +17587,7 @@
       <c r="P371" s="115"/>
       <c r="Q371" s="10"/>
     </row>
-    <row r="372" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:17" hidden="1">
       <c r="A372" s="4"/>
       <c r="B372" s="112" t="s">
         <v>41</v>
@@ -17617,7 +17620,7 @@
       <c r="P372" s="9"/>
       <c r="Q372" s="10"/>
     </row>
-    <row r="373" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:17" hidden="1">
       <c r="A373" s="4"/>
       <c r="B373" s="112" t="s">
         <v>41</v>
@@ -17652,7 +17655,7 @@
       <c r="P373" s="115"/>
       <c r="Q373" s="10"/>
     </row>
-    <row r="374" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:17" hidden="1">
       <c r="A374" s="4"/>
       <c r="B374" s="112" t="s">
         <v>41</v>
@@ -17687,7 +17690,7 @@
       <c r="P374" s="9"/>
       <c r="Q374" s="10"/>
     </row>
-    <row r="375" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:17" hidden="1">
       <c r="A375" s="4"/>
       <c r="B375" s="5" t="s">
         <v>41</v>
@@ -17726,7 +17729,7 @@
       <c r="P375" s="9"/>
       <c r="Q375" s="10"/>
     </row>
-    <row r="376" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:17" hidden="1">
       <c r="A376" s="4"/>
       <c r="B376" s="5" t="s">
         <v>41</v>
@@ -17765,7 +17768,7 @@
       <c r="P376" s="9"/>
       <c r="Q376" s="10"/>
     </row>
-    <row r="377" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:17" hidden="1">
       <c r="A377" s="4"/>
       <c r="B377" s="5" t="s">
         <v>41</v>
@@ -17804,7 +17807,7 @@
       <c r="P377" s="9"/>
       <c r="Q377" s="10"/>
     </row>
-    <row r="378" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:17" hidden="1">
       <c r="A378" s="4"/>
       <c r="B378" s="5" t="s">
         <v>41</v>
@@ -17843,7 +17846,7 @@
       <c r="P378" s="9"/>
       <c r="Q378" s="10"/>
     </row>
-    <row r="379" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:17" hidden="1">
       <c r="A379" s="4"/>
       <c r="B379" s="5" t="s">
         <v>41</v>
@@ -17882,7 +17885,7 @@
       <c r="P379" s="9"/>
       <c r="Q379" s="10"/>
     </row>
-    <row r="380" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:17" hidden="1">
       <c r="A380" s="4"/>
       <c r="B380" s="5" t="s">
         <v>41</v>
@@ -17923,7 +17926,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="381" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:17" hidden="1">
       <c r="A381" s="4"/>
       <c r="B381" s="5" t="s">
         <v>41</v>
@@ -17962,7 +17965,7 @@
       <c r="P381" s="9"/>
       <c r="Q381" s="10"/>
     </row>
-    <row r="382" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:17" hidden="1">
       <c r="A382" s="4"/>
       <c r="B382" s="5" t="s">
         <v>41</v>
@@ -18001,7 +18004,7 @@
       <c r="P382" s="9"/>
       <c r="Q382" s="10"/>
     </row>
-    <row r="383" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:17" hidden="1">
       <c r="A383" s="4"/>
       <c r="B383" s="112" t="s">
         <v>41</v>
@@ -18034,7 +18037,7 @@
       <c r="P383" s="9"/>
       <c r="Q383" s="10"/>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:17" hidden="1">
       <c r="A384" s="117"/>
       <c r="B384" s="118"/>
       <c r="C384" s="118"/>
@@ -18053,7 +18056,7 @@
       <c r="P384" s="121"/>
       <c r="Q384" s="122"/>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:17" hidden="1">
       <c r="A385" s="117"/>
       <c r="B385" s="118"/>
       <c r="C385" s="118"/>
@@ -18072,7 +18075,7 @@
       <c r="P385" s="121"/>
       <c r="Q385" s="122"/>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:17" hidden="1">
       <c r="A386" s="117"/>
       <c r="B386" s="118"/>
       <c r="C386" s="118"/>
@@ -18091,7 +18094,7 @@
       <c r="P386" s="121"/>
       <c r="Q386" s="122"/>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:17" hidden="1">
       <c r="A387" s="117"/>
       <c r="B387" s="118"/>
       <c r="C387" s="118"/>
@@ -18113,15 +18116,31 @@
   </sheetData>
   <autoFilter ref="A1:S387" xr:uid="{F526BBEE-5653-4805-B17E-42C581B68C69}">
     <filterColumn colId="4">
-      <filters blank="1">
-        <filter val="N/A"/>
+      <filters>
+        <filter val="68_CIM_0F6CBAEDE0081BE277627DD8EBDFF240"/>
+        <filter val="68_CIM_1E2DF4543D85E40AA57080D3FDD9086D"/>
+        <filter val="68_CIM_2479202AE40BEB5443C7DCF0FC4BD5E3"/>
+        <filter val="68_CIM_2E165A02DEE5CD02A4A1F50A6F0FE556"/>
+        <filter val="68_CIM_3E34D62006DB48F8634C08A5EAFAD566"/>
+        <filter val="68_CIM_4BC5712ECBFF2D28E135A916C97B6FC1"/>
+        <filter val="68_CIM_4EB8C16894D9A775EF6526AA73275F1C"/>
+        <filter val="68_CIM_5E83620A8390E131950E009E3482B09E"/>
+        <filter val="68_CIM_60F39F02198D856414F9AB87B00D6EC6"/>
+        <filter val="68_CIM_625BDC6839DD942ED72DA6E6D9E55809"/>
+        <filter val="68_CIM_7993507C2EFE4883CBA1AE5673511ECF"/>
+        <filter val="68_CIM_909090B63C222B820D811475DFF6511F"/>
+        <filter val="68_CIM_93E4EDD9E199E8E3645A4858A0851F97"/>
+        <filter val="68_CIM_9C17BEA96EA496953BD8C10EE5F51AE0"/>
+        <filter val="68_CIM_A3BE410904204122F5CBD116B7D83569"/>
+        <filter val="68_CIM_A52A35007D3F56EE4971080B0DACBC45"/>
+        <filter val="68_CIM_B03D773BB87F8234AA80584A43D34120"/>
+        <filter val="68_CIM_C3C0D91D7BEBACB0B6F9127E3F4E48A9"/>
+        <filter val="68_CIM_F28F179764E68DC942FFD608AA87B372"/>
       </filters>
     </filterColumn>
     <filterColumn colId="8">
-      <filters blank="1">
-        <filter val="N/A"/>
-        <filter val="Not found"/>
-        <filter val="TBC"/>
+      <filters>
+        <filter val="68_CIM_C3C0D91D7BEBACB0B6F9127E3F4E48A9"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Update dependency template (open, mainframe)
</commit_message>
<xml_diff>
--- a/data/online-dependency-mf_template.xlsx
+++ b/data/online-dependency-mf_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Source Code\Python\jupiter-service-inventory-importer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B8DCA0-4A48-4A72-AEC2-D37F2FF0AFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E02888-809C-4FD6-B6A9-43B567C162B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7920" yWindow="516" windowWidth="30588" windowHeight="13572" xr2:uid="{4FBA0D69-02F4-49F3-BDD3-DC0A888CC705}"/>
   </bookViews>
@@ -3636,14 +3636,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F526BBEE-5653-4805-B17E-42C581B68C69}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor theme="8" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:S387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D398" sqref="D398"/>
+      <selection pane="bottomLeft" activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="18"/>
@@ -3719,7 +3719,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="2" spans="1:19" hidden="1">
+    <row r="2" spans="1:19">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>3</v>
@@ -3756,7 +3756,7 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="1:19" hidden="1">
+    <row r="3" spans="1:19">
       <c r="A3" s="4"/>
       <c r="B3" s="11" t="s">
         <v>11</v>
@@ -3791,7 +3791,7 @@
       <c r="P3" s="14"/>
       <c r="Q3" s="10"/>
     </row>
-    <row r="4" spans="1:19" hidden="1">
+    <row r="4" spans="1:19">
       <c r="A4" s="4"/>
       <c r="B4" s="11" t="s">
         <v>11</v>
@@ -3826,7 +3826,7 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="10"/>
     </row>
-    <row r="5" spans="1:19" hidden="1">
+    <row r="5" spans="1:19">
       <c r="A5" s="4"/>
       <c r="B5" s="11" t="s">
         <v>11</v>
@@ -3861,7 +3861,7 @@
       <c r="P5" s="14"/>
       <c r="Q5" s="10"/>
     </row>
-    <row r="6" spans="1:19" ht="26.1" hidden="1" customHeight="1">
+    <row r="6" spans="1:19" ht="26.1" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="11" t="s">
         <v>11</v>
@@ -3896,7 +3896,7 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="10"/>
     </row>
-    <row r="7" spans="1:19" hidden="1">
+    <row r="7" spans="1:19">
       <c r="A7" s="4"/>
       <c r="B7" s="11" t="s">
         <v>11</v>
@@ -3931,7 +3931,7 @@
       <c r="P7" s="14"/>
       <c r="Q7" s="10"/>
     </row>
-    <row r="8" spans="1:19" hidden="1">
+    <row r="8" spans="1:19">
       <c r="A8" s="4"/>
       <c r="B8" s="11" t="s">
         <v>26</v>
@@ -3966,7 +3966,7 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="1:19" hidden="1">
+    <row r="9" spans="1:19">
       <c r="A9" s="4"/>
       <c r="B9" s="11" t="s">
         <v>32</v>
@@ -4003,7 +4003,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:19" hidden="1">
+    <row r="10" spans="1:19">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="s">
         <v>32</v>
@@ -4040,7 +4040,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="11" spans="1:19" ht="18.600000000000001" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="21" t="s">
         <v>41</v>
@@ -4075,7 +4075,7 @@
       <c r="P11" s="24"/>
       <c r="Q11" s="10"/>
     </row>
-    <row r="12" spans="1:19" hidden="1">
+    <row r="12" spans="1:19">
       <c r="A12" s="4"/>
       <c r="B12" s="11" t="s">
         <v>48</v>
@@ -4110,7 +4110,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" hidden="1">
+    <row r="13" spans="1:19">
       <c r="A13" s="4"/>
       <c r="B13" s="11" t="s">
         <v>48</v>
@@ -4147,7 +4147,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" hidden="1">
+    <row r="14" spans="1:19">
       <c r="A14" s="4"/>
       <c r="B14" s="11" t="s">
         <v>48</v>
@@ -4184,7 +4184,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" hidden="1">
+    <row r="15" spans="1:19">
       <c r="A15" s="4"/>
       <c r="B15" s="11" t="s">
         <v>48</v>
@@ -4219,7 +4219,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" hidden="1">
+    <row r="16" spans="1:19">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="s">
         <v>48</v>
@@ -4254,7 +4254,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" hidden="1">
+    <row r="17" spans="1:19">
       <c r="A17" s="4"/>
       <c r="B17" s="11" t="s">
         <v>48</v>
@@ -4289,7 +4289,7 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="1:19" hidden="1">
+    <row r="18" spans="1:19">
       <c r="A18" s="4"/>
       <c r="B18" s="11" t="s">
         <v>48</v>
@@ -4324,7 +4324,7 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="1:19" hidden="1">
+    <row r="19" spans="1:19">
       <c r="A19" s="4"/>
       <c r="B19" s="11" t="s">
         <v>48</v>
@@ -4359,7 +4359,7 @@
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
     </row>
-    <row r="20" spans="1:19" hidden="1">
+    <row r="20" spans="1:19">
       <c r="A20" s="4"/>
       <c r="B20" s="11" t="s">
         <v>48</v>
@@ -4394,7 +4394,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
     </row>
-    <row r="21" spans="1:19" hidden="1">
+    <row r="21" spans="1:19">
       <c r="A21" s="4"/>
       <c r="B21" s="11" t="s">
         <v>48</v>
@@ -4429,7 +4429,7 @@
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
     </row>
-    <row r="22" spans="1:19" hidden="1">
+    <row r="22" spans="1:19">
       <c r="A22" s="4"/>
       <c r="B22" s="11" t="s">
         <v>48</v>
@@ -4462,7 +4462,7 @@
       <c r="P22" s="14"/>
       <c r="Q22" s="10"/>
     </row>
-    <row r="23" spans="1:19" hidden="1">
+    <row r="23" spans="1:19">
       <c r="A23" s="4"/>
       <c r="B23" s="11" t="s">
         <v>48</v>
@@ -4499,7 +4499,7 @@
       <c r="P23" s="14"/>
       <c r="Q23" s="10"/>
     </row>
-    <row r="24" spans="1:19" hidden="1">
+    <row r="24" spans="1:19">
       <c r="A24" s="4"/>
       <c r="B24" s="11" t="s">
         <v>48</v>
@@ -4536,7 +4536,7 @@
       <c r="P24" s="14"/>
       <c r="Q24" s="10"/>
     </row>
-    <row r="25" spans="1:19" hidden="1">
+    <row r="25" spans="1:19">
       <c r="A25" s="4"/>
       <c r="B25" s="11" t="s">
         <v>48</v>
@@ -4569,7 +4569,7 @@
       <c r="P25" s="14"/>
       <c r="Q25" s="10"/>
     </row>
-    <row r="26" spans="1:19" hidden="1">
+    <row r="26" spans="1:19">
       <c r="A26" s="4"/>
       <c r="B26" s="11" t="s">
         <v>48</v>
@@ -4602,7 +4602,7 @@
       <c r="P26" s="14"/>
       <c r="Q26" s="10"/>
     </row>
-    <row r="27" spans="1:19" hidden="1">
+    <row r="27" spans="1:19">
       <c r="A27" s="4"/>
       <c r="B27" s="11" t="s">
         <v>48</v>
@@ -4637,7 +4637,7 @@
       <c r="P27" s="14"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="1:19" hidden="1">
+    <row r="28" spans="1:19">
       <c r="A28" s="4"/>
       <c r="B28" s="11" t="s">
         <v>48</v>
@@ -4670,7 +4670,7 @@
       <c r="P28" s="14"/>
       <c r="Q28" s="10"/>
     </row>
-    <row r="29" spans="1:19" hidden="1">
+    <row r="29" spans="1:19">
       <c r="A29" s="4"/>
       <c r="B29" s="11" t="s">
         <v>48</v>
@@ -4705,7 +4705,7 @@
       <c r="P29" s="14"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="30" spans="1:19" hidden="1">
+    <row r="30" spans="1:19">
       <c r="A30" s="4"/>
       <c r="B30" s="11" t="s">
         <v>48</v>
@@ -4738,7 +4738,7 @@
       <c r="P30" s="14"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="1:19" hidden="1">
+    <row r="31" spans="1:19">
       <c r="A31" s="4"/>
       <c r="B31" s="11" t="s">
         <v>48</v>
@@ -4771,7 +4771,7 @@
       <c r="P31" s="14"/>
       <c r="Q31" s="10"/>
     </row>
-    <row r="32" spans="1:19" hidden="1">
+    <row r="32" spans="1:19">
       <c r="A32" s="4"/>
       <c r="B32" s="11" t="s">
         <v>48</v>
@@ -4804,7 +4804,7 @@
       <c r="P32" s="14"/>
       <c r="Q32" s="10"/>
     </row>
-    <row r="33" spans="1:17" hidden="1">
+    <row r="33" spans="1:17">
       <c r="A33" s="4"/>
       <c r="B33" s="11" t="s">
         <v>48</v>
@@ -4837,7 +4837,7 @@
       <c r="P33" s="14"/>
       <c r="Q33" s="10"/>
     </row>
-    <row r="34" spans="1:17" hidden="1">
+    <row r="34" spans="1:17">
       <c r="A34" s="4"/>
       <c r="B34" s="11" t="s">
         <v>48</v>
@@ -4870,7 +4870,7 @@
       <c r="P34" s="14"/>
       <c r="Q34" s="10"/>
     </row>
-    <row r="35" spans="1:17" hidden="1">
+    <row r="35" spans="1:17">
       <c r="A35" s="4"/>
       <c r="B35" s="11" t="s">
         <v>48</v>
@@ -4903,7 +4903,7 @@
       <c r="P35" s="14"/>
       <c r="Q35" s="10"/>
     </row>
-    <row r="36" spans="1:17" hidden="1">
+    <row r="36" spans="1:17">
       <c r="A36" s="4"/>
       <c r="B36" s="11" t="s">
         <v>48</v>
@@ -4936,7 +4936,7 @@
       <c r="P36" s="14"/>
       <c r="Q36" s="10"/>
     </row>
-    <row r="37" spans="1:17" hidden="1">
+    <row r="37" spans="1:17">
       <c r="A37" s="4"/>
       <c r="B37" s="11" t="s">
         <v>48</v>
@@ -4969,7 +4969,7 @@
       <c r="P37" s="14"/>
       <c r="Q37" s="10"/>
     </row>
-    <row r="38" spans="1:17" hidden="1">
+    <row r="38" spans="1:17">
       <c r="A38" s="4"/>
       <c r="B38" s="11" t="s">
         <v>48</v>
@@ -5002,7 +5002,7 @@
       <c r="P38" s="14"/>
       <c r="Q38" s="10"/>
     </row>
-    <row r="39" spans="1:17" hidden="1">
+    <row r="39" spans="1:17">
       <c r="A39" s="4"/>
       <c r="B39" s="11" t="s">
         <v>48</v>
@@ -5035,7 +5035,7 @@
       <c r="P39" s="14"/>
       <c r="Q39" s="10"/>
     </row>
-    <row r="40" spans="1:17" hidden="1">
+    <row r="40" spans="1:17">
       <c r="A40" s="4"/>
       <c r="B40" s="11" t="s">
         <v>3</v>
@@ -5068,7 +5068,7 @@
       <c r="P40" s="14"/>
       <c r="Q40" s="10"/>
     </row>
-    <row r="41" spans="1:17" hidden="1">
+    <row r="41" spans="1:17">
       <c r="A41" s="4"/>
       <c r="B41" s="11" t="s">
         <v>3</v>
@@ -5101,7 +5101,7 @@
       <c r="P41" s="14"/>
       <c r="Q41" s="10"/>
     </row>
-    <row r="42" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="42" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="11" t="s">
         <v>3</v>
@@ -5134,7 +5134,7 @@
       <c r="P42" s="14"/>
       <c r="Q42" s="10"/>
     </row>
-    <row r="43" spans="1:17" hidden="1">
+    <row r="43" spans="1:17">
       <c r="A43" s="4"/>
       <c r="B43" s="11" t="s">
         <v>3</v>
@@ -5167,7 +5167,7 @@
       <c r="P43" s="14"/>
       <c r="Q43" s="10"/>
     </row>
-    <row r="44" spans="1:17" hidden="1">
+    <row r="44" spans="1:17">
       <c r="A44" s="4"/>
       <c r="B44" s="11" t="s">
         <v>3</v>
@@ -5200,7 +5200,7 @@
       <c r="P44" s="14"/>
       <c r="Q44" s="10"/>
     </row>
-    <row r="45" spans="1:17" hidden="1">
+    <row r="45" spans="1:17">
       <c r="A45" s="4"/>
       <c r="B45" s="11" t="s">
         <v>3</v>
@@ -5233,7 +5233,7 @@
       <c r="P45" s="14"/>
       <c r="Q45" s="10"/>
     </row>
-    <row r="46" spans="1:17" hidden="1">
+    <row r="46" spans="1:17">
       <c r="A46" s="4"/>
       <c r="B46" s="11" t="s">
         <v>3</v>
@@ -5268,7 +5268,7 @@
       <c r="P46" s="14"/>
       <c r="Q46" s="10"/>
     </row>
-    <row r="47" spans="1:17" hidden="1">
+    <row r="47" spans="1:17">
       <c r="A47" s="4"/>
       <c r="B47" s="11" t="s">
         <v>3</v>
@@ -5301,7 +5301,7 @@
       <c r="P47" s="14"/>
       <c r="Q47" s="10"/>
     </row>
-    <row r="48" spans="1:17" hidden="1">
+    <row r="48" spans="1:17">
       <c r="A48" s="4"/>
       <c r="B48" s="11" t="s">
         <v>3</v>
@@ -5334,7 +5334,7 @@
       <c r="P48" s="14"/>
       <c r="Q48" s="10"/>
     </row>
-    <row r="49" spans="1:17" hidden="1">
+    <row r="49" spans="1:17">
       <c r="A49" s="4"/>
       <c r="B49" s="11" t="s">
         <v>3</v>
@@ -5367,7 +5367,7 @@
       <c r="P49" s="14"/>
       <c r="Q49" s="10"/>
     </row>
-    <row r="50" spans="1:17" hidden="1">
+    <row r="50" spans="1:17">
       <c r="A50" s="4"/>
       <c r="B50" s="11" t="s">
         <v>3</v>
@@ -5400,7 +5400,7 @@
       <c r="P50" s="14"/>
       <c r="Q50" s="10"/>
     </row>
-    <row r="51" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="51" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A51" s="4"/>
       <c r="B51" s="11" t="s">
         <v>3</v>
@@ -5437,7 +5437,7 @@
       <c r="P51" s="14"/>
       <c r="Q51" s="10"/>
     </row>
-    <row r="52" spans="1:17" hidden="1">
+    <row r="52" spans="1:17">
       <c r="A52" s="4"/>
       <c r="B52" s="11" t="s">
         <v>3</v>
@@ -5474,7 +5474,7 @@
       <c r="P52" s="14"/>
       <c r="Q52" s="10"/>
     </row>
-    <row r="53" spans="1:17" hidden="1">
+    <row r="53" spans="1:17">
       <c r="A53" s="4"/>
       <c r="B53" s="11" t="s">
         <v>3</v>
@@ -5509,7 +5509,7 @@
       <c r="P53" s="14"/>
       <c r="Q53" s="10"/>
     </row>
-    <row r="54" spans="1:17" hidden="1">
+    <row r="54" spans="1:17">
       <c r="A54" s="4"/>
       <c r="B54" s="11" t="s">
         <v>127</v>
@@ -5542,7 +5542,7 @@
       <c r="P54" s="14"/>
       <c r="Q54" s="10"/>
     </row>
-    <row r="55" spans="1:17" hidden="1">
+    <row r="55" spans="1:17">
       <c r="A55" s="4"/>
       <c r="B55" s="11" t="s">
         <v>127</v>
@@ -5575,7 +5575,7 @@
       <c r="P55" s="14"/>
       <c r="Q55" s="10"/>
     </row>
-    <row r="56" spans="1:17" hidden="1">
+    <row r="56" spans="1:17">
       <c r="A56" s="4"/>
       <c r="B56" s="11" t="s">
         <v>127</v>
@@ -5608,7 +5608,7 @@
       <c r="P56" s="14"/>
       <c r="Q56" s="10"/>
     </row>
-    <row r="57" spans="1:17" hidden="1">
+    <row r="57" spans="1:17">
       <c r="A57" s="4"/>
       <c r="B57" s="11" t="s">
         <v>127</v>
@@ -5641,7 +5641,7 @@
       <c r="P57" s="14"/>
       <c r="Q57" s="10"/>
     </row>
-    <row r="58" spans="1:17" hidden="1">
+    <row r="58" spans="1:17">
       <c r="A58" s="4"/>
       <c r="B58" s="11" t="s">
         <v>127</v>
@@ -5674,7 +5674,7 @@
       <c r="P58" s="14"/>
       <c r="Q58" s="10"/>
     </row>
-    <row r="59" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="59" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A59" s="4"/>
       <c r="B59" s="11" t="s">
         <v>127</v>
@@ -5707,7 +5707,7 @@
       <c r="P59" s="14"/>
       <c r="Q59" s="10"/>
     </row>
-    <row r="60" spans="1:17" hidden="1">
+    <row r="60" spans="1:17">
       <c r="A60" s="4"/>
       <c r="B60" s="11" t="s">
         <v>127</v>
@@ -5740,7 +5740,7 @@
       <c r="P60" s="14"/>
       <c r="Q60" s="10"/>
     </row>
-    <row r="61" spans="1:17" hidden="1">
+    <row r="61" spans="1:17">
       <c r="A61" s="4"/>
       <c r="B61" s="11" t="s">
         <v>127</v>
@@ -5773,7 +5773,7 @@
       <c r="P61" s="14"/>
       <c r="Q61" s="10"/>
     </row>
-    <row r="62" spans="1:17" hidden="1">
+    <row r="62" spans="1:17">
       <c r="A62" s="4"/>
       <c r="B62" s="11" t="s">
         <v>127</v>
@@ -5806,7 +5806,7 @@
       <c r="P62" s="14"/>
       <c r="Q62" s="10"/>
     </row>
-    <row r="63" spans="1:17" hidden="1">
+    <row r="63" spans="1:17">
       <c r="A63" s="4"/>
       <c r="B63" s="11" t="s">
         <v>127</v>
@@ -5839,7 +5839,7 @@
       <c r="P63" s="14"/>
       <c r="Q63" s="10"/>
     </row>
-    <row r="64" spans="1:17" hidden="1">
+    <row r="64" spans="1:17">
       <c r="A64" s="4"/>
       <c r="B64" s="11" t="s">
         <v>127</v>
@@ -5872,7 +5872,7 @@
       <c r="P64" s="14"/>
       <c r="Q64" s="10"/>
     </row>
-    <row r="65" spans="1:17" hidden="1">
+    <row r="65" spans="1:17">
       <c r="A65" s="4"/>
       <c r="B65" s="11" t="s">
         <v>127</v>
@@ -5905,7 +5905,7 @@
       <c r="P65" s="14"/>
       <c r="Q65" s="10"/>
     </row>
-    <row r="66" spans="1:17" hidden="1">
+    <row r="66" spans="1:17">
       <c r="A66" s="4"/>
       <c r="B66" s="11" t="s">
         <v>127</v>
@@ -5938,7 +5938,7 @@
       <c r="P66" s="14"/>
       <c r="Q66" s="10"/>
     </row>
-    <row r="67" spans="1:17" hidden="1">
+    <row r="67" spans="1:17">
       <c r="A67" s="4"/>
       <c r="B67" s="11" t="s">
         <v>127</v>
@@ -5971,7 +5971,7 @@
       <c r="P67" s="14"/>
       <c r="Q67" s="10"/>
     </row>
-    <row r="68" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="68" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A68" s="4"/>
       <c r="B68" s="11" t="s">
         <v>127</v>
@@ -6006,7 +6006,7 @@
       <c r="P68" s="14"/>
       <c r="Q68" s="10"/>
     </row>
-    <row r="69" spans="1:17" hidden="1">
+    <row r="69" spans="1:17">
       <c r="A69" s="4"/>
       <c r="B69" s="11" t="s">
         <v>127</v>
@@ -6043,7 +6043,7 @@
       <c r="P69" s="14"/>
       <c r="Q69" s="10"/>
     </row>
-    <row r="70" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="70" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A70" s="4"/>
       <c r="B70" s="11" t="s">
         <v>127</v>
@@ -6080,7 +6080,7 @@
       <c r="P70" s="14"/>
       <c r="Q70" s="10"/>
     </row>
-    <row r="71" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="71" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A71" s="4"/>
       <c r="B71" s="11" t="s">
         <v>127</v>
@@ -6117,7 +6117,7 @@
       <c r="P71" s="14"/>
       <c r="Q71" s="10"/>
     </row>
-    <row r="72" spans="1:17" ht="39.6" hidden="1">
+    <row r="72" spans="1:17" ht="39.6">
       <c r="A72" s="4"/>
       <c r="B72" s="11" t="s">
         <v>127</v>
@@ -6154,7 +6154,7 @@
       <c r="P72" s="14"/>
       <c r="Q72" s="10"/>
     </row>
-    <row r="73" spans="1:17" ht="52.8" hidden="1">
+    <row r="73" spans="1:17" ht="52.8">
       <c r="A73" s="4"/>
       <c r="B73" s="11" t="s">
         <v>127</v>
@@ -6191,7 +6191,7 @@
       <c r="P73" s="14"/>
       <c r="Q73" s="10"/>
     </row>
-    <row r="74" spans="1:17" ht="79.2" hidden="1">
+    <row r="74" spans="1:17" ht="79.2">
       <c r="A74" s="4"/>
       <c r="B74" s="11" t="s">
         <v>127</v>
@@ -6228,7 +6228,7 @@
       <c r="P74" s="14"/>
       <c r="Q74" s="10"/>
     </row>
-    <row r="75" spans="1:17" ht="52.8" hidden="1">
+    <row r="75" spans="1:17" ht="52.8">
       <c r="A75" s="4"/>
       <c r="B75" s="11" t="s">
         <v>127</v>
@@ -6265,7 +6265,7 @@
       <c r="P75" s="14"/>
       <c r="Q75" s="10"/>
     </row>
-    <row r="76" spans="1:17" hidden="1">
+    <row r="76" spans="1:17">
       <c r="A76" s="4"/>
       <c r="B76" s="11" t="s">
         <v>127</v>
@@ -6302,7 +6302,7 @@
       <c r="P76" s="14"/>
       <c r="Q76" s="10"/>
     </row>
-    <row r="77" spans="1:17" hidden="1">
+    <row r="77" spans="1:17">
       <c r="A77" s="4"/>
       <c r="B77" s="11" t="s">
         <v>127</v>
@@ -6339,7 +6339,7 @@
       <c r="P77" s="14"/>
       <c r="Q77" s="10"/>
     </row>
-    <row r="78" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="78" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A78" s="4"/>
       <c r="B78" s="11" t="s">
         <v>127</v>
@@ -6374,7 +6374,7 @@
       <c r="P78" s="14"/>
       <c r="Q78" s="10"/>
     </row>
-    <row r="79" spans="1:17" hidden="1">
+    <row r="79" spans="1:17">
       <c r="A79" s="4"/>
       <c r="B79" s="11" t="s">
         <v>127</v>
@@ -6409,7 +6409,7 @@
       <c r="P79" s="14"/>
       <c r="Q79" s="10"/>
     </row>
-    <row r="80" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="80" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A80" s="4"/>
       <c r="B80" s="11" t="s">
         <v>127</v>
@@ -6446,7 +6446,7 @@
       <c r="P80" s="14"/>
       <c r="Q80" s="10"/>
     </row>
-    <row r="81" spans="1:17" hidden="1">
+    <row r="81" spans="1:17">
       <c r="A81" s="4"/>
       <c r="B81" s="11" t="s">
         <v>127</v>
@@ -6483,7 +6483,7 @@
       <c r="P81" s="14"/>
       <c r="Q81" s="10"/>
     </row>
-    <row r="82" spans="1:17" hidden="1">
+    <row r="82" spans="1:17">
       <c r="A82" s="4"/>
       <c r="B82" s="11" t="s">
         <v>127</v>
@@ -6520,7 +6520,7 @@
       <c r="P82" s="14"/>
       <c r="Q82" s="10"/>
     </row>
-    <row r="83" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="83" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A83" s="4"/>
       <c r="B83" s="11" t="s">
         <v>127</v>
@@ -6557,7 +6557,7 @@
       <c r="P83" s="14"/>
       <c r="Q83" s="10"/>
     </row>
-    <row r="84" spans="1:17" hidden="1">
+    <row r="84" spans="1:17">
       <c r="A84" s="4"/>
       <c r="B84" s="11" t="s">
         <v>127</v>
@@ -6594,7 +6594,7 @@
       <c r="P84" s="14"/>
       <c r="Q84" s="10"/>
     </row>
-    <row r="85" spans="1:17" hidden="1">
+    <row r="85" spans="1:17">
       <c r="A85" s="4"/>
       <c r="B85" s="11" t="s">
         <v>127</v>
@@ -6631,7 +6631,7 @@
       <c r="P85" s="14"/>
       <c r="Q85" s="10"/>
     </row>
-    <row r="86" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="86" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A86" s="4"/>
       <c r="B86" s="11" t="s">
         <v>127</v>
@@ -6668,7 +6668,7 @@
       <c r="P86" s="14"/>
       <c r="Q86" s="10"/>
     </row>
-    <row r="87" spans="1:17" hidden="1">
+    <row r="87" spans="1:17">
       <c r="A87" s="4"/>
       <c r="B87" s="11" t="s">
         <v>194</v>
@@ -6703,7 +6703,7 @@
       <c r="P87" s="14"/>
       <c r="Q87" s="10"/>
     </row>
-    <row r="88" spans="1:17" hidden="1">
+    <row r="88" spans="1:17">
       <c r="A88" s="4"/>
       <c r="B88" s="11" t="s">
         <v>194</v>
@@ -6738,7 +6738,7 @@
       <c r="P88" s="14"/>
       <c r="Q88" s="10"/>
     </row>
-    <row r="89" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="89" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A89" s="4"/>
       <c r="B89" s="11" t="s">
         <v>194</v>
@@ -6775,7 +6775,7 @@
       <c r="P89" s="14"/>
       <c r="Q89" s="10"/>
     </row>
-    <row r="90" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="90" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A90" s="4"/>
       <c r="B90" s="11" t="s">
         <v>194</v>
@@ -6812,7 +6812,7 @@
       <c r="P90" s="14"/>
       <c r="Q90" s="10"/>
     </row>
-    <row r="91" spans="1:17" hidden="1">
+    <row r="91" spans="1:17">
       <c r="A91" s="4"/>
       <c r="B91" s="11" t="s">
         <v>194</v>
@@ -6849,7 +6849,7 @@
       <c r="P91" s="14"/>
       <c r="Q91" s="10"/>
     </row>
-    <row r="92" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="92" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A92" s="4"/>
       <c r="B92" s="11" t="s">
         <v>194</v>
@@ -6886,7 +6886,7 @@
       <c r="P92" s="14"/>
       <c r="Q92" s="10"/>
     </row>
-    <row r="93" spans="1:17" hidden="1">
+    <row r="93" spans="1:17">
       <c r="A93" s="4"/>
       <c r="B93" s="11" t="s">
         <v>213</v>
@@ -6919,7 +6919,7 @@
       <c r="P93" s="14"/>
       <c r="Q93" s="10"/>
     </row>
-    <row r="94" spans="1:17" hidden="1">
+    <row r="94" spans="1:17">
       <c r="A94" s="4"/>
       <c r="B94" s="11" t="s">
         <v>213</v>
@@ -6954,7 +6954,7 @@
       <c r="P94" s="14"/>
       <c r="Q94" s="10"/>
     </row>
-    <row r="95" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="95" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A95" s="4"/>
       <c r="B95" s="11" t="s">
         <v>213</v>
@@ -6991,7 +6991,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="96" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A96" s="4"/>
       <c r="B96" s="11" t="s">
         <v>213</v>
@@ -7028,7 +7028,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="97" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A97" s="4"/>
       <c r="B97" s="11" t="s">
         <v>213</v>
@@ -7065,7 +7065,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="98" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A98" s="4"/>
       <c r="B98" s="11" t="s">
         <v>213</v>
@@ -7102,7 +7102,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="99" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A99" s="4"/>
       <c r="B99" s="11" t="s">
         <v>213</v>
@@ -7139,7 +7139,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="100" spans="1:17" hidden="1">
+    <row r="100" spans="1:17">
       <c r="A100" s="4"/>
       <c r="B100" s="11" t="s">
         <v>11</v>
@@ -7172,7 +7172,7 @@
       <c r="P100" s="14"/>
       <c r="Q100" s="10"/>
     </row>
-    <row r="101" spans="1:17" hidden="1">
+    <row r="101" spans="1:17">
       <c r="A101" s="4"/>
       <c r="B101" s="11" t="s">
         <v>11</v>
@@ -7205,7 +7205,7 @@
       <c r="P101" s="14"/>
       <c r="Q101" s="10"/>
     </row>
-    <row r="102" spans="1:17" hidden="1">
+    <row r="102" spans="1:17">
       <c r="A102" s="4"/>
       <c r="B102" s="11" t="s">
         <v>11</v>
@@ -7238,7 +7238,7 @@
       <c r="P102" s="14"/>
       <c r="Q102" s="10"/>
     </row>
-    <row r="103" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="103" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A103" s="4"/>
       <c r="B103" s="11" t="s">
         <v>11</v>
@@ -7271,7 +7271,7 @@
       <c r="P103" s="14"/>
       <c r="Q103" s="10"/>
     </row>
-    <row r="104" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="104" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A104" s="4"/>
       <c r="B104" s="11" t="s">
         <v>11</v>
@@ -7308,7 +7308,7 @@
       <c r="P104" s="14"/>
       <c r="Q104" s="10"/>
     </row>
-    <row r="105" spans="1:17" hidden="1">
+    <row r="105" spans="1:17">
       <c r="A105" s="4"/>
       <c r="B105" s="11" t="s">
         <v>11</v>
@@ -7345,7 +7345,7 @@
       <c r="P105" s="14"/>
       <c r="Q105" s="10"/>
     </row>
-    <row r="106" spans="1:17" hidden="1">
+    <row r="106" spans="1:17">
       <c r="A106" s="4"/>
       <c r="B106" s="11" t="s">
         <v>11</v>
@@ -7382,7 +7382,7 @@
       <c r="P106" s="14"/>
       <c r="Q106" s="10"/>
     </row>
-    <row r="107" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="107" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A107" s="4"/>
       <c r="B107" s="11" t="s">
         <v>11</v>
@@ -7419,7 +7419,7 @@
       <c r="P107" s="14"/>
       <c r="Q107" s="10"/>
     </row>
-    <row r="108" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="108" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A108" s="4"/>
       <c r="B108" s="11" t="s">
         <v>11</v>
@@ -7456,7 +7456,7 @@
       <c r="P108" s="14"/>
       <c r="Q108" s="10"/>
     </row>
-    <row r="109" spans="1:17" hidden="1">
+    <row r="109" spans="1:17">
       <c r="A109" s="4"/>
       <c r="B109" s="11" t="s">
         <v>11</v>
@@ -7493,7 +7493,7 @@
       <c r="P109" s="14"/>
       <c r="Q109" s="10"/>
     </row>
-    <row r="110" spans="1:17" hidden="1">
+    <row r="110" spans="1:17">
       <c r="A110" s="4"/>
       <c r="B110" s="5" t="s">
         <v>11</v>
@@ -7530,7 +7530,7 @@
       <c r="P110" s="9"/>
       <c r="Q110" s="10"/>
     </row>
-    <row r="111" spans="1:17" hidden="1">
+    <row r="111" spans="1:17">
       <c r="A111" s="4"/>
       <c r="B111" s="5" t="s">
         <v>11</v>
@@ -7567,7 +7567,7 @@
       <c r="P111" s="9"/>
       <c r="Q111" s="10"/>
     </row>
-    <row r="112" spans="1:17" hidden="1">
+    <row r="112" spans="1:17">
       <c r="A112" s="4"/>
       <c r="B112" s="11" t="s">
         <v>11</v>
@@ -7633,7 +7633,7 @@
       <c r="P113" s="14"/>
       <c r="Q113" s="10"/>
     </row>
-    <row r="114" spans="1:17" hidden="1">
+    <row r="114" spans="1:17">
       <c r="A114" s="4"/>
       <c r="B114" s="11" t="s">
         <v>26</v>
@@ -7666,7 +7666,7 @@
       <c r="P114" s="14"/>
       <c r="Q114" s="10"/>
     </row>
-    <row r="115" spans="1:17" hidden="1">
+    <row r="115" spans="1:17">
       <c r="A115" s="4"/>
       <c r="B115" s="11" t="s">
         <v>26</v>
@@ -7699,7 +7699,7 @@
       <c r="P115" s="14"/>
       <c r="Q115" s="10"/>
     </row>
-    <row r="116" spans="1:17" hidden="1">
+    <row r="116" spans="1:17">
       <c r="A116" s="4"/>
       <c r="B116" s="11" t="s">
         <v>26</v>
@@ -7732,7 +7732,7 @@
       <c r="P116" s="14"/>
       <c r="Q116" s="10"/>
     </row>
-    <row r="117" spans="1:17" hidden="1">
+    <row r="117" spans="1:17">
       <c r="A117" s="4"/>
       <c r="B117" s="11" t="s">
         <v>26</v>
@@ -7765,7 +7765,7 @@
       <c r="P117" s="14"/>
       <c r="Q117" s="10"/>
     </row>
-    <row r="118" spans="1:17" hidden="1">
+    <row r="118" spans="1:17">
       <c r="A118" s="4"/>
       <c r="B118" s="11" t="s">
         <v>26</v>
@@ -7798,7 +7798,7 @@
       <c r="P118" s="14"/>
       <c r="Q118" s="10"/>
     </row>
-    <row r="119" spans="1:17" hidden="1">
+    <row r="119" spans="1:17">
       <c r="A119" s="4"/>
       <c r="B119" s="11" t="s">
         <v>26</v>
@@ -7831,7 +7831,7 @@
       <c r="P119" s="14"/>
       <c r="Q119" s="10"/>
     </row>
-    <row r="120" spans="1:17" hidden="1">
+    <row r="120" spans="1:17">
       <c r="A120" s="4"/>
       <c r="B120" s="11" t="s">
         <v>26</v>
@@ -7864,7 +7864,7 @@
       <c r="P120" s="14"/>
       <c r="Q120" s="10"/>
     </row>
-    <row r="121" spans="1:17" hidden="1">
+    <row r="121" spans="1:17">
       <c r="A121" s="4"/>
       <c r="B121" s="11" t="s">
         <v>26</v>
@@ -7897,7 +7897,7 @@
       <c r="P121" s="14"/>
       <c r="Q121" s="10"/>
     </row>
-    <row r="122" spans="1:17" hidden="1">
+    <row r="122" spans="1:17">
       <c r="A122" s="4"/>
       <c r="B122" s="11" t="s">
         <v>26</v>
@@ -7930,7 +7930,7 @@
       <c r="P122" s="14"/>
       <c r="Q122" s="10"/>
     </row>
-    <row r="123" spans="1:17" hidden="1">
+    <row r="123" spans="1:17">
       <c r="A123" s="4"/>
       <c r="B123" s="11" t="s">
         <v>26</v>
@@ -7963,7 +7963,7 @@
       <c r="P123" s="14"/>
       <c r="Q123" s="10"/>
     </row>
-    <row r="124" spans="1:17" hidden="1">
+    <row r="124" spans="1:17">
       <c r="A124" s="4"/>
       <c r="B124" s="11" t="s">
         <v>26</v>
@@ -8004,7 +8004,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="125" spans="1:17" hidden="1">
+    <row r="125" spans="1:17">
       <c r="A125" s="4"/>
       <c r="B125" s="11" t="s">
         <v>26</v>
@@ -8045,7 +8045,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="126" spans="1:17" hidden="1">
+    <row r="126" spans="1:17">
       <c r="A126" s="4"/>
       <c r="B126" s="11" t="s">
         <v>26</v>
@@ -8086,7 +8086,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="127" spans="1:17" hidden="1">
+    <row r="127" spans="1:17">
       <c r="A127" s="4"/>
       <c r="B127" s="11" t="s">
         <v>26</v>
@@ -8121,7 +8121,7 @@
       <c r="P127" s="14"/>
       <c r="Q127" s="10"/>
     </row>
-    <row r="128" spans="1:17" hidden="1">
+    <row r="128" spans="1:17">
       <c r="A128" s="4"/>
       <c r="B128" s="11" t="s">
         <v>26</v>
@@ -8156,7 +8156,7 @@
       <c r="P128" s="14"/>
       <c r="Q128" s="10"/>
     </row>
-    <row r="129" spans="1:17" hidden="1">
+    <row r="129" spans="1:17">
       <c r="A129" s="4"/>
       <c r="B129" s="11" t="s">
         <v>26</v>
@@ -8191,7 +8191,7 @@
       <c r="P129" s="14"/>
       <c r="Q129" s="10"/>
     </row>
-    <row r="130" spans="1:17" hidden="1">
+    <row r="130" spans="1:17">
       <c r="A130" s="4"/>
       <c r="B130" s="11" t="s">
         <v>26</v>
@@ -8228,7 +8228,7 @@
       <c r="P130" s="14"/>
       <c r="Q130" s="10"/>
     </row>
-    <row r="131" spans="1:17" hidden="1">
+    <row r="131" spans="1:17">
       <c r="A131" s="4"/>
       <c r="B131" s="11" t="s">
         <v>26</v>
@@ -8263,7 +8263,7 @@
       <c r="P131" s="14"/>
       <c r="Q131" s="10"/>
     </row>
-    <row r="132" spans="1:17" hidden="1">
+    <row r="132" spans="1:17">
       <c r="A132" s="4"/>
       <c r="B132" s="11" t="s">
         <v>26</v>
@@ -8302,7 +8302,7 @@
       <c r="P132" s="14"/>
       <c r="Q132" s="10"/>
     </row>
-    <row r="133" spans="1:17" hidden="1">
+    <row r="133" spans="1:17">
       <c r="A133" s="4"/>
       <c r="B133" s="11" t="s">
         <v>26</v>
@@ -8341,7 +8341,7 @@
       <c r="P133" s="14"/>
       <c r="Q133" s="10"/>
     </row>
-    <row r="134" spans="1:17" hidden="1">
+    <row r="134" spans="1:17">
       <c r="A134" s="4"/>
       <c r="B134" s="11" t="s">
         <v>26</v>
@@ -8380,7 +8380,7 @@
       <c r="P134" s="14"/>
       <c r="Q134" s="10"/>
     </row>
-    <row r="135" spans="1:17" hidden="1">
+    <row r="135" spans="1:17">
       <c r="A135" s="4"/>
       <c r="B135" s="11" t="s">
         <v>26</v>
@@ -8419,7 +8419,7 @@
       <c r="P135" s="14"/>
       <c r="Q135" s="10"/>
     </row>
-    <row r="136" spans="1:17" hidden="1">
+    <row r="136" spans="1:17">
       <c r="A136" s="4"/>
       <c r="B136" s="11" t="s">
         <v>26</v>
@@ -8458,7 +8458,7 @@
       <c r="P136" s="14"/>
       <c r="Q136" s="10"/>
     </row>
-    <row r="137" spans="1:17" hidden="1">
+    <row r="137" spans="1:17">
       <c r="A137" s="4"/>
       <c r="B137" s="11" t="s">
         <v>26</v>
@@ -8497,7 +8497,7 @@
       <c r="P137" s="14"/>
       <c r="Q137" s="10"/>
     </row>
-    <row r="138" spans="1:17" hidden="1">
+    <row r="138" spans="1:17">
       <c r="A138" s="4"/>
       <c r="B138" s="11" t="s">
         <v>26</v>
@@ -8536,7 +8536,7 @@
       <c r="P138" s="14"/>
       <c r="Q138" s="10"/>
     </row>
-    <row r="139" spans="1:17" hidden="1">
+    <row r="139" spans="1:17">
       <c r="A139" s="4"/>
       <c r="B139" s="11" t="s">
         <v>26</v>
@@ -8575,7 +8575,7 @@
       <c r="P139" s="14"/>
       <c r="Q139" s="10"/>
     </row>
-    <row r="140" spans="1:17" hidden="1">
+    <row r="140" spans="1:17">
       <c r="A140" s="4"/>
       <c r="B140" s="11" t="s">
         <v>26</v>
@@ -8612,7 +8612,7 @@
       <c r="P140" s="14"/>
       <c r="Q140" s="10"/>
     </row>
-    <row r="141" spans="1:17" hidden="1">
+    <row r="141" spans="1:17">
       <c r="A141" s="4"/>
       <c r="B141" s="11" t="s">
         <v>26</v>
@@ -8649,7 +8649,7 @@
       <c r="P141" s="14"/>
       <c r="Q141" s="10"/>
     </row>
-    <row r="142" spans="1:17" hidden="1">
+    <row r="142" spans="1:17">
       <c r="A142" s="4"/>
       <c r="B142" s="11" t="s">
         <v>26</v>
@@ -8686,7 +8686,7 @@
       <c r="P142" s="14"/>
       <c r="Q142" s="10"/>
     </row>
-    <row r="143" spans="1:17" hidden="1">
+    <row r="143" spans="1:17">
       <c r="A143" s="4"/>
       <c r="B143" s="11" t="s">
         <v>26</v>
@@ -8723,7 +8723,7 @@
       <c r="P143" s="14"/>
       <c r="Q143" s="10"/>
     </row>
-    <row r="144" spans="1:17" hidden="1">
+    <row r="144" spans="1:17">
       <c r="A144" s="4"/>
       <c r="B144" s="11" t="s">
         <v>26</v>
@@ -8760,7 +8760,7 @@
       <c r="P144" s="14"/>
       <c r="Q144" s="10"/>
     </row>
-    <row r="145" spans="1:17" hidden="1">
+    <row r="145" spans="1:17">
       <c r="A145" s="4"/>
       <c r="B145" s="11" t="s">
         <v>26</v>
@@ -8797,7 +8797,7 @@
       <c r="P145" s="14"/>
       <c r="Q145" s="10"/>
     </row>
-    <row r="146" spans="1:17" hidden="1">
+    <row r="146" spans="1:17">
       <c r="A146" s="4"/>
       <c r="B146" s="11" t="s">
         <v>26</v>
@@ -8834,7 +8834,7 @@
       <c r="P146" s="14"/>
       <c r="Q146" s="10"/>
     </row>
-    <row r="147" spans="1:17" hidden="1">
+    <row r="147" spans="1:17">
       <c r="A147" s="4"/>
       <c r="B147" s="11" t="s">
         <v>26</v>
@@ -8871,7 +8871,7 @@
       <c r="P147" s="14"/>
       <c r="Q147" s="10"/>
     </row>
-    <row r="148" spans="1:17" hidden="1">
+    <row r="148" spans="1:17">
       <c r="A148" s="4"/>
       <c r="B148" s="11" t="s">
         <v>26</v>
@@ -8908,7 +8908,7 @@
       <c r="P148" s="14"/>
       <c r="Q148" s="10"/>
     </row>
-    <row r="149" spans="1:17" hidden="1">
+    <row r="149" spans="1:17">
       <c r="A149" s="4"/>
       <c r="B149" s="11" t="s">
         <v>26</v>
@@ -8945,7 +8945,7 @@
       <c r="P149" s="14"/>
       <c r="Q149" s="10"/>
     </row>
-    <row r="150" spans="1:17" hidden="1">
+    <row r="150" spans="1:17">
       <c r="A150" s="4"/>
       <c r="B150" s="11" t="s">
         <v>26</v>
@@ -8982,7 +8982,7 @@
       <c r="P150" s="14"/>
       <c r="Q150" s="10"/>
     </row>
-    <row r="151" spans="1:17" hidden="1">
+    <row r="151" spans="1:17">
       <c r="A151" s="4"/>
       <c r="B151" s="11" t="s">
         <v>26</v>
@@ -9019,7 +9019,7 @@
       <c r="P151" s="14"/>
       <c r="Q151" s="10"/>
     </row>
-    <row r="152" spans="1:17" hidden="1">
+    <row r="152" spans="1:17">
       <c r="A152" s="4"/>
       <c r="B152" s="11" t="s">
         <v>26</v>
@@ -9056,7 +9056,7 @@
       <c r="P152" s="14"/>
       <c r="Q152" s="10"/>
     </row>
-    <row r="153" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="153" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A153" s="4"/>
       <c r="B153" s="11" t="s">
         <v>26</v>
@@ -9093,7 +9093,7 @@
       <c r="P153" s="14"/>
       <c r="Q153" s="10"/>
     </row>
-    <row r="154" spans="1:17" ht="26.4" hidden="1">
+    <row r="154" spans="1:17" ht="26.4">
       <c r="A154" s="4"/>
       <c r="B154" s="11" t="s">
         <v>32</v>
@@ -9128,7 +9128,7 @@
       <c r="P154" s="14"/>
       <c r="Q154" s="10"/>
     </row>
-    <row r="155" spans="1:17" ht="26.4" hidden="1">
+    <row r="155" spans="1:17" ht="26.4">
       <c r="A155" s="4"/>
       <c r="B155" s="11" t="s">
         <v>32</v>
@@ -9161,7 +9161,7 @@
       <c r="P155" s="14"/>
       <c r="Q155" s="10"/>
     </row>
-    <row r="156" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="156" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A156" s="4"/>
       <c r="B156" s="11" t="s">
         <v>32</v>
@@ -9196,7 +9196,7 @@
       <c r="P156" s="14"/>
       <c r="Q156" s="10"/>
     </row>
-    <row r="157" spans="1:17" hidden="1">
+    <row r="157" spans="1:17">
       <c r="A157" s="4"/>
       <c r="B157" s="11" t="s">
         <v>32</v>
@@ -9233,7 +9233,7 @@
       <c r="P157" s="14"/>
       <c r="Q157" s="10"/>
     </row>
-    <row r="158" spans="1:17" hidden="1">
+    <row r="158" spans="1:17">
       <c r="A158" s="4"/>
       <c r="B158" s="11" t="s">
         <v>32</v>
@@ -9270,7 +9270,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="159" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A159" s="4"/>
       <c r="B159" s="11" t="s">
         <v>32</v>
@@ -9305,7 +9305,7 @@
       <c r="P159" s="14"/>
       <c r="Q159" s="10"/>
     </row>
-    <row r="160" spans="1:17" hidden="1">
+    <row r="160" spans="1:17">
       <c r="A160" s="4"/>
       <c r="B160" s="11" t="s">
         <v>32</v>
@@ -9340,7 +9340,7 @@
       <c r="P160" s="14"/>
       <c r="Q160" s="10"/>
     </row>
-    <row r="161" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="161" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A161" s="4"/>
       <c r="B161" s="11" t="s">
         <v>32</v>
@@ -9375,7 +9375,7 @@
       <c r="P161" s="14"/>
       <c r="Q161" s="10"/>
     </row>
-    <row r="162" spans="1:17" hidden="1">
+    <row r="162" spans="1:17">
       <c r="A162" s="4"/>
       <c r="B162" s="11" t="s">
         <v>32</v>
@@ -9410,7 +9410,7 @@
       <c r="P162" s="14"/>
       <c r="Q162" s="10"/>
     </row>
-    <row r="163" spans="1:17" hidden="1">
+    <row r="163" spans="1:17">
       <c r="A163" s="4"/>
       <c r="B163" s="11" t="s">
         <v>32</v>
@@ -9447,7 +9447,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="164" spans="1:17" hidden="1">
+    <row r="164" spans="1:17">
       <c r="A164" s="4"/>
       <c r="B164" s="11" t="s">
         <v>32</v>
@@ -9480,7 +9480,7 @@
       <c r="P164" s="14"/>
       <c r="Q164" s="10"/>
     </row>
-    <row r="165" spans="1:17" hidden="1">
+    <row r="165" spans="1:17">
       <c r="A165" s="4"/>
       <c r="B165" s="11" t="s">
         <v>32</v>
@@ -9513,7 +9513,7 @@
       <c r="P165" s="14"/>
       <c r="Q165" s="10"/>
     </row>
-    <row r="166" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="166" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A166" s="4"/>
       <c r="B166" s="11" t="s">
         <v>32</v>
@@ -9546,7 +9546,7 @@
       <c r="P166" s="14"/>
       <c r="Q166" s="10"/>
     </row>
-    <row r="167" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="167" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A167" s="4"/>
       <c r="B167" s="11" t="s">
         <v>32</v>
@@ -9579,7 +9579,7 @@
       <c r="P167" s="14"/>
       <c r="Q167" s="10"/>
     </row>
-    <row r="168" spans="1:17" hidden="1">
+    <row r="168" spans="1:17">
       <c r="A168" s="4"/>
       <c r="B168" s="11" t="s">
         <v>32</v>
@@ -9614,7 +9614,7 @@
       <c r="P168" s="14"/>
       <c r="Q168" s="10"/>
     </row>
-    <row r="169" spans="1:17" hidden="1">
+    <row r="169" spans="1:17">
       <c r="A169" s="4"/>
       <c r="B169" s="11" t="s">
         <v>32</v>
@@ -9647,7 +9647,7 @@
       <c r="P169" s="14"/>
       <c r="Q169" s="10"/>
     </row>
-    <row r="170" spans="1:17" ht="26.4" hidden="1">
+    <row r="170" spans="1:17" ht="26.4">
       <c r="A170" s="4"/>
       <c r="B170" s="11" t="s">
         <v>32</v>
@@ -9680,7 +9680,7 @@
       <c r="P170" s="14"/>
       <c r="Q170" s="10"/>
     </row>
-    <row r="171" spans="1:17" hidden="1">
+    <row r="171" spans="1:17">
       <c r="A171" s="4"/>
       <c r="B171" s="11" t="s">
         <v>32</v>
@@ -9717,7 +9717,7 @@
       <c r="P171" s="14"/>
       <c r="Q171" s="10"/>
     </row>
-    <row r="172" spans="1:17" hidden="1">
+    <row r="172" spans="1:17">
       <c r="A172" s="4"/>
       <c r="B172" s="11" t="s">
         <v>32</v>
@@ -9750,7 +9750,7 @@
       <c r="P172" s="14"/>
       <c r="Q172" s="10"/>
     </row>
-    <row r="173" spans="1:17" hidden="1">
+    <row r="173" spans="1:17">
       <c r="A173" s="4"/>
       <c r="B173" s="11" t="s">
         <v>32</v>
@@ -9783,7 +9783,7 @@
       <c r="P173" s="46"/>
       <c r="Q173" s="10"/>
     </row>
-    <row r="174" spans="1:17" ht="26.4" hidden="1">
+    <row r="174" spans="1:17" ht="26.4">
       <c r="A174" s="4"/>
       <c r="B174" s="11">
         <v>72</v>
@@ -9832,7 +9832,7 @@
       </c>
       <c r="Q174" s="10"/>
     </row>
-    <row r="175" spans="1:17" hidden="1">
+    <row r="175" spans="1:17">
       <c r="A175" s="4"/>
       <c r="B175" s="11">
         <v>72</v>
@@ -9881,7 +9881,7 @@
       </c>
       <c r="Q175" s="10"/>
     </row>
-    <row r="176" spans="1:17" hidden="1">
+    <row r="176" spans="1:17">
       <c r="A176" s="4"/>
       <c r="B176" s="5" t="s">
         <v>353</v>
@@ -9914,7 +9914,7 @@
       <c r="P176" s="9"/>
       <c r="Q176" s="10"/>
     </row>
-    <row r="177" spans="1:17" hidden="1">
+    <row r="177" spans="1:17">
       <c r="A177" s="4"/>
       <c r="B177" s="5" t="s">
         <v>353</v>
@@ -9947,7 +9947,7 @@
       <c r="P177" s="9"/>
       <c r="Q177" s="10"/>
     </row>
-    <row r="178" spans="1:17" hidden="1">
+    <row r="178" spans="1:17">
       <c r="A178" s="4"/>
       <c r="B178" s="5" t="s">
         <v>353</v>
@@ -9980,7 +9980,7 @@
       <c r="P178" s="9"/>
       <c r="Q178" s="10"/>
     </row>
-    <row r="179" spans="1:17" hidden="1">
+    <row r="179" spans="1:17">
       <c r="A179" s="4"/>
       <c r="B179" s="5" t="s">
         <v>353</v>
@@ -10019,7 +10019,7 @@
       </c>
       <c r="Q179" s="10"/>
     </row>
-    <row r="180" spans="1:17" hidden="1">
+    <row r="180" spans="1:17">
       <c r="A180" s="4"/>
       <c r="B180" s="5" t="s">
         <v>353</v>
@@ -10058,7 +10058,7 @@
       </c>
       <c r="Q180" s="10"/>
     </row>
-    <row r="181" spans="1:17" hidden="1">
+    <row r="181" spans="1:17">
       <c r="A181" s="4"/>
       <c r="B181" s="5" t="s">
         <v>353</v>
@@ -10097,7 +10097,7 @@
       </c>
       <c r="Q181" s="10"/>
     </row>
-    <row r="182" spans="1:17" hidden="1">
+    <row r="182" spans="1:17">
       <c r="A182" s="4"/>
       <c r="B182" s="5" t="s">
         <v>353</v>
@@ -10134,7 +10134,7 @@
       <c r="P182" s="9"/>
       <c r="Q182" s="10"/>
     </row>
-    <row r="183" spans="1:17" hidden="1">
+    <row r="183" spans="1:17">
       <c r="A183" s="4"/>
       <c r="B183" s="5" t="s">
         <v>353</v>
@@ -10169,7 +10169,7 @@
       <c r="P183" s="9"/>
       <c r="Q183" s="10"/>
     </row>
-    <row r="184" spans="1:17" hidden="1">
+    <row r="184" spans="1:17">
       <c r="A184" s="4"/>
       <c r="B184" s="5" t="s">
         <v>353</v>
@@ -10212,7 +10212,7 @@
       </c>
       <c r="Q184" s="10"/>
     </row>
-    <row r="185" spans="1:17" hidden="1">
+    <row r="185" spans="1:17">
       <c r="A185" s="4"/>
       <c r="B185" s="5" t="s">
         <v>353</v>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="Q185" s="10"/>
     </row>
-    <row r="186" spans="1:17" hidden="1">
+    <row r="186" spans="1:17">
       <c r="A186" s="4"/>
       <c r="B186" s="5" t="s">
         <v>353</v>
@@ -10294,7 +10294,7 @@
       <c r="P186" s="9"/>
       <c r="Q186" s="10"/>
     </row>
-    <row r="187" spans="1:17" hidden="1">
+    <row r="187" spans="1:17">
       <c r="A187" s="4"/>
       <c r="B187" s="5" t="s">
         <v>353</v>
@@ -10333,7 +10333,7 @@
       <c r="P187" s="9"/>
       <c r="Q187" s="10"/>
     </row>
-    <row r="188" spans="1:17" hidden="1">
+    <row r="188" spans="1:17">
       <c r="A188" s="4"/>
       <c r="B188" s="5" t="s">
         <v>353</v>
@@ -10370,7 +10370,7 @@
       <c r="P188" s="9"/>
       <c r="Q188" s="10"/>
     </row>
-    <row r="189" spans="1:17" hidden="1">
+    <row r="189" spans="1:17">
       <c r="A189" s="4"/>
       <c r="B189" s="5" t="s">
         <v>353</v>
@@ -10407,7 +10407,7 @@
       <c r="P189" s="9"/>
       <c r="Q189" s="10"/>
     </row>
-    <row r="190" spans="1:17" hidden="1">
+    <row r="190" spans="1:17">
       <c r="A190" s="4"/>
       <c r="B190" s="5" t="s">
         <v>390</v>
@@ -10440,7 +10440,7 @@
       <c r="P190" s="9"/>
       <c r="Q190" s="10"/>
     </row>
-    <row r="191" spans="1:17" hidden="1">
+    <row r="191" spans="1:17">
       <c r="A191" s="4"/>
       <c r="B191" s="5" t="s">
         <v>390</v>
@@ -10473,7 +10473,7 @@
       <c r="P191" s="9"/>
       <c r="Q191" s="10"/>
     </row>
-    <row r="192" spans="1:17" hidden="1">
+    <row r="192" spans="1:17">
       <c r="A192" s="4"/>
       <c r="B192" s="5" t="s">
         <v>390</v>
@@ -10506,7 +10506,7 @@
       <c r="P192" s="9"/>
       <c r="Q192" s="10"/>
     </row>
-    <row r="193" spans="1:17" hidden="1">
+    <row r="193" spans="1:17">
       <c r="A193" s="4"/>
       <c r="B193" s="5" t="s">
         <v>390</v>
@@ -10539,7 +10539,7 @@
       <c r="P193" s="9"/>
       <c r="Q193" s="10"/>
     </row>
-    <row r="194" spans="1:17" hidden="1">
+    <row r="194" spans="1:17">
       <c r="A194" s="4"/>
       <c r="B194" s="5" t="s">
         <v>390</v>
@@ -10572,7 +10572,7 @@
       <c r="P194" s="9"/>
       <c r="Q194" s="10"/>
     </row>
-    <row r="195" spans="1:17" hidden="1">
+    <row r="195" spans="1:17">
       <c r="A195" s="4"/>
       <c r="B195" s="5" t="s">
         <v>390</v>
@@ -10611,7 +10611,7 @@
       </c>
       <c r="Q195" s="10"/>
     </row>
-    <row r="196" spans="1:17" hidden="1">
+    <row r="196" spans="1:17">
       <c r="A196" s="4"/>
       <c r="B196" s="5" t="s">
         <v>390</v>
@@ -10650,7 +10650,7 @@
       </c>
       <c r="Q196" s="10"/>
     </row>
-    <row r="197" spans="1:17" hidden="1">
+    <row r="197" spans="1:17">
       <c r="A197" s="4"/>
       <c r="B197" s="5" t="s">
         <v>390</v>
@@ -10689,7 +10689,7 @@
       </c>
       <c r="Q197" s="10"/>
     </row>
-    <row r="198" spans="1:17" hidden="1">
+    <row r="198" spans="1:17">
       <c r="A198" s="4"/>
       <c r="B198" s="5" t="s">
         <v>390</v>
@@ -10728,7 +10728,7 @@
       </c>
       <c r="Q198" s="10"/>
     </row>
-    <row r="199" spans="1:17" hidden="1">
+    <row r="199" spans="1:17">
       <c r="A199" s="4"/>
       <c r="B199" s="5" t="s">
         <v>390</v>
@@ -10765,7 +10765,7 @@
       <c r="P199" s="9"/>
       <c r="Q199" s="10"/>
     </row>
-    <row r="200" spans="1:17" hidden="1">
+    <row r="200" spans="1:17">
       <c r="A200" s="4"/>
       <c r="B200" s="5" t="s">
         <v>390</v>
@@ -10802,7 +10802,7 @@
       <c r="P200" s="64"/>
       <c r="Q200" s="10"/>
     </row>
-    <row r="201" spans="1:17" hidden="1">
+    <row r="201" spans="1:17">
       <c r="A201" s="4"/>
       <c r="B201" s="65">
         <v>60</v>
@@ -10851,7 +10851,7 @@
       </c>
       <c r="Q201" s="10"/>
     </row>
-    <row r="202" spans="1:17" hidden="1">
+    <row r="202" spans="1:17">
       <c r="A202" s="4"/>
       <c r="B202" s="65">
         <v>60</v>
@@ -10900,7 +10900,7 @@
       </c>
       <c r="Q202" s="10"/>
     </row>
-    <row r="203" spans="1:17" hidden="1">
+    <row r="203" spans="1:17">
       <c r="A203" s="4"/>
       <c r="B203" s="65">
         <v>60</v>
@@ -10949,7 +10949,7 @@
       </c>
       <c r="Q203" s="10"/>
     </row>
-    <row r="204" spans="1:17" hidden="1">
+    <row r="204" spans="1:17">
       <c r="A204" s="4"/>
       <c r="B204" s="65">
         <v>60</v>
@@ -10998,7 +10998,7 @@
       </c>
       <c r="Q204" s="10"/>
     </row>
-    <row r="205" spans="1:17" hidden="1">
+    <row r="205" spans="1:17">
       <c r="A205" s="4"/>
       <c r="B205" s="65">
         <v>60</v>
@@ -11047,7 +11047,7 @@
       </c>
       <c r="Q205" s="10"/>
     </row>
-    <row r="206" spans="1:17" hidden="1">
+    <row r="206" spans="1:17">
       <c r="A206" s="4"/>
       <c r="B206" s="65">
         <v>60</v>
@@ -11096,7 +11096,7 @@
       </c>
       <c r="Q206" s="10"/>
     </row>
-    <row r="207" spans="1:17" hidden="1">
+    <row r="207" spans="1:17">
       <c r="A207" s="4"/>
       <c r="B207" s="65">
         <v>60</v>
@@ -11145,7 +11145,7 @@
       </c>
       <c r="Q207" s="10"/>
     </row>
-    <row r="208" spans="1:17" hidden="1">
+    <row r="208" spans="1:17">
       <c r="A208" s="4"/>
       <c r="B208" s="65">
         <v>60</v>
@@ -11194,7 +11194,7 @@
       </c>
       <c r="Q208" s="10"/>
     </row>
-    <row r="209" spans="1:17" hidden="1">
+    <row r="209" spans="1:17">
       <c r="A209" s="4"/>
       <c r="B209" s="65">
         <v>60</v>
@@ -11243,7 +11243,7 @@
       </c>
       <c r="Q209" s="10"/>
     </row>
-    <row r="210" spans="1:17" hidden="1">
+    <row r="210" spans="1:17">
       <c r="A210" s="4"/>
       <c r="B210" s="65">
         <v>60</v>
@@ -11292,7 +11292,7 @@
       </c>
       <c r="Q210" s="10"/>
     </row>
-    <row r="211" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="211" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A211" s="4"/>
       <c r="B211" s="70">
         <v>60</v>
@@ -11341,7 +11341,7 @@
       </c>
       <c r="Q211" s="10"/>
     </row>
-    <row r="212" spans="1:17" hidden="1">
+    <row r="212" spans="1:17">
       <c r="A212" s="4"/>
       <c r="B212" s="7" t="s">
         <v>425</v>
@@ -11378,7 +11378,7 @@
       <c r="P212" s="83"/>
       <c r="Q212" s="10"/>
     </row>
-    <row r="213" spans="1:17" hidden="1">
+    <row r="213" spans="1:17">
       <c r="A213" s="4"/>
       <c r="B213" s="65">
         <v>60</v>
@@ -11427,7 +11427,7 @@
       </c>
       <c r="Q213" s="10"/>
     </row>
-    <row r="214" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="214" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A214" s="4"/>
       <c r="B214" s="65">
         <v>60</v>
@@ -11476,7 +11476,7 @@
       </c>
       <c r="Q214" s="10"/>
     </row>
-    <row r="215" spans="1:17" hidden="1">
+    <row r="215" spans="1:17">
       <c r="A215" s="4"/>
       <c r="B215" s="65">
         <v>60</v>
@@ -11525,7 +11525,7 @@
       </c>
       <c r="Q215" s="10"/>
     </row>
-    <row r="216" spans="1:17" hidden="1">
+    <row r="216" spans="1:17">
       <c r="A216" s="4"/>
       <c r="B216" s="65">
         <v>60</v>
@@ -11574,7 +11574,7 @@
       </c>
       <c r="Q216" s="10"/>
     </row>
-    <row r="217" spans="1:17" hidden="1">
+    <row r="217" spans="1:17">
       <c r="A217" s="4"/>
       <c r="B217" s="65">
         <v>60</v>
@@ -11623,7 +11623,7 @@
       </c>
       <c r="Q217" s="10"/>
     </row>
-    <row r="218" spans="1:17" hidden="1">
+    <row r="218" spans="1:17">
       <c r="A218" s="4"/>
       <c r="B218" s="65">
         <v>60</v>
@@ -11672,7 +11672,7 @@
       </c>
       <c r="Q218" s="10"/>
     </row>
-    <row r="219" spans="1:17" hidden="1">
+    <row r="219" spans="1:17">
       <c r="A219" s="4"/>
       <c r="B219" s="65">
         <v>60</v>
@@ -11721,7 +11721,7 @@
       </c>
       <c r="Q219" s="10"/>
     </row>
-    <row r="220" spans="1:17" hidden="1">
+    <row r="220" spans="1:17">
       <c r="A220" s="4"/>
       <c r="B220" s="65">
         <v>60</v>
@@ -11770,7 +11770,7 @@
       </c>
       <c r="Q220" s="10"/>
     </row>
-    <row r="221" spans="1:17" hidden="1">
+    <row r="221" spans="1:17">
       <c r="A221" s="4"/>
       <c r="B221" s="65">
         <v>60</v>
@@ -11819,7 +11819,7 @@
       </c>
       <c r="Q221" s="10"/>
     </row>
-    <row r="222" spans="1:17" hidden="1">
+    <row r="222" spans="1:17">
       <c r="A222" s="4"/>
       <c r="B222" s="65">
         <v>60</v>
@@ -11868,7 +11868,7 @@
       </c>
       <c r="Q222" s="10"/>
     </row>
-    <row r="223" spans="1:17" hidden="1">
+    <row r="223" spans="1:17">
       <c r="A223" s="4"/>
       <c r="B223" s="65">
         <v>60</v>
@@ -11917,7 +11917,7 @@
       </c>
       <c r="Q223" s="10"/>
     </row>
-    <row r="224" spans="1:17" hidden="1">
+    <row r="224" spans="1:17">
       <c r="A224" s="4"/>
       <c r="B224" s="65">
         <v>60</v>
@@ -11966,7 +11966,7 @@
       </c>
       <c r="Q224" s="10"/>
     </row>
-    <row r="225" spans="1:17" hidden="1">
+    <row r="225" spans="1:17">
       <c r="A225" s="4"/>
       <c r="B225" s="65">
         <v>60</v>
@@ -12015,7 +12015,7 @@
       </c>
       <c r="Q225" s="10"/>
     </row>
-    <row r="226" spans="1:17" hidden="1">
+    <row r="226" spans="1:17">
       <c r="A226" s="4"/>
       <c r="B226" s="65">
         <v>60</v>
@@ -12064,7 +12064,7 @@
       </c>
       <c r="Q226" s="10"/>
     </row>
-    <row r="227" spans="1:17" hidden="1">
+    <row r="227" spans="1:17">
       <c r="A227" s="4"/>
       <c r="B227" s="65">
         <v>60</v>
@@ -12113,7 +12113,7 @@
       </c>
       <c r="Q227" s="10"/>
     </row>
-    <row r="228" spans="1:17" hidden="1">
+    <row r="228" spans="1:17">
       <c r="A228" s="4"/>
       <c r="B228" s="65">
         <v>60</v>
@@ -12162,7 +12162,7 @@
       </c>
       <c r="Q228" s="10"/>
     </row>
-    <row r="229" spans="1:17" hidden="1">
+    <row r="229" spans="1:17">
       <c r="A229" s="4"/>
       <c r="B229" s="65">
         <v>60</v>
@@ -12211,7 +12211,7 @@
       </c>
       <c r="Q229" s="10"/>
     </row>
-    <row r="230" spans="1:17" hidden="1">
+    <row r="230" spans="1:17">
       <c r="A230" s="4"/>
       <c r="B230" s="65">
         <v>60</v>
@@ -12260,7 +12260,7 @@
       </c>
       <c r="Q230" s="10"/>
     </row>
-    <row r="231" spans="1:17" hidden="1">
+    <row r="231" spans="1:17">
       <c r="A231" s="4"/>
       <c r="B231" s="65">
         <v>60</v>
@@ -12309,7 +12309,7 @@
       </c>
       <c r="Q231" s="10"/>
     </row>
-    <row r="232" spans="1:17" hidden="1">
+    <row r="232" spans="1:17">
       <c r="A232" s="4"/>
       <c r="B232" s="68">
         <v>60</v>
@@ -12358,7 +12358,7 @@
       </c>
       <c r="Q232" s="10"/>
     </row>
-    <row r="233" spans="1:17" hidden="1">
+    <row r="233" spans="1:17">
       <c r="A233" s="4"/>
       <c r="B233" s="66">
         <v>654</v>
@@ -12407,7 +12407,7 @@
       </c>
       <c r="Q233" s="10"/>
     </row>
-    <row r="234" spans="1:17" hidden="1">
+    <row r="234" spans="1:17">
       <c r="A234" s="4"/>
       <c r="B234" s="66">
         <v>654</v>
@@ -12456,7 +12456,7 @@
       </c>
       <c r="Q234" s="10"/>
     </row>
-    <row r="235" spans="1:17" hidden="1">
+    <row r="235" spans="1:17">
       <c r="A235" s="4"/>
       <c r="B235" s="66">
         <v>654</v>
@@ -12505,7 +12505,7 @@
       </c>
       <c r="Q235" s="10"/>
     </row>
-    <row r="236" spans="1:17" hidden="1">
+    <row r="236" spans="1:17">
       <c r="A236" s="4"/>
       <c r="B236" s="66">
         <v>654</v>
@@ -12554,7 +12554,7 @@
       </c>
       <c r="Q236" s="10"/>
     </row>
-    <row r="237" spans="1:17" hidden="1">
+    <row r="237" spans="1:17">
       <c r="A237" s="4"/>
       <c r="B237" s="66">
         <v>654</v>
@@ -12603,7 +12603,7 @@
       </c>
       <c r="Q237" s="10"/>
     </row>
-    <row r="238" spans="1:17" hidden="1">
+    <row r="238" spans="1:17">
       <c r="A238" s="4"/>
       <c r="B238" s="66">
         <v>654</v>
@@ -12652,7 +12652,7 @@
       </c>
       <c r="Q238" s="10"/>
     </row>
-    <row r="239" spans="1:17" hidden="1">
+    <row r="239" spans="1:17">
       <c r="A239" s="4"/>
       <c r="B239" s="66">
         <v>654</v>
@@ -12701,7 +12701,7 @@
       </c>
       <c r="Q239" s="10"/>
     </row>
-    <row r="240" spans="1:17" hidden="1">
+    <row r="240" spans="1:17">
       <c r="A240" s="4"/>
       <c r="B240" s="66">
         <v>654</v>
@@ -12750,7 +12750,7 @@
       </c>
       <c r="Q240" s="10"/>
     </row>
-    <row r="241" spans="1:17" hidden="1">
+    <row r="241" spans="1:17">
       <c r="A241" s="4"/>
       <c r="B241" s="66">
         <v>654</v>
@@ -12797,7 +12797,7 @@
       </c>
       <c r="Q241" s="10"/>
     </row>
-    <row r="242" spans="1:17" hidden="1">
+    <row r="242" spans="1:17">
       <c r="A242" s="4"/>
       <c r="B242" s="66">
         <v>654</v>
@@ -12846,7 +12846,7 @@
       </c>
       <c r="Q242" s="10"/>
     </row>
-    <row r="243" spans="1:17" hidden="1">
+    <row r="243" spans="1:17">
       <c r="A243" s="4"/>
       <c r="B243" s="66">
         <v>654</v>
@@ -12895,7 +12895,7 @@
       </c>
       <c r="Q243" s="10"/>
     </row>
-    <row r="244" spans="1:17" hidden="1">
+    <row r="244" spans="1:17">
       <c r="A244" s="4"/>
       <c r="B244" s="66">
         <v>654</v>
@@ -12944,7 +12944,7 @@
       </c>
       <c r="Q244" s="10"/>
     </row>
-    <row r="245" spans="1:17" hidden="1">
+    <row r="245" spans="1:17">
       <c r="A245" s="4"/>
       <c r="B245" s="66">
         <v>654</v>
@@ -12993,7 +12993,7 @@
       </c>
       <c r="Q245" s="10"/>
     </row>
-    <row r="246" spans="1:17" hidden="1">
+    <row r="246" spans="1:17">
       <c r="A246" s="4"/>
       <c r="B246" s="66">
         <v>654</v>
@@ -13042,7 +13042,7 @@
       </c>
       <c r="Q246" s="10"/>
     </row>
-    <row r="247" spans="1:17" hidden="1">
+    <row r="247" spans="1:17">
       <c r="A247" s="4"/>
       <c r="B247" s="66">
         <v>654</v>
@@ -13091,7 +13091,7 @@
       </c>
       <c r="Q247" s="10"/>
     </row>
-    <row r="248" spans="1:17" hidden="1">
+    <row r="248" spans="1:17">
       <c r="A248" s="4"/>
       <c r="B248" s="66">
         <v>654</v>
@@ -13140,7 +13140,7 @@
       </c>
       <c r="Q248" s="10"/>
     </row>
-    <row r="249" spans="1:17" hidden="1">
+    <row r="249" spans="1:17">
       <c r="A249" s="4"/>
       <c r="B249" s="70">
         <v>654</v>
@@ -13189,7 +13189,7 @@
       </c>
       <c r="Q249" s="10"/>
     </row>
-    <row r="250" spans="1:17" hidden="1">
+    <row r="250" spans="1:17">
       <c r="A250" s="4"/>
       <c r="B250" s="11" t="s">
         <v>490</v>
@@ -13224,7 +13224,7 @@
       <c r="P250" s="14"/>
       <c r="Q250" s="10"/>
     </row>
-    <row r="251" spans="1:17" hidden="1">
+    <row r="251" spans="1:17">
       <c r="A251" s="4"/>
       <c r="B251" s="11" t="s">
         <v>490</v>
@@ -13259,7 +13259,7 @@
       <c r="P251" s="14"/>
       <c r="Q251" s="10"/>
     </row>
-    <row r="252" spans="1:17" hidden="1">
+    <row r="252" spans="1:17">
       <c r="A252" s="4"/>
       <c r="B252" s="11" t="s">
         <v>490</v>
@@ -13296,7 +13296,7 @@
       <c r="P252" s="14"/>
       <c r="Q252" s="10"/>
     </row>
-    <row r="253" spans="1:17" hidden="1">
+    <row r="253" spans="1:17">
       <c r="A253" s="4"/>
       <c r="B253" s="11" t="s">
         <v>490</v>
@@ -13337,7 +13337,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="254" spans="1:17" hidden="1">
+    <row r="254" spans="1:17">
       <c r="A254" s="4"/>
       <c r="B254" s="11" t="s">
         <v>490</v>
@@ -13376,7 +13376,7 @@
       <c r="P254" s="14"/>
       <c r="Q254" s="10"/>
     </row>
-    <row r="255" spans="1:17" hidden="1">
+    <row r="255" spans="1:17">
       <c r="A255" s="4"/>
       <c r="B255" s="11" t="s">
         <v>490</v>
@@ -13415,7 +13415,7 @@
       <c r="P255" s="14"/>
       <c r="Q255" s="10"/>
     </row>
-    <row r="256" spans="1:17" hidden="1">
+    <row r="256" spans="1:17">
       <c r="A256" s="4"/>
       <c r="B256" s="11" t="s">
         <v>490</v>
@@ -13454,7 +13454,7 @@
       <c r="P256" s="14"/>
       <c r="Q256" s="10"/>
     </row>
-    <row r="257" spans="1:17" hidden="1">
+    <row r="257" spans="1:17">
       <c r="A257" s="4"/>
       <c r="B257" s="5" t="s">
         <v>490</v>
@@ -13493,7 +13493,7 @@
       <c r="P257" s="9"/>
       <c r="Q257" s="10"/>
     </row>
-    <row r="258" spans="1:17" hidden="1">
+    <row r="258" spans="1:17">
       <c r="A258" s="4"/>
       <c r="B258" s="11" t="s">
         <v>490</v>
@@ -13530,7 +13530,7 @@
       <c r="P258" s="14"/>
       <c r="Q258" s="10"/>
     </row>
-    <row r="259" spans="1:17" hidden="1">
+    <row r="259" spans="1:17">
       <c r="A259" s="4"/>
       <c r="B259" s="11" t="s">
         <v>490</v>
@@ -13567,7 +13567,7 @@
       <c r="P259" s="14"/>
       <c r="Q259" s="10"/>
     </row>
-    <row r="260" spans="1:17" hidden="1">
+    <row r="260" spans="1:17">
       <c r="A260" s="4"/>
       <c r="B260" s="11" t="s">
         <v>490</v>
@@ -13602,7 +13602,7 @@
       <c r="P260" s="14"/>
       <c r="Q260" s="10"/>
     </row>
-    <row r="261" spans="1:17" hidden="1">
+    <row r="261" spans="1:17">
       <c r="A261" s="4"/>
       <c r="B261" s="11" t="s">
         <v>490</v>
@@ -13637,7 +13637,7 @@
       <c r="P261" s="14"/>
       <c r="Q261" s="10"/>
     </row>
-    <row r="262" spans="1:17" hidden="1">
+    <row r="262" spans="1:17">
       <c r="A262" s="4"/>
       <c r="B262" s="5" t="s">
         <v>490</v>
@@ -13674,7 +13674,7 @@
       <c r="P262" s="9"/>
       <c r="Q262" s="10"/>
     </row>
-    <row r="263" spans="1:17" hidden="1">
+    <row r="263" spans="1:17">
       <c r="A263" s="4"/>
       <c r="B263" s="5" t="s">
         <v>490</v>
@@ -13709,7 +13709,7 @@
       <c r="P263" s="9"/>
       <c r="Q263" s="10"/>
     </row>
-    <row r="264" spans="1:17" hidden="1">
+    <row r="264" spans="1:17">
       <c r="A264" s="4"/>
       <c r="B264" s="5" t="s">
         <v>490</v>
@@ -13744,7 +13744,7 @@
       <c r="P264" s="9"/>
       <c r="Q264" s="10"/>
     </row>
-    <row r="265" spans="1:17" hidden="1">
+    <row r="265" spans="1:17">
       <c r="A265" s="4"/>
       <c r="B265" s="11" t="s">
         <v>490</v>
@@ -13781,7 +13781,7 @@
       <c r="P265" s="14"/>
       <c r="Q265" s="10"/>
     </row>
-    <row r="266" spans="1:17" hidden="1">
+    <row r="266" spans="1:17">
       <c r="A266" s="4"/>
       <c r="B266" s="11" t="s">
         <v>490</v>
@@ -13816,7 +13816,7 @@
       <c r="P266" s="14"/>
       <c r="Q266" s="10"/>
     </row>
-    <row r="267" spans="1:17" hidden="1">
+    <row r="267" spans="1:17">
       <c r="A267" s="4"/>
       <c r="B267" s="11" t="s">
         <v>490</v>
@@ -13851,7 +13851,7 @@
       <c r="P267" s="14"/>
       <c r="Q267" s="10"/>
     </row>
-    <row r="268" spans="1:17" hidden="1">
+    <row r="268" spans="1:17">
       <c r="A268" s="4"/>
       <c r="B268" s="11" t="s">
         <v>490</v>
@@ -13888,7 +13888,7 @@
       <c r="P268" s="14"/>
       <c r="Q268" s="10"/>
     </row>
-    <row r="269" spans="1:17" hidden="1">
+    <row r="269" spans="1:17">
       <c r="A269" s="4"/>
       <c r="B269" s="11" t="s">
         <v>490</v>
@@ -13923,7 +13923,7 @@
       <c r="P269" s="14"/>
       <c r="Q269" s="10"/>
     </row>
-    <row r="270" spans="1:17" hidden="1">
+    <row r="270" spans="1:17">
       <c r="A270" s="4"/>
       <c r="B270" s="11" t="s">
         <v>490</v>
@@ -13958,7 +13958,7 @@
       <c r="P270" s="14"/>
       <c r="Q270" s="10"/>
     </row>
-    <row r="271" spans="1:17" hidden="1">
+    <row r="271" spans="1:17">
       <c r="A271" s="4"/>
       <c r="B271" s="11" t="s">
         <v>490</v>
@@ -13993,7 +13993,7 @@
       <c r="P271" s="14"/>
       <c r="Q271" s="10"/>
     </row>
-    <row r="272" spans="1:17" hidden="1">
+    <row r="272" spans="1:17">
       <c r="A272" s="4"/>
       <c r="B272" s="11" t="s">
         <v>490</v>
@@ -14028,7 +14028,7 @@
       <c r="P272" s="14"/>
       <c r="Q272" s="10"/>
     </row>
-    <row r="273" spans="1:17" hidden="1">
+    <row r="273" spans="1:17">
       <c r="A273" s="4"/>
       <c r="B273" s="11" t="s">
         <v>490</v>
@@ -14067,7 +14067,7 @@
       <c r="P273" s="14"/>
       <c r="Q273" s="10"/>
     </row>
-    <row r="274" spans="1:17" hidden="1">
+    <row r="274" spans="1:17">
       <c r="A274" s="4"/>
       <c r="B274" s="11" t="s">
         <v>490</v>
@@ -14106,7 +14106,7 @@
       <c r="P274" s="14"/>
       <c r="Q274" s="10"/>
     </row>
-    <row r="275" spans="1:17" hidden="1">
+    <row r="275" spans="1:17">
       <c r="A275" s="4"/>
       <c r="B275" s="11" t="s">
         <v>490</v>
@@ -14143,7 +14143,7 @@
       <c r="P275" s="14"/>
       <c r="Q275" s="10"/>
     </row>
-    <row r="276" spans="1:17" hidden="1">
+    <row r="276" spans="1:17">
       <c r="A276" s="4"/>
       <c r="B276" s="11" t="s">
         <v>490</v>
@@ -14180,7 +14180,7 @@
       <c r="P276" s="14"/>
       <c r="Q276" s="10"/>
     </row>
-    <row r="277" spans="1:17" hidden="1">
+    <row r="277" spans="1:17">
       <c r="A277" s="4"/>
       <c r="B277" s="11" t="s">
         <v>490</v>
@@ -14213,7 +14213,7 @@
       <c r="P277" s="14"/>
       <c r="Q277" s="10"/>
     </row>
-    <row r="278" spans="1:17" hidden="1">
+    <row r="278" spans="1:17">
       <c r="A278" s="4"/>
       <c r="B278" s="11" t="s">
         <v>490</v>
@@ -14246,7 +14246,7 @@
       <c r="P278" s="14"/>
       <c r="Q278" s="10"/>
     </row>
-    <row r="279" spans="1:17" hidden="1">
+    <row r="279" spans="1:17">
       <c r="A279" s="4"/>
       <c r="B279" s="11" t="s">
         <v>490</v>
@@ -14279,7 +14279,7 @@
       <c r="P279" s="14"/>
       <c r="Q279" s="10"/>
     </row>
-    <row r="280" spans="1:17" hidden="1">
+    <row r="280" spans="1:17">
       <c r="A280" s="4"/>
       <c r="B280" s="11" t="s">
         <v>490</v>
@@ -14314,7 +14314,7 @@
       <c r="P280" s="14"/>
       <c r="Q280" s="10"/>
     </row>
-    <row r="281" spans="1:17" hidden="1">
+    <row r="281" spans="1:17">
       <c r="A281" s="4"/>
       <c r="B281" s="11" t="s">
         <v>490</v>
@@ -14347,7 +14347,7 @@
       <c r="P281" s="14"/>
       <c r="Q281" s="10"/>
     </row>
-    <row r="282" spans="1:17" hidden="1">
+    <row r="282" spans="1:17">
       <c r="A282" s="4"/>
       <c r="B282" s="11" t="s">
         <v>490</v>
@@ -14382,7 +14382,7 @@
       <c r="P282" s="14"/>
       <c r="Q282" s="10"/>
     </row>
-    <row r="283" spans="1:17" hidden="1">
+    <row r="283" spans="1:17">
       <c r="A283" s="4"/>
       <c r="B283" s="11" t="s">
         <v>490</v>
@@ -14417,7 +14417,7 @@
       <c r="P283" s="14"/>
       <c r="Q283" s="10"/>
     </row>
-    <row r="284" spans="1:17" hidden="1">
+    <row r="284" spans="1:17">
       <c r="A284" s="4"/>
       <c r="B284" s="11" t="s">
         <v>490</v>
@@ -14452,7 +14452,7 @@
       <c r="P284" s="14"/>
       <c r="Q284" s="10"/>
     </row>
-    <row r="285" spans="1:17" hidden="1">
+    <row r="285" spans="1:17">
       <c r="A285" s="4"/>
       <c r="B285" s="11" t="s">
         <v>490</v>
@@ -14487,7 +14487,7 @@
       <c r="P285" s="14"/>
       <c r="Q285" s="10"/>
     </row>
-    <row r="286" spans="1:17" hidden="1">
+    <row r="286" spans="1:17">
       <c r="A286" s="4"/>
       <c r="B286" s="11" t="s">
         <v>490</v>
@@ -14520,7 +14520,7 @@
       <c r="P286" s="14"/>
       <c r="Q286" s="10"/>
     </row>
-    <row r="287" spans="1:17" hidden="1">
+    <row r="287" spans="1:17">
       <c r="A287" s="4"/>
       <c r="B287" s="11" t="s">
         <v>490</v>
@@ -14555,7 +14555,7 @@
       <c r="P287" s="14"/>
       <c r="Q287" s="10"/>
     </row>
-    <row r="288" spans="1:17" hidden="1">
+    <row r="288" spans="1:17">
       <c r="A288" s="4"/>
       <c r="B288" s="11" t="s">
         <v>490</v>
@@ -14590,7 +14590,7 @@
       <c r="P288" s="14"/>
       <c r="Q288" s="10"/>
     </row>
-    <row r="289" spans="1:17" hidden="1">
+    <row r="289" spans="1:17">
       <c r="A289" s="4"/>
       <c r="B289" s="11" t="s">
         <v>490</v>
@@ -14625,7 +14625,7 @@
       <c r="P289" s="14"/>
       <c r="Q289" s="10"/>
     </row>
-    <row r="290" spans="1:17" hidden="1">
+    <row r="290" spans="1:17">
       <c r="A290" s="4"/>
       <c r="B290" s="11" t="s">
         <v>490</v>
@@ -14660,7 +14660,7 @@
       <c r="P290" s="14"/>
       <c r="Q290" s="10"/>
     </row>
-    <row r="291" spans="1:17" hidden="1">
+    <row r="291" spans="1:17">
       <c r="A291" s="4"/>
       <c r="B291" s="11" t="s">
         <v>490</v>
@@ -14695,7 +14695,7 @@
       <c r="P291" s="14"/>
       <c r="Q291" s="10"/>
     </row>
-    <row r="292" spans="1:17" hidden="1">
+    <row r="292" spans="1:17">
       <c r="A292" s="4"/>
       <c r="B292" s="11" t="s">
         <v>490</v>
@@ -14730,7 +14730,7 @@
       <c r="P292" s="14"/>
       <c r="Q292" s="10"/>
     </row>
-    <row r="293" spans="1:17" hidden="1">
+    <row r="293" spans="1:17">
       <c r="A293" s="4"/>
       <c r="B293" s="11" t="s">
         <v>490</v>
@@ -14765,7 +14765,7 @@
       <c r="P293" s="14"/>
       <c r="Q293" s="10"/>
     </row>
-    <row r="294" spans="1:17" hidden="1">
+    <row r="294" spans="1:17">
       <c r="A294" s="4"/>
       <c r="B294" s="11" t="s">
         <v>490</v>
@@ -14800,7 +14800,7 @@
       <c r="P294" s="14"/>
       <c r="Q294" s="10"/>
     </row>
-    <row r="295" spans="1:17" hidden="1">
+    <row r="295" spans="1:17">
       <c r="A295" s="4"/>
       <c r="B295" s="11" t="s">
         <v>490</v>
@@ -14835,7 +14835,7 @@
       <c r="P295" s="14"/>
       <c r="Q295" s="10"/>
     </row>
-    <row r="296" spans="1:17" hidden="1">
+    <row r="296" spans="1:17">
       <c r="A296" s="4"/>
       <c r="B296" s="11" t="s">
         <v>490</v>
@@ -14870,7 +14870,7 @@
       <c r="P296" s="14"/>
       <c r="Q296" s="10"/>
     </row>
-    <row r="297" spans="1:17" hidden="1">
+    <row r="297" spans="1:17">
       <c r="A297" s="4"/>
       <c r="B297" s="11" t="s">
         <v>490</v>
@@ -14905,7 +14905,7 @@
       <c r="P297" s="14"/>
       <c r="Q297" s="10"/>
     </row>
-    <row r="298" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="298" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A298" s="4"/>
       <c r="B298" s="11" t="s">
         <v>490</v>
@@ -14940,7 +14940,7 @@
       <c r="P298" s="14"/>
       <c r="Q298" s="10"/>
     </row>
-    <row r="299" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="299" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A299" s="4"/>
       <c r="B299" s="11" t="s">
         <v>539</v>
@@ -14975,7 +14975,7 @@
       <c r="P299" s="14"/>
       <c r="Q299" s="10"/>
     </row>
-    <row r="300" spans="1:17" hidden="1">
+    <row r="300" spans="1:17">
       <c r="A300" s="4"/>
       <c r="B300" s="11" t="s">
         <v>539</v>
@@ -15010,7 +15010,7 @@
       <c r="P300" s="14"/>
       <c r="Q300" s="10"/>
     </row>
-    <row r="301" spans="1:17" hidden="1">
+    <row r="301" spans="1:17">
       <c r="A301" s="4"/>
       <c r="B301" s="11" t="s">
         <v>545</v>
@@ -15047,7 +15047,7 @@
       <c r="P301" s="14"/>
       <c r="Q301" s="10"/>
     </row>
-    <row r="302" spans="1:17" hidden="1">
+    <row r="302" spans="1:17">
       <c r="A302" s="4"/>
       <c r="B302" s="11" t="s">
         <v>545</v>
@@ -15084,7 +15084,7 @@
       <c r="P302" s="14"/>
       <c r="Q302" s="10"/>
     </row>
-    <row r="303" spans="1:17" hidden="1">
+    <row r="303" spans="1:17">
       <c r="A303" s="4"/>
       <c r="B303" s="11" t="s">
         <v>545</v>
@@ -15121,7 +15121,7 @@
       <c r="P303" s="14"/>
       <c r="Q303" s="10"/>
     </row>
-    <row r="304" spans="1:17" hidden="1">
+    <row r="304" spans="1:17">
       <c r="A304" s="4"/>
       <c r="B304" s="11" t="s">
         <v>545</v>
@@ -15156,7 +15156,7 @@
       <c r="P304" s="14"/>
       <c r="Q304" s="10"/>
     </row>
-    <row r="305" spans="1:17" hidden="1">
+    <row r="305" spans="1:17">
       <c r="A305" s="4"/>
       <c r="B305" s="11" t="s">
         <v>545</v>
@@ -15191,7 +15191,7 @@
       <c r="P305" s="14"/>
       <c r="Q305" s="10"/>
     </row>
-    <row r="306" spans="1:17" hidden="1">
+    <row r="306" spans="1:17">
       <c r="A306" s="4"/>
       <c r="B306" s="11" t="s">
         <v>553</v>
@@ -15224,7 +15224,7 @@
       <c r="P306" s="14"/>
       <c r="Q306" s="10"/>
     </row>
-    <row r="307" spans="1:17" hidden="1">
+    <row r="307" spans="1:17">
       <c r="A307" s="4"/>
       <c r="B307" s="11" t="s">
         <v>553</v>
@@ -15259,7 +15259,7 @@
       <c r="P307" s="14"/>
       <c r="Q307" s="10"/>
     </row>
-    <row r="308" spans="1:17" hidden="1">
+    <row r="308" spans="1:17">
       <c r="A308" s="4"/>
       <c r="B308" s="11" t="s">
         <v>553</v>
@@ -15294,7 +15294,7 @@
       <c r="P308" s="14"/>
       <c r="Q308" s="10"/>
     </row>
-    <row r="309" spans="1:17" hidden="1">
+    <row r="309" spans="1:17">
       <c r="A309" s="4"/>
       <c r="B309" s="11" t="s">
         <v>553</v>
@@ -15329,7 +15329,7 @@
       <c r="P309" s="14"/>
       <c r="Q309" s="10"/>
     </row>
-    <row r="310" spans="1:17" hidden="1">
+    <row r="310" spans="1:17">
       <c r="A310" s="4"/>
       <c r="B310" s="11" t="s">
         <v>553</v>
@@ -15364,7 +15364,7 @@
       <c r="P310" s="14"/>
       <c r="Q310" s="10"/>
     </row>
-    <row r="311" spans="1:17" hidden="1">
+    <row r="311" spans="1:17">
       <c r="A311" s="4"/>
       <c r="B311" s="11" t="s">
         <v>553</v>
@@ -15401,7 +15401,7 @@
       <c r="P311" s="14"/>
       <c r="Q311" s="10"/>
     </row>
-    <row r="312" spans="1:17" hidden="1">
+    <row r="312" spans="1:17">
       <c r="A312" s="4"/>
       <c r="B312" s="11" t="s">
         <v>553</v>
@@ -15438,7 +15438,7 @@
       <c r="P312" s="14"/>
       <c r="Q312" s="10"/>
     </row>
-    <row r="313" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="313" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A313" s="4"/>
       <c r="B313" s="11" t="s">
         <v>553</v>
@@ -15475,7 +15475,7 @@
       <c r="P313" s="14"/>
       <c r="Q313" s="10"/>
     </row>
-    <row r="314" spans="1:17" hidden="1">
+    <row r="314" spans="1:17">
       <c r="A314" s="4"/>
       <c r="B314" s="11" t="s">
         <v>553</v>
@@ -15512,7 +15512,7 @@
       <c r="P314" s="14"/>
       <c r="Q314" s="10"/>
     </row>
-    <row r="315" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="315" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A315" s="4"/>
       <c r="B315" s="11" t="s">
         <v>553</v>
@@ -15549,7 +15549,7 @@
       <c r="P315" s="14"/>
       <c r="Q315" s="10"/>
     </row>
-    <row r="316" spans="1:17" hidden="1">
+    <row r="316" spans="1:17">
       <c r="A316" s="4"/>
       <c r="B316" s="11" t="s">
         <v>553</v>
@@ -15584,7 +15584,7 @@
       <c r="P316" s="14"/>
       <c r="Q316" s="10"/>
     </row>
-    <row r="317" spans="1:17" hidden="1">
+    <row r="317" spans="1:17">
       <c r="A317" s="4"/>
       <c r="B317" s="11" t="s">
         <v>553</v>
@@ -15619,7 +15619,7 @@
       <c r="P317" s="14"/>
       <c r="Q317" s="10"/>
     </row>
-    <row r="318" spans="1:17" hidden="1">
+    <row r="318" spans="1:17">
       <c r="A318" s="4"/>
       <c r="B318" s="11" t="s">
         <v>553</v>
@@ -15654,7 +15654,7 @@
       <c r="P318" s="14"/>
       <c r="Q318" s="10"/>
     </row>
-    <row r="319" spans="1:17" hidden="1">
+    <row r="319" spans="1:17">
       <c r="A319" s="4"/>
       <c r="B319" s="11" t="s">
         <v>553</v>
@@ -15689,7 +15689,7 @@
       <c r="P319" s="14"/>
       <c r="Q319" s="10"/>
     </row>
-    <row r="320" spans="1:17" hidden="1">
+    <row r="320" spans="1:17">
       <c r="A320" s="4"/>
       <c r="B320" s="11" t="s">
         <v>553</v>
@@ -15722,7 +15722,7 @@
       <c r="P320" s="14"/>
       <c r="Q320" s="10"/>
     </row>
-    <row r="321" spans="1:17" hidden="1">
+    <row r="321" spans="1:17">
       <c r="A321" s="4"/>
       <c r="B321" s="11" t="s">
         <v>553</v>
@@ -15755,7 +15755,7 @@
       <c r="P321" s="14"/>
       <c r="Q321" s="10"/>
     </row>
-    <row r="322" spans="1:17" hidden="1">
+    <row r="322" spans="1:17">
       <c r="A322" s="4"/>
       <c r="B322" s="11" t="s">
         <v>553</v>
@@ -15788,7 +15788,7 @@
       <c r="P322" s="14"/>
       <c r="Q322" s="10"/>
     </row>
-    <row r="323" spans="1:17" hidden="1">
+    <row r="323" spans="1:17">
       <c r="A323" s="4"/>
       <c r="B323" s="11" t="s">
         <v>553</v>
@@ -15823,7 +15823,7 @@
       <c r="P323" s="14"/>
       <c r="Q323" s="10"/>
     </row>
-    <row r="324" spans="1:17" hidden="1">
+    <row r="324" spans="1:17">
       <c r="A324" s="4"/>
       <c r="B324" s="11" t="s">
         <v>553</v>
@@ -15858,7 +15858,7 @@
       <c r="P324" s="14"/>
       <c r="Q324" s="10"/>
     </row>
-    <row r="325" spans="1:17" hidden="1">
+    <row r="325" spans="1:17">
       <c r="A325" s="4"/>
       <c r="B325" s="11" t="s">
         <v>553</v>
@@ -15893,7 +15893,7 @@
       <c r="P325" s="14"/>
       <c r="Q325" s="10"/>
     </row>
-    <row r="326" spans="1:17" hidden="1">
+    <row r="326" spans="1:17">
       <c r="A326" s="4"/>
       <c r="B326" s="11" t="s">
         <v>553</v>
@@ -15928,7 +15928,7 @@
       <c r="P326" s="14"/>
       <c r="Q326" s="10"/>
     </row>
-    <row r="327" spans="1:17" hidden="1">
+    <row r="327" spans="1:17">
       <c r="A327" s="4"/>
       <c r="B327" s="11" t="s">
         <v>553</v>
@@ -15963,7 +15963,7 @@
       <c r="P327" s="14"/>
       <c r="Q327" s="10"/>
     </row>
-    <row r="328" spans="1:17" hidden="1">
+    <row r="328" spans="1:17">
       <c r="A328" s="4"/>
       <c r="B328" s="11" t="s">
         <v>553</v>
@@ -15998,7 +15998,7 @@
       <c r="P328" s="14"/>
       <c r="Q328" s="10"/>
     </row>
-    <row r="329" spans="1:17" hidden="1">
+    <row r="329" spans="1:17">
       <c r="A329" s="4"/>
       <c r="B329" s="11" t="s">
         <v>553</v>
@@ -16033,7 +16033,7 @@
       <c r="P329" s="14"/>
       <c r="Q329" s="10"/>
     </row>
-    <row r="330" spans="1:17" hidden="1">
+    <row r="330" spans="1:17">
       <c r="A330" s="4"/>
       <c r="B330" s="11" t="s">
         <v>553</v>
@@ -16068,7 +16068,7 @@
       <c r="P330" s="14"/>
       <c r="Q330" s="10"/>
     </row>
-    <row r="331" spans="1:17" hidden="1">
+    <row r="331" spans="1:17">
       <c r="A331" s="4"/>
       <c r="B331" s="11" t="s">
         <v>597</v>
@@ -16101,7 +16101,7 @@
       <c r="P331" s="99"/>
       <c r="Q331" s="10"/>
     </row>
-    <row r="332" spans="1:17" hidden="1">
+    <row r="332" spans="1:17">
       <c r="A332" s="4"/>
       <c r="B332" s="11" t="s">
         <v>597</v>
@@ -16134,7 +16134,7 @@
       <c r="P332" s="103"/>
       <c r="Q332" s="10"/>
     </row>
-    <row r="333" spans="1:17" hidden="1">
+    <row r="333" spans="1:17">
       <c r="A333" s="4"/>
       <c r="B333" s="11" t="s">
         <v>597</v>
@@ -16167,7 +16167,7 @@
       <c r="P333" s="14"/>
       <c r="Q333" s="10"/>
     </row>
-    <row r="334" spans="1:17" hidden="1">
+    <row r="334" spans="1:17">
       <c r="A334" s="4"/>
       <c r="B334" s="11" t="s">
         <v>597</v>
@@ -16206,7 +16206,7 @@
       <c r="P334" s="14"/>
       <c r="Q334" s="10"/>
     </row>
-    <row r="335" spans="1:17" hidden="1">
+    <row r="335" spans="1:17">
       <c r="A335" s="4"/>
       <c r="B335" s="11" t="s">
         <v>606</v>
@@ -16239,7 +16239,7 @@
       <c r="P335" s="14"/>
       <c r="Q335" s="10"/>
     </row>
-    <row r="336" spans="1:17" hidden="1">
+    <row r="336" spans="1:17">
       <c r="A336" s="4"/>
       <c r="B336" s="11" t="s">
         <v>606</v>
@@ -16272,7 +16272,7 @@
       <c r="P336" s="14"/>
       <c r="Q336" s="10"/>
     </row>
-    <row r="337" spans="1:17" hidden="1">
+    <row r="337" spans="1:17">
       <c r="A337" s="4"/>
       <c r="B337" s="11" t="s">
         <v>606</v>
@@ -16305,7 +16305,7 @@
       <c r="P337" s="14"/>
       <c r="Q337" s="10"/>
     </row>
-    <row r="338" spans="1:17" hidden="1">
+    <row r="338" spans="1:17">
       <c r="A338" s="4"/>
       <c r="B338" s="11" t="s">
         <v>606</v>
@@ -16338,7 +16338,7 @@
       <c r="P338" s="14"/>
       <c r="Q338" s="10"/>
     </row>
-    <row r="339" spans="1:17" hidden="1">
+    <row r="339" spans="1:17">
       <c r="A339" s="4"/>
       <c r="B339" s="11" t="s">
         <v>606</v>
@@ -16371,7 +16371,7 @@
       <c r="P339" s="14"/>
       <c r="Q339" s="10"/>
     </row>
-    <row r="340" spans="1:17" ht="18.600000000000001" hidden="1" customHeight="1">
+    <row r="340" spans="1:17" ht="18.600000000000001" customHeight="1">
       <c r="A340" s="4"/>
       <c r="B340" s="11" t="s">
         <v>606</v>
@@ -16404,7 +16404,7 @@
       <c r="P340" s="14"/>
       <c r="Q340" s="10"/>
     </row>
-    <row r="341" spans="1:17" hidden="1">
+    <row r="341" spans="1:17">
       <c r="A341" s="4"/>
       <c r="B341" s="11" t="s">
         <v>41</v>
@@ -16443,7 +16443,7 @@
       <c r="P341" s="14"/>
       <c r="Q341" s="10"/>
     </row>
-    <row r="342" spans="1:17" hidden="1">
+    <row r="342" spans="1:17">
       <c r="A342" s="4"/>
       <c r="B342" s="11" t="s">
         <v>41</v>
@@ -16482,7 +16482,7 @@
       <c r="P342" s="14"/>
       <c r="Q342" s="10"/>
     </row>
-    <row r="343" spans="1:17" hidden="1">
+    <row r="343" spans="1:17">
       <c r="A343" s="4"/>
       <c r="B343" s="11" t="s">
         <v>41</v>
@@ -16521,7 +16521,7 @@
       <c r="P343" s="14"/>
       <c r="Q343" s="10"/>
     </row>
-    <row r="344" spans="1:17" hidden="1">
+    <row r="344" spans="1:17">
       <c r="A344" s="4"/>
       <c r="B344" s="11" t="s">
         <v>41</v>
@@ -16560,7 +16560,7 @@
       <c r="P344" s="14"/>
       <c r="Q344" s="10"/>
     </row>
-    <row r="345" spans="1:17" hidden="1">
+    <row r="345" spans="1:17">
       <c r="A345" s="4"/>
       <c r="B345" s="11" t="s">
         <v>41</v>
@@ -16599,7 +16599,7 @@
       <c r="P345" s="14"/>
       <c r="Q345" s="10"/>
     </row>
-    <row r="346" spans="1:17" hidden="1">
+    <row r="346" spans="1:17">
       <c r="A346" s="4"/>
       <c r="B346" s="11" t="s">
         <v>41</v>
@@ -16638,7 +16638,7 @@
       <c r="P346" s="14"/>
       <c r="Q346" s="10"/>
     </row>
-    <row r="347" spans="1:17" hidden="1">
+    <row r="347" spans="1:17">
       <c r="A347" s="4"/>
       <c r="B347" s="11" t="s">
         <v>41</v>
@@ -16677,7 +16677,7 @@
       <c r="P347" s="14"/>
       <c r="Q347" s="10"/>
     </row>
-    <row r="348" spans="1:17" hidden="1">
+    <row r="348" spans="1:17">
       <c r="A348" s="4"/>
       <c r="B348" s="5" t="s">
         <v>41</v>
@@ -16716,7 +16716,7 @@
       <c r="P348" s="9"/>
       <c r="Q348" s="10"/>
     </row>
-    <row r="349" spans="1:17" hidden="1">
+    <row r="349" spans="1:17">
       <c r="A349" s="4"/>
       <c r="B349" s="5" t="s">
         <v>41</v>
@@ -16755,7 +16755,7 @@
       <c r="P349" s="9"/>
       <c r="Q349" s="10"/>
     </row>
-    <row r="350" spans="1:17" hidden="1">
+    <row r="350" spans="1:17">
       <c r="A350" s="4"/>
       <c r="B350" s="11" t="s">
         <v>41</v>
@@ -16794,7 +16794,7 @@
       <c r="P350" s="9"/>
       <c r="Q350" s="10"/>
     </row>
-    <row r="351" spans="1:17" hidden="1">
+    <row r="351" spans="1:17">
       <c r="A351" s="4"/>
       <c r="B351" s="11" t="s">
         <v>41</v>
@@ -16833,7 +16833,7 @@
       <c r="P351" s="14"/>
       <c r="Q351" s="10"/>
     </row>
-    <row r="352" spans="1:17" hidden="1">
+    <row r="352" spans="1:17">
       <c r="A352" s="4"/>
       <c r="B352" s="11" t="s">
         <v>41</v>
@@ -16872,7 +16872,7 @@
       <c r="P352" s="14"/>
       <c r="Q352" s="10"/>
     </row>
-    <row r="353" spans="1:17" hidden="1">
+    <row r="353" spans="1:17">
       <c r="A353" s="4"/>
       <c r="B353" s="11" t="s">
         <v>41</v>
@@ -16911,7 +16911,7 @@
       <c r="P353" s="14"/>
       <c r="Q353" s="10"/>
     </row>
-    <row r="354" spans="1:17" hidden="1">
+    <row r="354" spans="1:17">
       <c r="A354" s="4"/>
       <c r="B354" s="11" t="s">
         <v>41</v>
@@ -16950,7 +16950,7 @@
       <c r="P354" s="14"/>
       <c r="Q354" s="10"/>
     </row>
-    <row r="355" spans="1:17" hidden="1">
+    <row r="355" spans="1:17">
       <c r="A355" s="4"/>
       <c r="B355" s="11" t="s">
         <v>41</v>
@@ -16989,7 +16989,7 @@
       <c r="P355" s="14"/>
       <c r="Q355" s="10"/>
     </row>
-    <row r="356" spans="1:17" hidden="1">
+    <row r="356" spans="1:17">
       <c r="A356" s="4"/>
       <c r="B356" s="11" t="s">
         <v>41</v>
@@ -17028,7 +17028,7 @@
       <c r="P356" s="14"/>
       <c r="Q356" s="10"/>
     </row>
-    <row r="357" spans="1:17" hidden="1">
+    <row r="357" spans="1:17">
       <c r="A357" s="4"/>
       <c r="B357" s="11" t="s">
         <v>41</v>
@@ -17067,7 +17067,7 @@
       <c r="P357" s="14"/>
       <c r="Q357" s="10"/>
     </row>
-    <row r="358" spans="1:17" hidden="1">
+    <row r="358" spans="1:17">
       <c r="A358" s="4"/>
       <c r="B358" s="11" t="s">
         <v>41</v>
@@ -17106,7 +17106,7 @@
       <c r="P358" s="14"/>
       <c r="Q358" s="10"/>
     </row>
-    <row r="359" spans="1:17" hidden="1">
+    <row r="359" spans="1:17">
       <c r="A359" s="4"/>
       <c r="B359" s="11" t="s">
         <v>41</v>
@@ -17145,7 +17145,7 @@
       <c r="P359" s="14"/>
       <c r="Q359" s="10"/>
     </row>
-    <row r="360" spans="1:17" hidden="1">
+    <row r="360" spans="1:17">
       <c r="A360" s="4"/>
       <c r="B360" s="5" t="s">
         <v>41</v>
@@ -17184,7 +17184,7 @@
       <c r="P360" s="9"/>
       <c r="Q360" s="10"/>
     </row>
-    <row r="361" spans="1:17" hidden="1">
+    <row r="361" spans="1:17">
       <c r="A361" s="4"/>
       <c r="B361" s="5" t="s">
         <v>41</v>
@@ -17223,7 +17223,7 @@
       <c r="P361" s="9"/>
       <c r="Q361" s="10"/>
     </row>
-    <row r="362" spans="1:17" hidden="1">
+    <row r="362" spans="1:17">
       <c r="A362" s="4"/>
       <c r="B362" s="11" t="s">
         <v>41</v>
@@ -17262,7 +17262,7 @@
       <c r="P362" s="14"/>
       <c r="Q362" s="10"/>
     </row>
-    <row r="363" spans="1:17" hidden="1">
+    <row r="363" spans="1:17">
       <c r="A363" s="4"/>
       <c r="B363" s="11" t="s">
         <v>41</v>
@@ -17301,7 +17301,7 @@
       <c r="P363" s="14"/>
       <c r="Q363" s="10"/>
     </row>
-    <row r="364" spans="1:17" hidden="1">
+    <row r="364" spans="1:17">
       <c r="A364" s="4"/>
       <c r="B364" s="11" t="s">
         <v>41</v>
@@ -17340,7 +17340,7 @@
       <c r="P364" s="14"/>
       <c r="Q364" s="10"/>
     </row>
-    <row r="365" spans="1:17" hidden="1">
+    <row r="365" spans="1:17">
       <c r="A365" s="4"/>
       <c r="B365" s="11" t="s">
         <v>41</v>
@@ -17377,7 +17377,7 @@
       <c r="P365" s="14"/>
       <c r="Q365" s="10"/>
     </row>
-    <row r="366" spans="1:17" hidden="1">
+    <row r="366" spans="1:17">
       <c r="A366" s="4"/>
       <c r="B366" s="11" t="s">
         <v>41</v>
@@ -17414,7 +17414,7 @@
       <c r="P366" s="14"/>
       <c r="Q366" s="10"/>
     </row>
-    <row r="367" spans="1:17" hidden="1">
+    <row r="367" spans="1:17">
       <c r="A367" s="4"/>
       <c r="B367" s="11" t="s">
         <v>41</v>
@@ -17451,7 +17451,7 @@
       <c r="P367" s="14"/>
       <c r="Q367" s="10"/>
     </row>
-    <row r="368" spans="1:17" hidden="1">
+    <row r="368" spans="1:17">
       <c r="A368" s="4"/>
       <c r="B368" s="21" t="s">
         <v>41</v>
@@ -17484,7 +17484,7 @@
       <c r="P368" s="24"/>
       <c r="Q368" s="10"/>
     </row>
-    <row r="369" spans="1:17" hidden="1">
+    <row r="369" spans="1:17">
       <c r="A369" s="4"/>
       <c r="B369" s="21" t="s">
         <v>41</v>
@@ -17517,7 +17517,7 @@
       <c r="P369" s="24"/>
       <c r="Q369" s="10"/>
     </row>
-    <row r="370" spans="1:17" s="111" customFormat="1" hidden="1">
+    <row r="370" spans="1:17" s="111" customFormat="1">
       <c r="A370" s="4"/>
       <c r="B370" s="5" t="s">
         <v>41</v>
@@ -17552,7 +17552,7 @@
       <c r="P370" s="9"/>
       <c r="Q370" s="10"/>
     </row>
-    <row r="371" spans="1:17" hidden="1">
+    <row r="371" spans="1:17">
       <c r="A371" s="4"/>
       <c r="B371" s="112" t="s">
         <v>41</v>
@@ -17587,7 +17587,7 @@
       <c r="P371" s="115"/>
       <c r="Q371" s="10"/>
     </row>
-    <row r="372" spans="1:17" hidden="1">
+    <row r="372" spans="1:17">
       <c r="A372" s="4"/>
       <c r="B372" s="112" t="s">
         <v>41</v>
@@ -17620,7 +17620,7 @@
       <c r="P372" s="9"/>
       <c r="Q372" s="10"/>
     </row>
-    <row r="373" spans="1:17" hidden="1">
+    <row r="373" spans="1:17">
       <c r="A373" s="4"/>
       <c r="B373" s="112" t="s">
         <v>41</v>
@@ -17655,7 +17655,7 @@
       <c r="P373" s="115"/>
       <c r="Q373" s="10"/>
     </row>
-    <row r="374" spans="1:17" hidden="1">
+    <row r="374" spans="1:17">
       <c r="A374" s="4"/>
       <c r="B374" s="112" t="s">
         <v>41</v>
@@ -17690,7 +17690,7 @@
       <c r="P374" s="9"/>
       <c r="Q374" s="10"/>
     </row>
-    <row r="375" spans="1:17" hidden="1">
+    <row r="375" spans="1:17">
       <c r="A375" s="4"/>
       <c r="B375" s="5" t="s">
         <v>41</v>
@@ -17729,7 +17729,7 @@
       <c r="P375" s="9"/>
       <c r="Q375" s="10"/>
     </row>
-    <row r="376" spans="1:17" hidden="1">
+    <row r="376" spans="1:17">
       <c r="A376" s="4"/>
       <c r="B376" s="5" t="s">
         <v>41</v>
@@ -17768,7 +17768,7 @@
       <c r="P376" s="9"/>
       <c r="Q376" s="10"/>
     </row>
-    <row r="377" spans="1:17" hidden="1">
+    <row r="377" spans="1:17">
       <c r="A377" s="4"/>
       <c r="B377" s="5" t="s">
         <v>41</v>
@@ -17807,7 +17807,7 @@
       <c r="P377" s="9"/>
       <c r="Q377" s="10"/>
     </row>
-    <row r="378" spans="1:17" hidden="1">
+    <row r="378" spans="1:17">
       <c r="A378" s="4"/>
       <c r="B378" s="5" t="s">
         <v>41</v>
@@ -17846,7 +17846,7 @@
       <c r="P378" s="9"/>
       <c r="Q378" s="10"/>
     </row>
-    <row r="379" spans="1:17" hidden="1">
+    <row r="379" spans="1:17">
       <c r="A379" s="4"/>
       <c r="B379" s="5" t="s">
         <v>41</v>
@@ -17885,7 +17885,7 @@
       <c r="P379" s="9"/>
       <c r="Q379" s="10"/>
     </row>
-    <row r="380" spans="1:17" hidden="1">
+    <row r="380" spans="1:17">
       <c r="A380" s="4"/>
       <c r="B380" s="5" t="s">
         <v>41</v>
@@ -17926,7 +17926,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="381" spans="1:17" hidden="1">
+    <row r="381" spans="1:17">
       <c r="A381" s="4"/>
       <c r="B381" s="5" t="s">
         <v>41</v>
@@ -17965,7 +17965,7 @@
       <c r="P381" s="9"/>
       <c r="Q381" s="10"/>
     </row>
-    <row r="382" spans="1:17" hidden="1">
+    <row r="382" spans="1:17">
       <c r="A382" s="4"/>
       <c r="B382" s="5" t="s">
         <v>41</v>
@@ -18004,7 +18004,7 @@
       <c r="P382" s="9"/>
       <c r="Q382" s="10"/>
     </row>
-    <row r="383" spans="1:17" hidden="1">
+    <row r="383" spans="1:17">
       <c r="A383" s="4"/>
       <c r="B383" s="112" t="s">
         <v>41</v>
@@ -18037,7 +18037,7 @@
       <c r="P383" s="9"/>
       <c r="Q383" s="10"/>
     </row>
-    <row r="384" spans="1:17" hidden="1">
+    <row r="384" spans="1:17">
       <c r="A384" s="117"/>
       <c r="B384" s="118"/>
       <c r="C384" s="118"/>
@@ -18056,7 +18056,7 @@
       <c r="P384" s="121"/>
       <c r="Q384" s="122"/>
     </row>
-    <row r="385" spans="1:17" hidden="1">
+    <row r="385" spans="1:17">
       <c r="A385" s="117"/>
       <c r="B385" s="118"/>
       <c r="C385" s="118"/>
@@ -18075,7 +18075,7 @@
       <c r="P385" s="121"/>
       <c r="Q385" s="122"/>
     </row>
-    <row r="386" spans="1:17" hidden="1">
+    <row r="386" spans="1:17">
       <c r="A386" s="117"/>
       <c r="B386" s="118"/>
       <c r="C386" s="118"/>
@@ -18094,7 +18094,7 @@
       <c r="P386" s="121"/>
       <c r="Q386" s="122"/>
     </row>
-    <row r="387" spans="1:17" hidden="1">
+    <row r="387" spans="1:17">
       <c r="A387" s="117"/>
       <c r="B387" s="118"/>
       <c r="C387" s="118"/>
@@ -18114,36 +18114,7 @@
       <c r="Q387" s="122"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S387" xr:uid="{F526BBEE-5653-4805-B17E-42C581B68C69}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="68_CIM_0F6CBAEDE0081BE277627DD8EBDFF240"/>
-        <filter val="68_CIM_1E2DF4543D85E40AA57080D3FDD9086D"/>
-        <filter val="68_CIM_2479202AE40BEB5443C7DCF0FC4BD5E3"/>
-        <filter val="68_CIM_2E165A02DEE5CD02A4A1F50A6F0FE556"/>
-        <filter val="68_CIM_3E34D62006DB48F8634C08A5EAFAD566"/>
-        <filter val="68_CIM_4BC5712ECBFF2D28E135A916C97B6FC1"/>
-        <filter val="68_CIM_4EB8C16894D9A775EF6526AA73275F1C"/>
-        <filter val="68_CIM_5E83620A8390E131950E009E3482B09E"/>
-        <filter val="68_CIM_60F39F02198D856414F9AB87B00D6EC6"/>
-        <filter val="68_CIM_625BDC6839DD942ED72DA6E6D9E55809"/>
-        <filter val="68_CIM_7993507C2EFE4883CBA1AE5673511ECF"/>
-        <filter val="68_CIM_909090B63C222B820D811475DFF6511F"/>
-        <filter val="68_CIM_93E4EDD9E199E8E3645A4858A0851F97"/>
-        <filter val="68_CIM_9C17BEA96EA496953BD8C10EE5F51AE0"/>
-        <filter val="68_CIM_A3BE410904204122F5CBD116B7D83569"/>
-        <filter val="68_CIM_A52A35007D3F56EE4971080B0DACBC45"/>
-        <filter val="68_CIM_B03D773BB87F8234AA80584A43D34120"/>
-        <filter val="68_CIM_C3C0D91D7BEBACB0B6F9127E3F4E48A9"/>
-        <filter val="68_CIM_F28F179764E68DC942FFD608AA87B372"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="68_CIM_C3C0D91D7BEBACB0B6F9127E3F4E48A9"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:S387" xr:uid="{F526BBEE-5653-4805-B17E-42C581B68C69}"/>
   <conditionalFormatting sqref="G2:G172 J2:J172 J249:J330 G303">
     <cfRule type="expression" dxfId="60" priority="60">
       <formula>INDIRECT("F" &amp; ROW())="Other"</formula>

</xml_diff>